<commit_message>
Finished up to 5th grade
</commit_message>
<xml_diff>
--- a/Rozklad_3zaizd.xlsx
+++ b/Rozklad_3zaizd.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9302"/>
-  <workbookPr filterPrivacy="1"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="540" windowWidth="20730" windowHeight="11220"/>
   </bookViews>
   <sheets>
     <sheet name="Лист1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -24,7 +24,7 @@
     <author>Автор</author>
   </authors>
   <commentList>
-    <comment ref="V12" authorId="0">
+    <comment ref="V12" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -55,7 +55,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="749" uniqueCount="230">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="877" uniqueCount="267">
   <si>
     <t>І</t>
   </si>
@@ -745,12 +745,123 @@
   </si>
   <si>
     <t>Історія земельних відносин  та землеустрою</t>
+  </si>
+  <si>
+    <t>Супутникова геодезія та сферична астрономія</t>
+  </si>
+  <si>
+    <t>проф. Каблак Н.І.; ас. Ваш Я.І.</t>
+  </si>
+  <si>
+    <t>Заповідна справа</t>
+  </si>
+  <si>
+    <t>Заповідна справа (залік)</t>
+  </si>
+  <si>
+    <t>Основи екології</t>
+  </si>
+  <si>
+    <t>Садово-паркове будівництво</t>
+  </si>
+  <si>
+    <t>доц. Чепур С.С,</t>
+  </si>
+  <si>
+    <t>Садово-паркове будівництво (залік)</t>
+  </si>
+  <si>
+    <t>Озеленення населених місць (де)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Основи лісоексплуатації </t>
+  </si>
+  <si>
+    <t>Основи лісоексплуатації (іспит)</t>
+  </si>
+  <si>
+    <t>Лісівництво в т.ч. рекреаційне (кп)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Лісове деревинознавство </t>
+  </si>
+  <si>
+    <t>Лісова таксація (де)</t>
+  </si>
+  <si>
+    <t>Механізація лісогосподарських та садово-паркових робіт</t>
+  </si>
+  <si>
+    <t>Державний земельний кадастр</t>
+  </si>
+  <si>
+    <t>Державний земельний кадастр (іспит)</t>
+  </si>
+  <si>
+    <t>ст. викл. Машика Н.В.</t>
+  </si>
+  <si>
+    <t>Підготовчий курс з іноземної мови (залік)</t>
+  </si>
+  <si>
+    <t>Оцінка землі і нерухомого майна</t>
+  </si>
+  <si>
+    <t>доц. Перович І.Л.</t>
+  </si>
+  <si>
+    <t>Оцінка землі і нерухомого майна (залік)</t>
+  </si>
+  <si>
+    <t>Управління земельними ресурсами</t>
+  </si>
+  <si>
+    <t>Землевпорядне  проектування</t>
+  </si>
+  <si>
+    <t>доц. Пересоляк В.Ю.</t>
+  </si>
+  <si>
+    <t>Землевпорядне  проектування (іспит)</t>
+  </si>
+  <si>
+    <t>Управління земельними ресурсами (іспит)</t>
+  </si>
+  <si>
+    <t>ст.викл. Жиган М.В.</t>
+  </si>
+  <si>
+    <t>Аерокосмічні методи та лісовпорядкування</t>
+  </si>
+  <si>
+    <t>Аерокосмічні методи та лісовпорядкування (іспит)</t>
+  </si>
+  <si>
+    <t>Ландшафтна архітектура</t>
+  </si>
+  <si>
+    <t>Ландшафтна архітектура (залік)</t>
+  </si>
+  <si>
+    <t>Основи наукових досліджень (залік)</t>
+  </si>
+  <si>
+    <t>Лісівництво в т.ч. рекреаційне (іспит)</t>
+  </si>
+  <si>
+    <t>Лісова селекція</t>
+  </si>
+  <si>
+    <t>Лісова селекція (іспит)</t>
+  </si>
+  <si>
+    <t>Лісівництво в т.ч. рекреаційне</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -1004,7 +1115,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="97">
+  <cellXfs count="98">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -1213,13 +1324,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1228,43 +1333,25 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
@@ -1276,23 +1363,50 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1566,7 +1680,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1577,10 +1691,10 @@
   <dimension ref="A1:BT92"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <pane xSplit="3" ySplit="3" topLeftCell="J4" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="3" ySplit="3" topLeftCell="D22" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="N10" sqref="N10"/>
+      <selection pane="bottomRight" activeCell="AT20" sqref="AT20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1661,373 +1775,373 @@
       <c r="A1" s="1"/>
       <c r="B1" s="1"/>
       <c r="C1" s="1"/>
-      <c r="D1" s="88" t="s">
+      <c r="D1" s="80" t="s">
         <v>14</v>
       </c>
-      <c r="E1" s="89"/>
-      <c r="F1" s="89"/>
-      <c r="G1" s="89"/>
-      <c r="H1" s="89"/>
-      <c r="I1" s="89"/>
-      <c r="J1" s="89"/>
-      <c r="K1" s="89"/>
-      <c r="L1" s="89"/>
-      <c r="M1" s="89"/>
-      <c r="N1" s="89"/>
-      <c r="O1" s="90"/>
-      <c r="P1" s="88" t="s">
+      <c r="E1" s="81"/>
+      <c r="F1" s="81"/>
+      <c r="G1" s="81"/>
+      <c r="H1" s="81"/>
+      <c r="I1" s="81"/>
+      <c r="J1" s="81"/>
+      <c r="K1" s="81"/>
+      <c r="L1" s="81"/>
+      <c r="M1" s="81"/>
+      <c r="N1" s="81"/>
+      <c r="O1" s="82"/>
+      <c r="P1" s="80" t="s">
         <v>15</v>
       </c>
-      <c r="Q1" s="89"/>
-      <c r="R1" s="89"/>
-      <c r="S1" s="89"/>
-      <c r="T1" s="89"/>
-      <c r="U1" s="89"/>
-      <c r="V1" s="89"/>
-      <c r="W1" s="89"/>
-      <c r="X1" s="90"/>
-      <c r="Y1" s="88" t="s">
+      <c r="Q1" s="81"/>
+      <c r="R1" s="81"/>
+      <c r="S1" s="81"/>
+      <c r="T1" s="81"/>
+      <c r="U1" s="81"/>
+      <c r="V1" s="81"/>
+      <c r="W1" s="81"/>
+      <c r="X1" s="82"/>
+      <c r="Y1" s="80" t="s">
         <v>16</v>
       </c>
-      <c r="Z1" s="89"/>
-      <c r="AA1" s="89"/>
-      <c r="AB1" s="89"/>
-      <c r="AC1" s="89"/>
-      <c r="AD1" s="89"/>
-      <c r="AE1" s="89"/>
-      <c r="AF1" s="89"/>
-      <c r="AG1" s="90"/>
-      <c r="AH1" s="88" t="s">
+      <c r="Z1" s="81"/>
+      <c r="AA1" s="81"/>
+      <c r="AB1" s="81"/>
+      <c r="AC1" s="81"/>
+      <c r="AD1" s="81"/>
+      <c r="AE1" s="81"/>
+      <c r="AF1" s="81"/>
+      <c r="AG1" s="82"/>
+      <c r="AH1" s="80" t="s">
         <v>17</v>
       </c>
-      <c r="AI1" s="89"/>
-      <c r="AJ1" s="89"/>
-      <c r="AK1" s="89"/>
-      <c r="AL1" s="89"/>
-      <c r="AM1" s="89"/>
-      <c r="AN1" s="89"/>
-      <c r="AO1" s="89"/>
-      <c r="AP1" s="90"/>
-      <c r="AQ1" s="88" t="s">
+      <c r="AI1" s="81"/>
+      <c r="AJ1" s="81"/>
+      <c r="AK1" s="81"/>
+      <c r="AL1" s="81"/>
+      <c r="AM1" s="81"/>
+      <c r="AN1" s="81"/>
+      <c r="AO1" s="81"/>
+      <c r="AP1" s="82"/>
+      <c r="AQ1" s="80" t="s">
         <v>18</v>
       </c>
-      <c r="AR1" s="89"/>
-      <c r="AS1" s="89"/>
-      <c r="AT1" s="89"/>
-      <c r="AU1" s="89"/>
-      <c r="AV1" s="89"/>
-      <c r="AW1" s="89"/>
-      <c r="AX1" s="89"/>
-      <c r="AY1" s="90"/>
-      <c r="AZ1" s="89" t="s">
+      <c r="AR1" s="81"/>
+      <c r="AS1" s="81"/>
+      <c r="AT1" s="81"/>
+      <c r="AU1" s="81"/>
+      <c r="AV1" s="81"/>
+      <c r="AW1" s="81"/>
+      <c r="AX1" s="81"/>
+      <c r="AY1" s="82"/>
+      <c r="AZ1" s="81" t="s">
         <v>19</v>
       </c>
-      <c r="BA1" s="89"/>
-      <c r="BB1" s="89"/>
-      <c r="BC1" s="89"/>
-      <c r="BD1" s="89"/>
-      <c r="BE1" s="89"/>
-      <c r="BF1" s="89"/>
-      <c r="BG1" s="89"/>
-      <c r="BH1" s="89"/>
-      <c r="BI1" s="89"/>
-      <c r="BJ1" s="89"/>
-      <c r="BK1" s="89"/>
-      <c r="BL1" s="89"/>
-      <c r="BM1" s="89"/>
-      <c r="BN1" s="90"/>
+      <c r="BA1" s="81"/>
+      <c r="BB1" s="81"/>
+      <c r="BC1" s="81"/>
+      <c r="BD1" s="81"/>
+      <c r="BE1" s="81"/>
+      <c r="BF1" s="81"/>
+      <c r="BG1" s="81"/>
+      <c r="BH1" s="81"/>
+      <c r="BI1" s="81"/>
+      <c r="BJ1" s="81"/>
+      <c r="BK1" s="81"/>
+      <c r="BL1" s="81"/>
+      <c r="BM1" s="81"/>
+      <c r="BN1" s="82"/>
     </row>
     <row r="2" spans="1:72" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="1"/>
       <c r="B2" s="1"/>
       <c r="C2" s="1"/>
-      <c r="D2" s="79" t="s">
+      <c r="D2" s="83" t="s">
         <v>24</v>
       </c>
-      <c r="E2" s="77"/>
-      <c r="F2" s="80"/>
-      <c r="G2" s="76" t="s">
+      <c r="E2" s="84"/>
+      <c r="F2" s="86"/>
+      <c r="G2" s="87" t="s">
         <v>25</v>
       </c>
-      <c r="H2" s="77"/>
-      <c r="I2" s="80"/>
-      <c r="J2" s="76" t="s">
+      <c r="H2" s="84"/>
+      <c r="I2" s="86"/>
+      <c r="J2" s="87" t="s">
         <v>26</v>
       </c>
-      <c r="K2" s="77"/>
-      <c r="L2" s="80"/>
-      <c r="M2" s="77" t="s">
+      <c r="K2" s="84"/>
+      <c r="L2" s="86"/>
+      <c r="M2" s="84" t="s">
         <v>27</v>
       </c>
-      <c r="N2" s="77"/>
-      <c r="O2" s="86"/>
-      <c r="P2" s="79" t="s">
+      <c r="N2" s="84"/>
+      <c r="O2" s="88"/>
+      <c r="P2" s="83" t="s">
         <v>28</v>
       </c>
-      <c r="Q2" s="77"/>
-      <c r="R2" s="80"/>
-      <c r="S2" s="76" t="s">
+      <c r="Q2" s="84"/>
+      <c r="R2" s="86"/>
+      <c r="S2" s="87" t="s">
         <v>26</v>
       </c>
-      <c r="T2" s="77"/>
-      <c r="U2" s="80"/>
-      <c r="V2" s="77" t="s">
+      <c r="T2" s="84"/>
+      <c r="U2" s="86"/>
+      <c r="V2" s="84" t="s">
         <v>29</v>
       </c>
-      <c r="W2" s="77"/>
-      <c r="X2" s="86"/>
-      <c r="Y2" s="79" t="s">
+      <c r="W2" s="84"/>
+      <c r="X2" s="88"/>
+      <c r="Y2" s="83" t="s">
         <v>28</v>
       </c>
-      <c r="Z2" s="77"/>
-      <c r="AA2" s="80"/>
-      <c r="AB2" s="76" t="s">
+      <c r="Z2" s="84"/>
+      <c r="AA2" s="86"/>
+      <c r="AB2" s="87" t="s">
         <v>26</v>
       </c>
-      <c r="AC2" s="77"/>
-      <c r="AD2" s="80"/>
-      <c r="AE2" s="77" t="s">
+      <c r="AC2" s="84"/>
+      <c r="AD2" s="86"/>
+      <c r="AE2" s="84" t="s">
         <v>29</v>
       </c>
-      <c r="AF2" s="77"/>
-      <c r="AG2" s="86"/>
-      <c r="AH2" s="79" t="s">
+      <c r="AF2" s="84"/>
+      <c r="AG2" s="88"/>
+      <c r="AH2" s="83" t="s">
         <v>28</v>
       </c>
-      <c r="AI2" s="77"/>
-      <c r="AJ2" s="80"/>
-      <c r="AK2" s="76" t="s">
+      <c r="AI2" s="84"/>
+      <c r="AJ2" s="86"/>
+      <c r="AK2" s="87" t="s">
         <v>26</v>
       </c>
-      <c r="AL2" s="77"/>
-      <c r="AM2" s="80"/>
-      <c r="AN2" s="77" t="s">
+      <c r="AL2" s="84"/>
+      <c r="AM2" s="86"/>
+      <c r="AN2" s="84" t="s">
         <v>29</v>
       </c>
-      <c r="AO2" s="77"/>
-      <c r="AP2" s="86"/>
-      <c r="AQ2" s="79" t="s">
+      <c r="AO2" s="84"/>
+      <c r="AP2" s="88"/>
+      <c r="AQ2" s="83" t="s">
         <v>28</v>
       </c>
-      <c r="AR2" s="77"/>
-      <c r="AS2" s="80"/>
-      <c r="AT2" s="76" t="s">
+      <c r="AR2" s="84"/>
+      <c r="AS2" s="86"/>
+      <c r="AT2" s="87" t="s">
         <v>26</v>
       </c>
-      <c r="AU2" s="77"/>
-      <c r="AV2" s="80"/>
-      <c r="AW2" s="77" t="s">
+      <c r="AU2" s="84"/>
+      <c r="AV2" s="86"/>
+      <c r="AW2" s="84" t="s">
         <v>29</v>
       </c>
-      <c r="AX2" s="77"/>
-      <c r="AY2" s="86"/>
-      <c r="AZ2" s="79" t="s">
+      <c r="AX2" s="84"/>
+      <c r="AY2" s="88"/>
+      <c r="AZ2" s="83" t="s">
         <v>30</v>
       </c>
-      <c r="BA2" s="77"/>
-      <c r="BB2" s="77"/>
-      <c r="BC2" s="77"/>
-      <c r="BD2" s="77"/>
-      <c r="BE2" s="80"/>
-      <c r="BF2" s="76" t="s">
+      <c r="BA2" s="84"/>
+      <c r="BB2" s="84"/>
+      <c r="BC2" s="84"/>
+      <c r="BD2" s="84"/>
+      <c r="BE2" s="86"/>
+      <c r="BF2" s="87" t="s">
         <v>26</v>
       </c>
-      <c r="BG2" s="77"/>
-      <c r="BH2" s="77"/>
-      <c r="BI2" s="77"/>
-      <c r="BJ2" s="77"/>
-      <c r="BK2" s="80"/>
-      <c r="BL2" s="77" t="s">
+      <c r="BG2" s="84"/>
+      <c r="BH2" s="84"/>
+      <c r="BI2" s="84"/>
+      <c r="BJ2" s="84"/>
+      <c r="BK2" s="86"/>
+      <c r="BL2" s="84" t="s">
         <v>35</v>
       </c>
-      <c r="BM2" s="77"/>
-      <c r="BN2" s="86"/>
+      <c r="BM2" s="84"/>
+      <c r="BN2" s="88"/>
     </row>
     <row r="3" spans="1:72" x14ac:dyDescent="0.25">
-      <c r="D3" s="79"/>
-      <c r="E3" s="77"/>
-      <c r="F3" s="80"/>
-      <c r="G3" s="76"/>
-      <c r="H3" s="77"/>
-      <c r="I3" s="80"/>
-      <c r="J3" s="76"/>
-      <c r="K3" s="77"/>
-      <c r="L3" s="80"/>
-      <c r="M3" s="77"/>
-      <c r="N3" s="77"/>
-      <c r="O3" s="86"/>
-      <c r="P3" s="79"/>
-      <c r="Q3" s="77"/>
-      <c r="R3" s="80"/>
-      <c r="S3" s="76"/>
-      <c r="T3" s="77"/>
-      <c r="U3" s="80"/>
-      <c r="V3" s="77"/>
-      <c r="W3" s="77"/>
-      <c r="X3" s="86"/>
-      <c r="Y3" s="79"/>
-      <c r="Z3" s="77"/>
-      <c r="AA3" s="80"/>
-      <c r="AB3" s="76"/>
-      <c r="AC3" s="77"/>
-      <c r="AD3" s="80"/>
-      <c r="AE3" s="77"/>
-      <c r="AF3" s="77"/>
-      <c r="AG3" s="86"/>
-      <c r="AH3" s="79"/>
-      <c r="AI3" s="77"/>
-      <c r="AJ3" s="80"/>
-      <c r="AK3" s="76"/>
-      <c r="AL3" s="77"/>
-      <c r="AM3" s="80"/>
-      <c r="AN3" s="77"/>
-      <c r="AO3" s="77"/>
-      <c r="AP3" s="86"/>
-      <c r="AQ3" s="79"/>
-      <c r="AR3" s="77"/>
-      <c r="AS3" s="80"/>
-      <c r="AT3" s="76"/>
-      <c r="AU3" s="77"/>
-      <c r="AV3" s="80"/>
-      <c r="AW3" s="77"/>
-      <c r="AX3" s="77"/>
-      <c r="AY3" s="86"/>
-      <c r="AZ3" s="79" t="s">
+      <c r="D3" s="83"/>
+      <c r="E3" s="84"/>
+      <c r="F3" s="86"/>
+      <c r="G3" s="87"/>
+      <c r="H3" s="84"/>
+      <c r="I3" s="86"/>
+      <c r="J3" s="87"/>
+      <c r="K3" s="84"/>
+      <c r="L3" s="86"/>
+      <c r="M3" s="84"/>
+      <c r="N3" s="84"/>
+      <c r="O3" s="88"/>
+      <c r="P3" s="83"/>
+      <c r="Q3" s="84"/>
+      <c r="R3" s="86"/>
+      <c r="S3" s="87"/>
+      <c r="T3" s="84"/>
+      <c r="U3" s="86"/>
+      <c r="V3" s="84"/>
+      <c r="W3" s="84"/>
+      <c r="X3" s="88"/>
+      <c r="Y3" s="83"/>
+      <c r="Z3" s="84"/>
+      <c r="AA3" s="86"/>
+      <c r="AB3" s="87"/>
+      <c r="AC3" s="84"/>
+      <c r="AD3" s="86"/>
+      <c r="AE3" s="84"/>
+      <c r="AF3" s="84"/>
+      <c r="AG3" s="88"/>
+      <c r="AH3" s="83"/>
+      <c r="AI3" s="84"/>
+      <c r="AJ3" s="86"/>
+      <c r="AK3" s="87"/>
+      <c r="AL3" s="84"/>
+      <c r="AM3" s="86"/>
+      <c r="AN3" s="84"/>
+      <c r="AO3" s="84"/>
+      <c r="AP3" s="88"/>
+      <c r="AQ3" s="83"/>
+      <c r="AR3" s="84"/>
+      <c r="AS3" s="86"/>
+      <c r="AT3" s="87"/>
+      <c r="AU3" s="84"/>
+      <c r="AV3" s="86"/>
+      <c r="AW3" s="84"/>
+      <c r="AX3" s="84"/>
+      <c r="AY3" s="88"/>
+      <c r="AZ3" s="83" t="s">
         <v>31</v>
       </c>
-      <c r="BA3" s="77"/>
-      <c r="BB3" s="78"/>
-      <c r="BC3" s="77" t="s">
+      <c r="BA3" s="84"/>
+      <c r="BB3" s="85"/>
+      <c r="BC3" s="84" t="s">
         <v>32</v>
       </c>
-      <c r="BD3" s="77"/>
-      <c r="BE3" s="80"/>
-      <c r="BF3" s="76" t="s">
+      <c r="BD3" s="84"/>
+      <c r="BE3" s="86"/>
+      <c r="BF3" s="87" t="s">
         <v>33</v>
       </c>
-      <c r="BG3" s="77"/>
-      <c r="BH3" s="78"/>
-      <c r="BI3" s="77" t="s">
+      <c r="BG3" s="84"/>
+      <c r="BH3" s="85"/>
+      <c r="BI3" s="84" t="s">
         <v>34</v>
       </c>
-      <c r="BJ3" s="77"/>
-      <c r="BK3" s="80"/>
-      <c r="BL3" s="77" t="s">
+      <c r="BJ3" s="84"/>
+      <c r="BK3" s="86"/>
+      <c r="BL3" s="84" t="s">
         <v>34</v>
       </c>
-      <c r="BM3" s="77"/>
-      <c r="BN3" s="86"/>
-      <c r="BO3" s="91"/>
-      <c r="BP3" s="91"/>
-      <c r="BQ3" s="91"/>
-      <c r="BR3" s="91"/>
-      <c r="BS3" s="91"/>
-      <c r="BT3" s="91"/>
+      <c r="BM3" s="84"/>
+      <c r="BN3" s="88"/>
+      <c r="BO3" s="90"/>
+      <c r="BP3" s="90"/>
+      <c r="BQ3" s="90"/>
+      <c r="BR3" s="90"/>
+      <c r="BS3" s="90"/>
+      <c r="BT3" s="90"/>
     </row>
     <row r="4" spans="1:72" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D4" s="79" t="s">
+      <c r="D4" s="83" t="s">
         <v>41</v>
       </c>
-      <c r="E4" s="77"/>
-      <c r="F4" s="80"/>
-      <c r="G4" s="79" t="s">
+      <c r="E4" s="84"/>
+      <c r="F4" s="86"/>
+      <c r="G4" s="83" t="s">
         <v>41</v>
       </c>
-      <c r="H4" s="77"/>
-      <c r="I4" s="80"/>
-      <c r="J4" s="79" t="s">
+      <c r="H4" s="84"/>
+      <c r="I4" s="86"/>
+      <c r="J4" s="83" t="s">
         <v>41</v>
       </c>
-      <c r="K4" s="77"/>
-      <c r="L4" s="80"/>
-      <c r="M4" s="79" t="s">
+      <c r="K4" s="84"/>
+      <c r="L4" s="86"/>
+      <c r="M4" s="83" t="s">
         <v>41</v>
       </c>
-      <c r="N4" s="77"/>
-      <c r="O4" s="80"/>
-      <c r="P4" s="79" t="s">
+      <c r="N4" s="84"/>
+      <c r="O4" s="86"/>
+      <c r="P4" s="83" t="s">
         <v>50</v>
       </c>
-      <c r="Q4" s="77"/>
-      <c r="R4" s="80"/>
-      <c r="S4" s="79" t="s">
+      <c r="Q4" s="84"/>
+      <c r="R4" s="86"/>
+      <c r="S4" s="83" t="s">
         <v>50</v>
       </c>
-      <c r="T4" s="77"/>
-      <c r="U4" s="80"/>
-      <c r="V4" s="79" t="s">
+      <c r="T4" s="84"/>
+      <c r="U4" s="86"/>
+      <c r="V4" s="83" t="s">
         <v>50</v>
       </c>
-      <c r="W4" s="77"/>
-      <c r="X4" s="80"/>
-      <c r="Y4" s="79" t="s">
+      <c r="W4" s="84"/>
+      <c r="X4" s="86"/>
+      <c r="Y4" s="83" t="s">
         <v>52</v>
       </c>
-      <c r="Z4" s="77"/>
-      <c r="AA4" s="80"/>
-      <c r="AB4" s="79" t="s">
+      <c r="Z4" s="84"/>
+      <c r="AA4" s="86"/>
+      <c r="AB4" s="83" t="s">
         <v>50</v>
       </c>
-      <c r="AC4" s="77"/>
-      <c r="AD4" s="80"/>
-      <c r="AE4" s="79" t="s">
+      <c r="AC4" s="84"/>
+      <c r="AD4" s="86"/>
+      <c r="AE4" s="83" t="s">
         <v>52</v>
       </c>
-      <c r="AF4" s="77"/>
-      <c r="AG4" s="80"/>
-      <c r="AH4" s="79" t="s">
+      <c r="AF4" s="84"/>
+      <c r="AG4" s="86"/>
+      <c r="AH4" s="83" t="s">
         <v>52</v>
       </c>
-      <c r="AI4" s="77"/>
-      <c r="AJ4" s="80"/>
-      <c r="AK4" s="79" t="s">
+      <c r="AI4" s="84"/>
+      <c r="AJ4" s="86"/>
+      <c r="AK4" s="83" t="s">
         <v>50</v>
       </c>
-      <c r="AL4" s="77"/>
-      <c r="AM4" s="80"/>
-      <c r="AN4" s="79" t="s">
+      <c r="AL4" s="84"/>
+      <c r="AM4" s="86"/>
+      <c r="AN4" s="83" t="s">
         <v>52</v>
       </c>
-      <c r="AO4" s="77"/>
-      <c r="AP4" s="80"/>
-      <c r="AQ4" s="79"/>
-      <c r="AR4" s="77"/>
-      <c r="AS4" s="80"/>
-      <c r="AT4" s="79" t="s">
+      <c r="AO4" s="84"/>
+      <c r="AP4" s="86"/>
+      <c r="AQ4" s="83"/>
+      <c r="AR4" s="84"/>
+      <c r="AS4" s="86"/>
+      <c r="AT4" s="83" t="s">
         <v>50</v>
       </c>
-      <c r="AU4" s="77"/>
-      <c r="AV4" s="80"/>
-      <c r="AW4" s="76" t="s">
+      <c r="AU4" s="84"/>
+      <c r="AV4" s="86"/>
+      <c r="AW4" s="87" t="s">
         <v>58</v>
       </c>
-      <c r="AX4" s="77"/>
-      <c r="AY4" s="86"/>
-      <c r="AZ4" s="79" t="s">
+      <c r="AX4" s="84"/>
+      <c r="AY4" s="88"/>
+      <c r="AZ4" s="83" t="s">
         <v>52</v>
       </c>
-      <c r="BA4" s="77"/>
-      <c r="BB4" s="80"/>
-      <c r="BC4" s="79" t="s">
+      <c r="BA4" s="84"/>
+      <c r="BB4" s="86"/>
+      <c r="BC4" s="83" t="s">
         <v>52</v>
       </c>
-      <c r="BD4" s="77"/>
-      <c r="BE4" s="80"/>
-      <c r="BF4" s="76" t="s">
+      <c r="BD4" s="84"/>
+      <c r="BE4" s="86"/>
+      <c r="BF4" s="87" t="s">
         <v>54</v>
       </c>
-      <c r="BG4" s="77"/>
-      <c r="BH4" s="78"/>
-      <c r="BI4" s="81" t="s">
+      <c r="BG4" s="84"/>
+      <c r="BH4" s="85"/>
+      <c r="BI4" s="95" t="s">
         <v>55</v>
       </c>
-      <c r="BJ4" s="82"/>
-      <c r="BK4" s="83"/>
-      <c r="BL4" s="84" t="s">
+      <c r="BJ4" s="96"/>
+      <c r="BK4" s="97"/>
+      <c r="BL4" s="91" t="s">
         <v>56</v>
       </c>
-      <c r="BM4" s="77"/>
-      <c r="BN4" s="86"/>
+      <c r="BM4" s="84"/>
+      <c r="BN4" s="88"/>
       <c r="BO4" s="25"/>
       <c r="BP4" s="25"/>
       <c r="BQ4" s="25"/>
@@ -2036,103 +2150,103 @@
       <c r="BT4" s="25"/>
     </row>
     <row r="5" spans="1:72" x14ac:dyDescent="0.25">
-      <c r="D5" s="85" t="s">
+      <c r="D5" s="77" t="s">
         <v>40</v>
       </c>
-      <c r="E5" s="85"/>
-      <c r="F5" s="85"/>
-      <c r="G5" s="85" t="s">
+      <c r="E5" s="77"/>
+      <c r="F5" s="77"/>
+      <c r="G5" s="77" t="s">
         <v>40</v>
       </c>
-      <c r="H5" s="85"/>
-      <c r="I5" s="85"/>
-      <c r="J5" s="85" t="s">
+      <c r="H5" s="77"/>
+      <c r="I5" s="77"/>
+      <c r="J5" s="77" t="s">
         <v>40</v>
       </c>
-      <c r="K5" s="85"/>
-      <c r="L5" s="85"/>
-      <c r="M5" s="85" t="s">
+      <c r="K5" s="77"/>
+      <c r="L5" s="77"/>
+      <c r="M5" s="77" t="s">
         <v>40</v>
       </c>
-      <c r="N5" s="85"/>
-      <c r="O5" s="85"/>
-      <c r="P5" s="79" t="s">
+      <c r="N5" s="77"/>
+      <c r="O5" s="77"/>
+      <c r="P5" s="83" t="s">
         <v>51</v>
       </c>
-      <c r="Q5" s="77"/>
-      <c r="R5" s="80"/>
-      <c r="S5" s="79" t="s">
+      <c r="Q5" s="84"/>
+      <c r="R5" s="86"/>
+      <c r="S5" s="83" t="s">
         <v>51</v>
       </c>
-      <c r="T5" s="77"/>
-      <c r="U5" s="80"/>
-      <c r="V5" s="79" t="s">
+      <c r="T5" s="84"/>
+      <c r="U5" s="86"/>
+      <c r="V5" s="83" t="s">
         <v>51</v>
       </c>
-      <c r="W5" s="77"/>
-      <c r="X5" s="80"/>
-      <c r="Y5" s="79" t="s">
+      <c r="W5" s="84"/>
+      <c r="X5" s="86"/>
+      <c r="Y5" s="83" t="s">
         <v>53</v>
       </c>
-      <c r="Z5" s="77"/>
-      <c r="AA5" s="80"/>
-      <c r="AB5" s="79" t="s">
+      <c r="Z5" s="84"/>
+      <c r="AA5" s="86"/>
+      <c r="AB5" s="83" t="s">
         <v>51</v>
       </c>
-      <c r="AC5" s="77"/>
-      <c r="AD5" s="80"/>
-      <c r="AE5" s="79" t="s">
+      <c r="AC5" s="84"/>
+      <c r="AD5" s="86"/>
+      <c r="AE5" s="83" t="s">
         <v>53</v>
       </c>
-      <c r="AF5" s="77"/>
-      <c r="AG5" s="80"/>
-      <c r="AH5" s="79" t="s">
+      <c r="AF5" s="84"/>
+      <c r="AG5" s="86"/>
+      <c r="AH5" s="83" t="s">
         <v>53</v>
       </c>
-      <c r="AI5" s="77"/>
-      <c r="AJ5" s="80"/>
-      <c r="AK5" s="79" t="s">
+      <c r="AI5" s="84"/>
+      <c r="AJ5" s="86"/>
+      <c r="AK5" s="83" t="s">
         <v>51</v>
       </c>
-      <c r="AL5" s="77"/>
-      <c r="AM5" s="80"/>
-      <c r="AN5" s="79" t="s">
+      <c r="AL5" s="84"/>
+      <c r="AM5" s="86"/>
+      <c r="AN5" s="83" t="s">
         <v>53</v>
       </c>
-      <c r="AO5" s="77"/>
-      <c r="AP5" s="80"/>
-      <c r="AQ5" s="79"/>
-      <c r="AR5" s="77"/>
-      <c r="AS5" s="80"/>
-      <c r="AT5" s="79" t="s">
+      <c r="AO5" s="84"/>
+      <c r="AP5" s="86"/>
+      <c r="AQ5" s="83"/>
+      <c r="AR5" s="84"/>
+      <c r="AS5" s="86"/>
+      <c r="AT5" s="83" t="s">
         <v>51</v>
       </c>
-      <c r="AU5" s="77"/>
-      <c r="AV5" s="80"/>
-      <c r="AW5" s="76"/>
-      <c r="AX5" s="77"/>
-      <c r="AY5" s="86"/>
-      <c r="AZ5" s="79" t="s">
+      <c r="AU5" s="84"/>
+      <c r="AV5" s="86"/>
+      <c r="AW5" s="87"/>
+      <c r="AX5" s="84"/>
+      <c r="AY5" s="88"/>
+      <c r="AZ5" s="83" t="s">
         <v>53</v>
       </c>
-      <c r="BA5" s="77"/>
-      <c r="BB5" s="80"/>
-      <c r="BC5" s="79" t="s">
+      <c r="BA5" s="84"/>
+      <c r="BB5" s="86"/>
+      <c r="BC5" s="83" t="s">
         <v>53</v>
       </c>
-      <c r="BD5" s="77"/>
-      <c r="BE5" s="80"/>
-      <c r="BF5" s="76"/>
-      <c r="BG5" s="77"/>
-      <c r="BH5" s="78"/>
-      <c r="BI5" s="84"/>
-      <c r="BJ5" s="77"/>
-      <c r="BK5" s="80"/>
-      <c r="BL5" s="76" t="s">
+      <c r="BD5" s="84"/>
+      <c r="BE5" s="86"/>
+      <c r="BF5" s="87"/>
+      <c r="BG5" s="84"/>
+      <c r="BH5" s="85"/>
+      <c r="BI5" s="91"/>
+      <c r="BJ5" s="84"/>
+      <c r="BK5" s="86"/>
+      <c r="BL5" s="87" t="s">
         <v>57</v>
       </c>
-      <c r="BM5" s="77"/>
-      <c r="BN5" s="86"/>
+      <c r="BM5" s="84"/>
+      <c r="BN5" s="88"/>
       <c r="BO5" s="25"/>
       <c r="BP5" s="25"/>
       <c r="BQ5" s="25"/>
@@ -2353,20 +2467,20 @@
       <c r="C7" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="D7" s="70" t="s">
+      <c r="D7" s="92" t="s">
         <v>90</v>
       </c>
-      <c r="E7" s="71"/>
-      <c r="F7" s="71"/>
-      <c r="G7" s="71"/>
-      <c r="H7" s="71"/>
-      <c r="I7" s="71"/>
-      <c r="J7" s="71"/>
-      <c r="K7" s="71"/>
-      <c r="L7" s="71"/>
-      <c r="M7" s="71"/>
-      <c r="N7" s="71"/>
-      <c r="O7" s="72"/>
+      <c r="E7" s="93"/>
+      <c r="F7" s="93"/>
+      <c r="G7" s="93"/>
+      <c r="H7" s="93"/>
+      <c r="I7" s="93"/>
+      <c r="J7" s="93"/>
+      <c r="K7" s="93"/>
+      <c r="L7" s="93"/>
+      <c r="M7" s="93"/>
+      <c r="N7" s="93"/>
+      <c r="O7" s="94"/>
       <c r="P7" s="44" t="s">
         <v>118</v>
       </c>
@@ -2433,11 +2547,19 @@
       <c r="AQ7" s="45"/>
       <c r="AR7" s="38"/>
       <c r="AS7" s="52"/>
-      <c r="AT7" s="51"/>
-      <c r="AU7" s="38"/>
+      <c r="AT7" s="51" t="s">
+        <v>252</v>
+      </c>
+      <c r="AU7" s="38" t="s">
+        <v>254</v>
+      </c>
       <c r="AV7" s="52"/>
-      <c r="AW7" s="37"/>
-      <c r="AX7" s="37"/>
+      <c r="AW7" s="37" t="s">
+        <v>266</v>
+      </c>
+      <c r="AX7" s="37" t="s">
+        <v>195</v>
+      </c>
       <c r="AY7" s="43"/>
       <c r="AZ7" s="35"/>
       <c r="BA7" s="36"/>
@@ -2467,20 +2589,20 @@
       <c r="C8" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D8" s="70" t="s">
+      <c r="D8" s="92" t="s">
         <v>90</v>
       </c>
-      <c r="E8" s="71"/>
-      <c r="F8" s="71"/>
-      <c r="G8" s="71"/>
-      <c r="H8" s="71"/>
-      <c r="I8" s="71"/>
-      <c r="J8" s="71"/>
-      <c r="K8" s="71"/>
-      <c r="L8" s="71"/>
-      <c r="M8" s="71"/>
-      <c r="N8" s="71"/>
-      <c r="O8" s="72"/>
+      <c r="E8" s="93"/>
+      <c r="F8" s="93"/>
+      <c r="G8" s="93"/>
+      <c r="H8" s="93"/>
+      <c r="I8" s="93"/>
+      <c r="J8" s="93"/>
+      <c r="K8" s="93"/>
+      <c r="L8" s="93"/>
+      <c r="M8" s="93"/>
+      <c r="N8" s="93"/>
+      <c r="O8" s="94"/>
       <c r="P8" s="7" t="s">
         <v>120</v>
       </c>
@@ -2547,11 +2669,19 @@
       <c r="AQ8" s="20"/>
       <c r="AR8" s="21"/>
       <c r="AS8" s="23"/>
-      <c r="AT8" s="10"/>
-      <c r="AU8" s="21"/>
+      <c r="AT8" s="10" t="s">
+        <v>253</v>
+      </c>
+      <c r="AU8" s="21" t="s">
+        <v>254</v>
+      </c>
       <c r="AV8" s="23"/>
-      <c r="AW8" s="6"/>
-      <c r="AX8" s="6"/>
+      <c r="AW8" s="6" t="s">
+        <v>258</v>
+      </c>
+      <c r="AX8" s="6" t="s">
+        <v>195</v>
+      </c>
       <c r="AY8" s="22"/>
       <c r="AZ8" s="28"/>
       <c r="BA8" s="29"/>
@@ -2581,14 +2711,14 @@
       <c r="C9" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="D9" s="94" t="s">
+      <c r="D9" s="74" t="s">
         <v>108</v>
       </c>
-      <c r="E9" s="87"/>
-      <c r="F9" s="87"/>
-      <c r="G9" s="87"/>
-      <c r="H9" s="87"/>
-      <c r="I9" s="95"/>
+      <c r="E9" s="75"/>
+      <c r="F9" s="75"/>
+      <c r="G9" s="75"/>
+      <c r="H9" s="75"/>
+      <c r="I9" s="76"/>
       <c r="J9" s="24"/>
       <c r="K9" s="21"/>
       <c r="L9" s="23"/>
@@ -2599,17 +2729,17 @@
         <v>104</v>
       </c>
       <c r="O9" s="22"/>
-      <c r="P9" s="70" t="s">
+      <c r="P9" s="92" t="s">
         <v>90</v>
       </c>
-      <c r="Q9" s="71"/>
-      <c r="R9" s="71"/>
-      <c r="S9" s="71"/>
-      <c r="T9" s="71"/>
-      <c r="U9" s="71"/>
-      <c r="V9" s="71"/>
-      <c r="W9" s="71"/>
-      <c r="X9" s="71"/>
+      <c r="Q9" s="93"/>
+      <c r="R9" s="93"/>
+      <c r="S9" s="93"/>
+      <c r="T9" s="93"/>
+      <c r="U9" s="93"/>
+      <c r="V9" s="93"/>
+      <c r="W9" s="93"/>
+      <c r="X9" s="93"/>
       <c r="Y9" s="36"/>
       <c r="Z9" s="36"/>
       <c r="AA9" s="64"/>
@@ -2641,14 +2771,22 @@
         <v>201</v>
       </c>
       <c r="AM9" s="23"/>
-      <c r="AN9" s="21"/>
-      <c r="AO9" s="21"/>
+      <c r="AN9" s="21" t="s">
+        <v>239</v>
+      </c>
+      <c r="AO9" s="21" t="s">
+        <v>195</v>
+      </c>
       <c r="AP9" s="22"/>
       <c r="AQ9" s="20"/>
       <c r="AR9" s="21"/>
       <c r="AS9" s="23"/>
-      <c r="AT9" s="10"/>
-      <c r="AU9" s="21"/>
+      <c r="AT9" s="10" t="s">
+        <v>253</v>
+      </c>
+      <c r="AU9" s="21" t="s">
+        <v>254</v>
+      </c>
       <c r="AV9" s="23"/>
       <c r="AW9" s="21"/>
       <c r="AX9" s="21"/>
@@ -2677,14 +2815,14 @@
       <c r="C10" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="D10" s="94" t="s">
+      <c r="D10" s="74" t="s">
         <v>108</v>
       </c>
-      <c r="E10" s="87"/>
-      <c r="F10" s="87"/>
-      <c r="G10" s="87"/>
-      <c r="H10" s="87"/>
-      <c r="I10" s="95"/>
+      <c r="E10" s="75"/>
+      <c r="F10" s="75"/>
+      <c r="G10" s="75"/>
+      <c r="H10" s="75"/>
+      <c r="I10" s="76"/>
       <c r="J10" s="31"/>
       <c r="K10" s="29"/>
       <c r="L10" s="30"/>
@@ -2733,14 +2871,22 @@
         <v>201</v>
       </c>
       <c r="AM10" s="23"/>
-      <c r="AN10" s="21"/>
-      <c r="AO10" s="6"/>
+      <c r="AN10" s="21" t="s">
+        <v>241</v>
+      </c>
+      <c r="AO10" s="6" t="s">
+        <v>195</v>
+      </c>
       <c r="AP10" s="22"/>
       <c r="AQ10" s="20"/>
       <c r="AR10" s="21"/>
       <c r="AS10" s="23"/>
-      <c r="AT10" s="24"/>
-      <c r="AU10" s="21"/>
+      <c r="AT10" s="24" t="s">
+        <v>248</v>
+      </c>
+      <c r="AU10" s="21" t="s">
+        <v>247</v>
+      </c>
       <c r="AV10" s="23"/>
       <c r="AW10" s="21"/>
       <c r="AX10" s="21"/>
@@ -2761,7 +2907,7 @@
       <c r="BM10" s="6"/>
       <c r="BN10" s="9"/>
     </row>
-    <row r="11" spans="1:72" ht="45" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:72" x14ac:dyDescent="0.25">
       <c r="D11" s="7"/>
       <c r="E11" s="6"/>
       <c r="F11" s="8"/>
@@ -2771,12 +2917,6 @@
       <c r="J11" s="10"/>
       <c r="K11" s="6"/>
       <c r="L11" s="8"/>
-      <c r="M11" s="6" t="s">
-        <v>103</v>
-      </c>
-      <c r="N11" s="6" t="s">
-        <v>104</v>
-      </c>
       <c r="O11" s="9"/>
       <c r="P11" s="7"/>
       <c r="Q11" s="6"/>
@@ -2838,20 +2978,20 @@
       <c r="C12" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="D12" s="73" t="s">
+      <c r="D12" s="71" t="s">
         <v>65</v>
       </c>
-      <c r="E12" s="74"/>
-      <c r="F12" s="74"/>
-      <c r="G12" s="74"/>
-      <c r="H12" s="74"/>
-      <c r="I12" s="74"/>
-      <c r="J12" s="74"/>
-      <c r="K12" s="74"/>
-      <c r="L12" s="74"/>
-      <c r="M12" s="74"/>
-      <c r="N12" s="74"/>
-      <c r="O12" s="75"/>
+      <c r="E12" s="72"/>
+      <c r="F12" s="72"/>
+      <c r="G12" s="72"/>
+      <c r="H12" s="72"/>
+      <c r="I12" s="72"/>
+      <c r="J12" s="72"/>
+      <c r="K12" s="72"/>
+      <c r="L12" s="72"/>
+      <c r="M12" s="72"/>
+      <c r="N12" s="72"/>
+      <c r="O12" s="89"/>
       <c r="P12" s="7" t="s">
         <v>120</v>
       </c>
@@ -2906,8 +3046,12 @@
         <v>84</v>
       </c>
       <c r="AM12" s="8"/>
-      <c r="AN12" s="6"/>
-      <c r="AO12" s="6"/>
+      <c r="AN12" s="6" t="s">
+        <v>234</v>
+      </c>
+      <c r="AO12" s="3" t="s">
+        <v>80</v>
+      </c>
       <c r="AP12" s="9"/>
       <c r="AQ12" s="7"/>
       <c r="AR12" s="6"/>
@@ -2942,20 +3086,20 @@
       <c r="C13" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D13" s="73" t="s">
+      <c r="D13" s="71" t="s">
         <v>65</v>
       </c>
-      <c r="E13" s="74"/>
-      <c r="F13" s="74"/>
-      <c r="G13" s="74"/>
-      <c r="H13" s="74"/>
-      <c r="I13" s="74"/>
-      <c r="J13" s="74"/>
-      <c r="K13" s="74"/>
-      <c r="L13" s="74"/>
-      <c r="M13" s="74"/>
-      <c r="N13" s="74"/>
-      <c r="O13" s="75"/>
+      <c r="E13" s="72"/>
+      <c r="F13" s="72"/>
+      <c r="G13" s="72"/>
+      <c r="H13" s="72"/>
+      <c r="I13" s="72"/>
+      <c r="J13" s="72"/>
+      <c r="K13" s="72"/>
+      <c r="L13" s="72"/>
+      <c r="M13" s="72"/>
+      <c r="N13" s="72"/>
+      <c r="O13" s="89"/>
       <c r="P13" s="7" t="s">
         <v>120</v>
       </c>
@@ -3014,14 +3158,22 @@
         <v>201</v>
       </c>
       <c r="AM13" s="8"/>
-      <c r="AN13" s="6"/>
-      <c r="AO13" s="6"/>
+      <c r="AN13" s="21" t="s">
+        <v>233</v>
+      </c>
+      <c r="AO13" s="3" t="s">
+        <v>80</v>
+      </c>
       <c r="AP13" s="9"/>
       <c r="AQ13" s="7"/>
       <c r="AR13" s="6"/>
       <c r="AS13" s="8"/>
-      <c r="AT13" s="10"/>
-      <c r="AU13" s="6"/>
+      <c r="AT13" s="10" t="s">
+        <v>245</v>
+      </c>
+      <c r="AU13" s="6" t="s">
+        <v>176</v>
+      </c>
       <c r="AV13" s="8"/>
       <c r="AW13" s="6"/>
       <c r="AX13" s="6"/>
@@ -3050,14 +3202,14 @@
       <c r="C14" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="D14" s="94" t="s">
+      <c r="D14" s="74" t="s">
         <v>108</v>
       </c>
-      <c r="E14" s="87"/>
-      <c r="F14" s="87"/>
-      <c r="G14" s="87"/>
-      <c r="H14" s="87"/>
-      <c r="I14" s="95"/>
+      <c r="E14" s="75"/>
+      <c r="F14" s="75"/>
+      <c r="G14" s="75"/>
+      <c r="H14" s="75"/>
+      <c r="I14" s="76"/>
       <c r="J14" s="10"/>
       <c r="K14" s="6"/>
       <c r="L14" s="8"/>
@@ -3126,8 +3278,12 @@
       <c r="AQ14" s="7"/>
       <c r="AR14" s="6"/>
       <c r="AS14" s="8"/>
-      <c r="AT14" s="10"/>
-      <c r="AU14" s="6"/>
+      <c r="AT14" s="10" t="s">
+        <v>246</v>
+      </c>
+      <c r="AU14" s="6" t="s">
+        <v>176</v>
+      </c>
       <c r="AV14" s="8"/>
       <c r="AW14" s="6"/>
       <c r="AX14" s="6"/>
@@ -3156,14 +3312,14 @@
       <c r="C15" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="D15" s="94" t="s">
+      <c r="D15" s="74" t="s">
         <v>108</v>
       </c>
-      <c r="E15" s="87"/>
-      <c r="F15" s="87"/>
-      <c r="G15" s="87"/>
-      <c r="H15" s="87"/>
-      <c r="I15" s="95"/>
+      <c r="E15" s="75"/>
+      <c r="F15" s="75"/>
+      <c r="G15" s="75"/>
+      <c r="H15" s="75"/>
+      <c r="I15" s="76"/>
       <c r="J15" s="10"/>
       <c r="K15" s="6"/>
       <c r="L15" s="8"/>
@@ -3245,7 +3401,7 @@
       <c r="BM15" s="6"/>
       <c r="BN15" s="9"/>
     </row>
-    <row r="16" spans="1:72" ht="90" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:72" ht="45" x14ac:dyDescent="0.25">
       <c r="C16" s="3" t="s">
         <v>37</v>
       </c>
@@ -3276,12 +3432,8 @@
       <c r="AB16" s="10"/>
       <c r="AC16" s="6"/>
       <c r="AD16" s="8"/>
-      <c r="AE16" s="6" t="s">
-        <v>184</v>
-      </c>
-      <c r="AF16" s="6" t="s">
-        <v>185</v>
-      </c>
+      <c r="AE16" s="6"/>
+      <c r="AF16" s="6"/>
       <c r="AG16" s="9"/>
       <c r="AH16" s="7"/>
       <c r="AI16" s="6"/>
@@ -3331,14 +3483,14 @@
       <c r="C17" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="D17" s="73" t="s">
+      <c r="D17" s="71" t="s">
         <v>94</v>
       </c>
-      <c r="E17" s="74"/>
-      <c r="F17" s="74"/>
-      <c r="G17" s="74"/>
-      <c r="H17" s="74"/>
-      <c r="I17" s="93"/>
+      <c r="E17" s="72"/>
+      <c r="F17" s="72"/>
+      <c r="G17" s="72"/>
+      <c r="H17" s="72"/>
+      <c r="I17" s="73"/>
       <c r="J17" s="10"/>
       <c r="K17" s="6"/>
       <c r="L17" s="8"/>
@@ -3393,8 +3545,12 @@
       <c r="AQ17" s="7"/>
       <c r="AR17" s="6"/>
       <c r="AS17" s="8"/>
-      <c r="AT17" s="10"/>
-      <c r="AU17" s="6"/>
+      <c r="AT17" s="10" t="s">
+        <v>252</v>
+      </c>
+      <c r="AU17" s="6" t="s">
+        <v>254</v>
+      </c>
       <c r="AV17" s="8"/>
       <c r="AW17" s="6"/>
       <c r="AX17" s="6"/>
@@ -3427,14 +3583,14 @@
       <c r="C18" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="D18" s="73" t="s">
+      <c r="D18" s="71" t="s">
         <v>95</v>
       </c>
-      <c r="E18" s="74"/>
-      <c r="F18" s="74"/>
-      <c r="G18" s="74"/>
-      <c r="H18" s="74"/>
-      <c r="I18" s="93"/>
+      <c r="E18" s="72"/>
+      <c r="F18" s="72"/>
+      <c r="G18" s="72"/>
+      <c r="H18" s="72"/>
+      <c r="I18" s="73"/>
       <c r="J18" s="10" t="s">
         <v>73</v>
       </c>
@@ -3451,17 +3607,17 @@
       <c r="O18" s="9" t="s">
         <v>59</v>
       </c>
-      <c r="P18" s="73" t="s">
+      <c r="P18" s="71" t="s">
         <v>72</v>
       </c>
-      <c r="Q18" s="74"/>
-      <c r="R18" s="74"/>
-      <c r="S18" s="74"/>
-      <c r="T18" s="74"/>
-      <c r="U18" s="74"/>
-      <c r="V18" s="74"/>
-      <c r="W18" s="74"/>
-      <c r="X18" s="75"/>
+      <c r="Q18" s="72"/>
+      <c r="R18" s="72"/>
+      <c r="S18" s="72"/>
+      <c r="T18" s="72"/>
+      <c r="U18" s="72"/>
+      <c r="V18" s="72"/>
+      <c r="W18" s="72"/>
+      <c r="X18" s="89"/>
       <c r="Y18" s="3" t="s">
         <v>151</v>
       </c>
@@ -3477,10 +3633,10 @@
       </c>
       <c r="AD18" s="8"/>
       <c r="AE18" s="6" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="AF18" s="6" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="AG18" s="9"/>
       <c r="AH18" s="7"/>
@@ -3495,17 +3651,29 @@
       <c r="AM18" s="8" t="s">
         <v>215</v>
       </c>
-      <c r="AN18" s="6"/>
-      <c r="AO18" s="6"/>
+      <c r="AN18" s="6" t="s">
+        <v>235</v>
+      </c>
+      <c r="AO18" s="6" t="s">
+        <v>145</v>
+      </c>
       <c r="AP18" s="9"/>
       <c r="AQ18" s="7"/>
       <c r="AR18" s="6"/>
       <c r="AS18" s="8"/>
-      <c r="AT18" s="10"/>
-      <c r="AU18" s="6"/>
+      <c r="AT18" s="10" t="s">
+        <v>255</v>
+      </c>
+      <c r="AU18" s="6" t="s">
+        <v>254</v>
+      </c>
       <c r="AV18" s="8"/>
-      <c r="AW18" s="6"/>
-      <c r="AX18" s="6"/>
+      <c r="AW18" s="6" t="s">
+        <v>189</v>
+      </c>
+      <c r="AX18" s="6" t="s">
+        <v>140</v>
+      </c>
       <c r="AY18" s="9"/>
       <c r="AZ18" s="7"/>
       <c r="BA18" s="6"/>
@@ -3548,20 +3716,24 @@
         <v>98</v>
       </c>
       <c r="L19" s="8"/>
-      <c r="M19" s="6"/>
-      <c r="N19" s="6"/>
+      <c r="M19" s="6" t="s">
+        <v>103</v>
+      </c>
+      <c r="N19" s="6" t="s">
+        <v>104</v>
+      </c>
       <c r="O19" s="9"/>
-      <c r="P19" s="73" t="s">
+      <c r="P19" s="71" t="s">
         <v>72</v>
       </c>
-      <c r="Q19" s="74"/>
-      <c r="R19" s="74"/>
-      <c r="S19" s="74"/>
-      <c r="T19" s="74"/>
-      <c r="U19" s="74"/>
-      <c r="V19" s="74"/>
-      <c r="W19" s="74"/>
-      <c r="X19" s="75"/>
+      <c r="Q19" s="72"/>
+      <c r="R19" s="72"/>
+      <c r="S19" s="72"/>
+      <c r="T19" s="72"/>
+      <c r="U19" s="72"/>
+      <c r="V19" s="72"/>
+      <c r="W19" s="72"/>
+      <c r="X19" s="89"/>
       <c r="Y19" s="3" t="s">
         <v>151</v>
       </c>
@@ -3593,8 +3765,12 @@
       <c r="AK19" s="10"/>
       <c r="AL19" s="6"/>
       <c r="AM19" s="8"/>
-      <c r="AN19" s="6"/>
-      <c r="AO19" s="6"/>
+      <c r="AN19" s="6" t="s">
+        <v>238</v>
+      </c>
+      <c r="AO19" s="6" t="s">
+        <v>145</v>
+      </c>
       <c r="AP19" s="9"/>
       <c r="AQ19" s="7"/>
       <c r="AR19" s="6"/>
@@ -3602,8 +3778,12 @@
       <c r="AT19" s="10"/>
       <c r="AU19" s="6"/>
       <c r="AV19" s="8"/>
-      <c r="AW19" s="6"/>
-      <c r="AX19" s="6"/>
+      <c r="AW19" s="6" t="s">
+        <v>266</v>
+      </c>
+      <c r="AX19" s="6" t="s">
+        <v>195</v>
+      </c>
       <c r="AY19" s="9"/>
       <c r="AZ19" s="7"/>
       <c r="BA19" s="6"/>
@@ -3662,12 +3842,6 @@
       </c>
       <c r="AA20" s="8"/>
       <c r="AD20" s="8"/>
-      <c r="AE20" s="6" t="s">
-        <v>186</v>
-      </c>
-      <c r="AF20" s="6" t="s">
-        <v>187</v>
-      </c>
       <c r="AG20" s="9"/>
       <c r="AH20" s="7"/>
       <c r="AI20" s="6"/>
@@ -3684,8 +3858,12 @@
       <c r="AT20" s="10"/>
       <c r="AU20" s="6"/>
       <c r="AV20" s="8"/>
-      <c r="AW20" s="6"/>
-      <c r="AX20" s="6"/>
+      <c r="AW20" s="3" t="s">
+        <v>258</v>
+      </c>
+      <c r="AX20" s="6" t="s">
+        <v>195</v>
+      </c>
       <c r="AY20" s="9"/>
       <c r="AZ20" s="7"/>
       <c r="BA20" s="6"/>
@@ -3743,7 +3921,9 @@
       <c r="AK21" s="10" t="s">
         <v>229</v>
       </c>
-      <c r="AL21" s="6"/>
+      <c r="AL21" s="6" t="s">
+        <v>133</v>
+      </c>
       <c r="AM21" s="8"/>
       <c r="AN21" s="6"/>
       <c r="AO21" s="6"/>
@@ -3783,20 +3963,20 @@
       <c r="C22" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="D22" s="73" t="s">
+      <c r="D22" s="71" t="s">
         <v>66</v>
       </c>
-      <c r="E22" s="74"/>
-      <c r="F22" s="74"/>
-      <c r="G22" s="74"/>
-      <c r="H22" s="74"/>
-      <c r="I22" s="74"/>
-      <c r="J22" s="74"/>
-      <c r="K22" s="74"/>
-      <c r="L22" s="74"/>
-      <c r="M22" s="74"/>
-      <c r="N22" s="74"/>
-      <c r="O22" s="75"/>
+      <c r="E22" s="72"/>
+      <c r="F22" s="72"/>
+      <c r="G22" s="72"/>
+      <c r="H22" s="72"/>
+      <c r="I22" s="72"/>
+      <c r="J22" s="72"/>
+      <c r="K22" s="72"/>
+      <c r="L22" s="72"/>
+      <c r="M22" s="72"/>
+      <c r="N22" s="72"/>
+      <c r="O22" s="89"/>
       <c r="P22" s="7" t="s">
         <v>126</v>
       </c>
@@ -3827,7 +4007,9 @@
       <c r="AK22" s="10" t="s">
         <v>228</v>
       </c>
-      <c r="AL22" s="6"/>
+      <c r="AL22" s="6" t="s">
+        <v>133</v>
+      </c>
       <c r="AM22" s="8"/>
       <c r="AN22" s="6"/>
       <c r="AO22" s="6"/>
@@ -3865,20 +4047,20 @@
       <c r="C23" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="D23" s="73" t="s">
+      <c r="D23" s="71" t="s">
         <v>70</v>
       </c>
-      <c r="E23" s="74"/>
-      <c r="F23" s="74"/>
-      <c r="G23" s="74"/>
-      <c r="H23" s="74"/>
-      <c r="I23" s="74"/>
-      <c r="J23" s="74"/>
-      <c r="K23" s="74"/>
-      <c r="L23" s="74"/>
-      <c r="M23" s="74"/>
-      <c r="N23" s="74"/>
-      <c r="O23" s="75"/>
+      <c r="E23" s="72"/>
+      <c r="F23" s="72"/>
+      <c r="G23" s="72"/>
+      <c r="H23" s="72"/>
+      <c r="I23" s="72"/>
+      <c r="J23" s="72"/>
+      <c r="K23" s="72"/>
+      <c r="L23" s="72"/>
+      <c r="M23" s="72"/>
+      <c r="N23" s="72"/>
+      <c r="O23" s="89"/>
       <c r="P23" s="7" t="s">
         <v>126</v>
       </c>
@@ -3928,17 +4110,29 @@
         <v>171</v>
       </c>
       <c r="AM23" s="8"/>
-      <c r="AN23" s="6"/>
-      <c r="AO23" s="6"/>
+      <c r="AN23" s="6" t="s">
+        <v>235</v>
+      </c>
+      <c r="AO23" s="6" t="s">
+        <v>145</v>
+      </c>
       <c r="AP23" s="9"/>
       <c r="AQ23" s="7"/>
       <c r="AR23" s="6"/>
       <c r="AS23" s="8"/>
-      <c r="AT23" s="10"/>
-      <c r="AU23" s="6"/>
+      <c r="AT23" s="10" t="s">
+        <v>256</v>
+      </c>
+      <c r="AU23" s="6" t="s">
+        <v>254</v>
+      </c>
       <c r="AV23" s="8"/>
-      <c r="AW23" s="6"/>
-      <c r="AX23" s="6"/>
+      <c r="AW23" s="6" t="s">
+        <v>263</v>
+      </c>
+      <c r="AX23" s="6" t="s">
+        <v>195</v>
+      </c>
       <c r="AY23" s="9"/>
       <c r="AZ23" s="7"/>
       <c r="BA23" s="6"/>
@@ -3964,14 +4158,14 @@
       <c r="C24" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="D24" s="85" t="s">
+      <c r="D24" s="77" t="s">
         <v>109</v>
       </c>
-      <c r="E24" s="85"/>
-      <c r="F24" s="85"/>
-      <c r="G24" s="85"/>
-      <c r="H24" s="85"/>
-      <c r="I24" s="96"/>
+      <c r="E24" s="77"/>
+      <c r="F24" s="77"/>
+      <c r="G24" s="77"/>
+      <c r="H24" s="77"/>
+      <c r="I24" s="78"/>
       <c r="J24" s="10" t="s">
         <v>73</v>
       </c>
@@ -4028,8 +4222,12 @@
         <v>171</v>
       </c>
       <c r="AM24" s="8"/>
-      <c r="AN24" s="6"/>
-      <c r="AO24" s="6"/>
+      <c r="AN24" s="6" t="s">
+        <v>238</v>
+      </c>
+      <c r="AO24" s="6" t="s">
+        <v>145</v>
+      </c>
       <c r="AP24" s="9"/>
       <c r="AQ24" s="7"/>
       <c r="AR24" s="6"/>
@@ -4037,8 +4235,12 @@
       <c r="AT24" s="10"/>
       <c r="AU24" s="6"/>
       <c r="AV24" s="8"/>
-      <c r="AW24" s="6"/>
-      <c r="AX24" s="6"/>
+      <c r="AW24" s="6" t="s">
+        <v>258</v>
+      </c>
+      <c r="AX24" s="6" t="s">
+        <v>195</v>
+      </c>
       <c r="AY24" s="9"/>
       <c r="AZ24" s="7"/>
       <c r="BA24" s="6"/>
@@ -4068,14 +4270,14 @@
       <c r="C25" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="D25" s="85" t="s">
+      <c r="D25" s="77" t="s">
         <v>109</v>
       </c>
-      <c r="E25" s="85"/>
-      <c r="F25" s="85"/>
-      <c r="G25" s="85"/>
-      <c r="H25" s="85"/>
-      <c r="I25" s="96"/>
+      <c r="E25" s="77"/>
+      <c r="F25" s="77"/>
+      <c r="G25" s="77"/>
+      <c r="H25" s="77"/>
+      <c r="I25" s="78"/>
       <c r="J25" s="10"/>
       <c r="K25" s="6"/>
       <c r="L25" s="8"/>
@@ -4127,10 +4329,13 @@
       <c r="AR25" s="6"/>
       <c r="AS25" s="8"/>
       <c r="AT25" s="10"/>
-      <c r="AU25" s="6"/>
       <c r="AV25" s="8"/>
-      <c r="AW25" s="6"/>
-      <c r="AX25" s="6"/>
+      <c r="AW25" s="6" t="s">
+        <v>259</v>
+      </c>
+      <c r="AX25" s="6" t="s">
+        <v>195</v>
+      </c>
       <c r="AY25" s="9"/>
       <c r="AZ25" s="7"/>
       <c r="BA25" s="6"/>
@@ -4395,8 +4600,12 @@
         <v>68</v>
       </c>
       <c r="AM28" s="8"/>
-      <c r="AN28" s="6"/>
-      <c r="AO28" s="6"/>
+      <c r="AN28" s="6" t="s">
+        <v>232</v>
+      </c>
+      <c r="AO28" s="3" t="s">
+        <v>80</v>
+      </c>
       <c r="AP28" s="9"/>
       <c r="AQ28" s="7"/>
       <c r="AR28" s="6"/>
@@ -4404,8 +4613,12 @@
       <c r="AT28" s="10"/>
       <c r="AU28" s="6"/>
       <c r="AV28" s="8"/>
-      <c r="AW28" s="6"/>
-      <c r="AX28" s="6"/>
+      <c r="AW28" s="6" t="s">
+        <v>189</v>
+      </c>
+      <c r="AX28" s="6" t="s">
+        <v>140</v>
+      </c>
       <c r="AY28" s="9"/>
       <c r="AZ28" s="7"/>
       <c r="BA28" s="6"/>
@@ -4423,7 +4636,7 @@
       <c r="BM28" s="6"/>
       <c r="BN28" s="9"/>
     </row>
-    <row r="29" spans="1:66" ht="45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:66" ht="45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="1"/>
       <c r="B29" s="1" t="s">
         <v>2</v>
@@ -4471,7 +4684,7 @@
         <v>98</v>
       </c>
       <c r="U29" s="8"/>
-      <c r="V29" s="6" t="s">
+      <c r="V29" s="10" t="s">
         <v>135</v>
       </c>
       <c r="W29" s="6" t="s">
@@ -4513,8 +4726,12 @@
         <v>68</v>
       </c>
       <c r="AM29" s="8"/>
-      <c r="AN29" s="6"/>
-      <c r="AO29" s="6"/>
+      <c r="AN29" s="6" t="s">
+        <v>239</v>
+      </c>
+      <c r="AO29" s="6" t="s">
+        <v>195</v>
+      </c>
       <c r="AP29" s="9"/>
       <c r="AQ29" s="7"/>
       <c r="AR29" s="6"/>
@@ -4522,8 +4739,12 @@
       <c r="AT29" s="10"/>
       <c r="AU29" s="6"/>
       <c r="AV29" s="8"/>
-      <c r="AW29" s="6"/>
-      <c r="AX29" s="6"/>
+      <c r="AW29" s="6" t="s">
+        <v>189</v>
+      </c>
+      <c r="AX29" s="6" t="s">
+        <v>140</v>
+      </c>
       <c r="AY29" s="9"/>
       <c r="AZ29" s="7"/>
       <c r="BA29" s="6"/>
@@ -4541,7 +4762,7 @@
       <c r="BM29" s="6"/>
       <c r="BN29" s="9"/>
     </row>
-    <row r="30" spans="1:66" ht="45" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:66" ht="60" x14ac:dyDescent="0.25">
       <c r="A30" s="1"/>
       <c r="B30" s="1" t="s">
         <v>3</v>
@@ -4570,11 +4791,11 @@
       <c r="R30" s="8"/>
       <c r="S30" s="10"/>
       <c r="T30" s="6"/>
-      <c r="U30" s="8"/>
-      <c r="V30" s="65" t="s">
+      <c r="U30" s="6"/>
+      <c r="V30" s="70" t="s">
         <v>139</v>
       </c>
-      <c r="W30" s="65" t="s">
+      <c r="W30" s="70" t="s">
         <v>140</v>
       </c>
       <c r="X30" s="9"/>
@@ -4595,8 +4816,12 @@
       <c r="AK30" s="10"/>
       <c r="AL30" s="6"/>
       <c r="AM30" s="8"/>
-      <c r="AN30" s="6"/>
-      <c r="AO30" s="6"/>
+      <c r="AN30" s="6" t="s">
+        <v>241</v>
+      </c>
+      <c r="AO30" s="6" t="s">
+        <v>195</v>
+      </c>
       <c r="AP30" s="9"/>
       <c r="AQ30" s="7"/>
       <c r="AR30" s="6"/>
@@ -4799,17 +5024,17 @@
         <v>78</v>
       </c>
       <c r="O33" s="9"/>
-      <c r="P33" s="73" t="s">
+      <c r="P33" s="71" t="s">
         <v>71</v>
       </c>
-      <c r="Q33" s="74"/>
-      <c r="R33" s="74"/>
-      <c r="S33" s="74"/>
-      <c r="T33" s="74"/>
-      <c r="U33" s="74"/>
-      <c r="V33" s="74"/>
-      <c r="W33" s="74"/>
-      <c r="X33" s="75"/>
+      <c r="Q33" s="72"/>
+      <c r="R33" s="72"/>
+      <c r="S33" s="72"/>
+      <c r="T33" s="72"/>
+      <c r="U33" s="72"/>
+      <c r="V33" s="72"/>
+      <c r="W33" s="72"/>
+      <c r="X33" s="89"/>
       <c r="Y33" s="20" t="s">
         <v>81</v>
       </c>
@@ -4824,6 +5049,12 @@
         <v>171</v>
       </c>
       <c r="AD33" s="8"/>
+      <c r="AE33" s="6" t="s">
+        <v>186</v>
+      </c>
+      <c r="AF33" s="6" t="s">
+        <v>187</v>
+      </c>
       <c r="AG33" s="9"/>
       <c r="AH33" s="7" t="s">
         <v>203</v>
@@ -4839,17 +5070,29 @@
         <v>68</v>
       </c>
       <c r="AM33" s="8"/>
-      <c r="AN33" s="6"/>
-      <c r="AO33" s="6"/>
+      <c r="AN33" s="3" t="s">
+        <v>242</v>
+      </c>
+      <c r="AO33" s="6" t="s">
+        <v>195</v>
+      </c>
       <c r="AP33" s="9"/>
       <c r="AQ33" s="7"/>
       <c r="AR33" s="6"/>
       <c r="AS33" s="8"/>
-      <c r="AT33" s="10"/>
-      <c r="AU33" s="6"/>
+      <c r="AT33" s="10" t="s">
+        <v>249</v>
+      </c>
+      <c r="AU33" s="6" t="s">
+        <v>250</v>
+      </c>
       <c r="AV33" s="8"/>
-      <c r="AW33" s="6"/>
-      <c r="AX33" s="6"/>
+      <c r="AW33" s="6" t="s">
+        <v>260</v>
+      </c>
+      <c r="AX33" s="6" t="s">
+        <v>145</v>
+      </c>
       <c r="AY33" s="9"/>
       <c r="AZ33" s="7"/>
       <c r="BA33" s="6"/>
@@ -4918,8 +5161,12 @@
         <v>112</v>
       </c>
       <c r="AD34" s="8"/>
-      <c r="AE34" s="6"/>
-      <c r="AF34" s="6"/>
+      <c r="AE34" s="6" t="s">
+        <v>186</v>
+      </c>
+      <c r="AF34" s="6" t="s">
+        <v>187</v>
+      </c>
       <c r="AG34" s="9"/>
       <c r="AH34" s="7" t="s">
         <v>203</v>
@@ -4935,17 +5182,29 @@
         <v>68</v>
       </c>
       <c r="AM34" s="8"/>
-      <c r="AN34" s="6"/>
-      <c r="AO34" s="6"/>
+      <c r="AN34" s="6" t="s">
+        <v>239</v>
+      </c>
+      <c r="AO34" s="6" t="s">
+        <v>195</v>
+      </c>
       <c r="AP34" s="9"/>
       <c r="AQ34" s="7"/>
       <c r="AR34" s="6"/>
       <c r="AS34" s="8"/>
-      <c r="AT34" s="10"/>
-      <c r="AU34" s="6"/>
+      <c r="AT34" s="10" t="s">
+        <v>251</v>
+      </c>
+      <c r="AU34" s="6" t="s">
+        <v>250</v>
+      </c>
       <c r="AV34" s="8"/>
-      <c r="AW34" s="6"/>
-      <c r="AX34" s="6"/>
+      <c r="AW34" s="6" t="s">
+        <v>261</v>
+      </c>
+      <c r="AX34" s="6" t="s">
+        <v>145</v>
+      </c>
       <c r="AY34" s="9"/>
       <c r="AZ34" s="7"/>
       <c r="BA34" s="6"/>
@@ -5028,8 +5287,12 @@
       <c r="AT35" s="10"/>
       <c r="AU35" s="6"/>
       <c r="AV35" s="8"/>
-      <c r="AW35" s="6"/>
-      <c r="AX35" s="6"/>
+      <c r="AW35" s="6" t="s">
+        <v>264</v>
+      </c>
+      <c r="AX35" s="6" t="s">
+        <v>195</v>
+      </c>
       <c r="AY35" s="9"/>
       <c r="AZ35" s="7"/>
       <c r="BA35" s="6"/>
@@ -5125,20 +5388,20 @@
       <c r="C37" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="D37" s="73" t="s">
+      <c r="D37" s="71" t="s">
         <v>69</v>
       </c>
-      <c r="E37" s="74"/>
-      <c r="F37" s="74"/>
-      <c r="G37" s="74"/>
-      <c r="H37" s="74"/>
-      <c r="I37" s="74"/>
-      <c r="J37" s="74"/>
-      <c r="K37" s="74"/>
-      <c r="L37" s="74"/>
-      <c r="M37" s="74"/>
-      <c r="N37" s="74"/>
-      <c r="O37" s="75"/>
+      <c r="E37" s="72"/>
+      <c r="F37" s="72"/>
+      <c r="G37" s="72"/>
+      <c r="H37" s="72"/>
+      <c r="I37" s="72"/>
+      <c r="J37" s="72"/>
+      <c r="K37" s="72"/>
+      <c r="L37" s="72"/>
+      <c r="M37" s="72"/>
+      <c r="N37" s="72"/>
+      <c r="O37" s="89"/>
       <c r="P37" s="7" t="s">
         <v>125</v>
       </c>
@@ -5211,14 +5474,14 @@
       <c r="C38" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="D38" s="85" t="s">
+      <c r="D38" s="77" t="s">
         <v>109</v>
       </c>
-      <c r="E38" s="85"/>
-      <c r="F38" s="85"/>
-      <c r="G38" s="85"/>
-      <c r="H38" s="85"/>
-      <c r="I38" s="96"/>
+      <c r="E38" s="77"/>
+      <c r="F38" s="77"/>
+      <c r="G38" s="77"/>
+      <c r="H38" s="77"/>
+      <c r="I38" s="78"/>
       <c r="J38" s="10" t="s">
         <v>111</v>
       </c>
@@ -5277,8 +5540,12 @@
         <v>171</v>
       </c>
       <c r="AM38" s="8"/>
-      <c r="AN38" s="6"/>
-      <c r="AO38" s="6"/>
+      <c r="AN38" s="3" t="s">
+        <v>242</v>
+      </c>
+      <c r="AO38" s="6" t="s">
+        <v>195</v>
+      </c>
       <c r="AP38" s="9"/>
       <c r="AQ38" s="7"/>
       <c r="AR38" s="6"/>
@@ -5286,8 +5553,12 @@
       <c r="AT38" s="10"/>
       <c r="AU38" s="6"/>
       <c r="AV38" s="8"/>
-      <c r="AW38" s="6"/>
-      <c r="AX38" s="6"/>
+      <c r="AW38" s="6" t="s">
+        <v>258</v>
+      </c>
+      <c r="AX38" s="6" t="s">
+        <v>257</v>
+      </c>
       <c r="AY38" s="9"/>
       <c r="AZ38" s="7"/>
       <c r="BA38" s="6"/>
@@ -5313,14 +5584,14 @@
       <c r="C39" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="D39" s="85" t="s">
+      <c r="D39" s="77" t="s">
         <v>110</v>
       </c>
-      <c r="E39" s="85"/>
-      <c r="F39" s="85"/>
-      <c r="G39" s="85"/>
-      <c r="H39" s="85"/>
-      <c r="I39" s="96"/>
+      <c r="E39" s="77"/>
+      <c r="F39" s="77"/>
+      <c r="G39" s="77"/>
+      <c r="H39" s="77"/>
+      <c r="I39" s="78"/>
       <c r="J39" s="10"/>
       <c r="K39" s="6"/>
       <c r="L39" s="8"/>
@@ -5369,8 +5640,12 @@
         <v>171</v>
       </c>
       <c r="AM39" s="8"/>
-      <c r="AN39" s="21"/>
-      <c r="AO39" s="21"/>
+      <c r="AN39" s="3" t="s">
+        <v>243</v>
+      </c>
+      <c r="AO39" s="6" t="s">
+        <v>195</v>
+      </c>
       <c r="AP39" s="9"/>
       <c r="AQ39" s="7"/>
       <c r="AR39" s="6"/>
@@ -5378,8 +5653,12 @@
       <c r="AT39" s="10"/>
       <c r="AU39" s="6"/>
       <c r="AV39" s="8"/>
-      <c r="AW39" s="6"/>
-      <c r="AX39" s="6"/>
+      <c r="AW39" s="6" t="s">
+        <v>258</v>
+      </c>
+      <c r="AX39" s="6" t="s">
+        <v>257</v>
+      </c>
       <c r="AY39" s="9"/>
       <c r="AZ39" s="7"/>
       <c r="BA39" s="6"/>
@@ -5449,8 +5728,6 @@
         <v>171</v>
       </c>
       <c r="AM40" s="8"/>
-      <c r="AN40" s="21"/>
-      <c r="AO40" s="21"/>
       <c r="AP40" s="9"/>
       <c r="AQ40" s="7"/>
       <c r="AR40" s="6"/>
@@ -5458,8 +5735,12 @@
       <c r="AT40" s="10"/>
       <c r="AU40" s="6"/>
       <c r="AV40" s="8"/>
-      <c r="AW40" s="6"/>
-      <c r="AX40" s="6"/>
+      <c r="AW40" s="6" t="s">
+        <v>264</v>
+      </c>
+      <c r="AX40" s="6" t="s">
+        <v>195</v>
+      </c>
       <c r="AY40" s="9"/>
       <c r="AZ40" s="7"/>
       <c r="BA40" s="6"/>
@@ -5568,17 +5849,17 @@
         <v>106</v>
       </c>
       <c r="O42" s="32"/>
-      <c r="P42" s="73" t="s">
+      <c r="P42" s="71" t="s">
         <v>91</v>
       </c>
-      <c r="Q42" s="74"/>
-      <c r="R42" s="74"/>
-      <c r="S42" s="74"/>
-      <c r="T42" s="74"/>
-      <c r="U42" s="74"/>
-      <c r="V42" s="74"/>
-      <c r="W42" s="74"/>
-      <c r="X42" s="75"/>
+      <c r="Q42" s="72"/>
+      <c r="R42" s="72"/>
+      <c r="S42" s="72"/>
+      <c r="T42" s="72"/>
+      <c r="U42" s="72"/>
+      <c r="V42" s="72"/>
+      <c r="W42" s="72"/>
+      <c r="X42" s="89"/>
       <c r="Y42" s="7" t="s">
         <v>162</v>
       </c>
@@ -5607,8 +5888,12 @@
         <v>209</v>
       </c>
       <c r="AJ42" s="8"/>
-      <c r="AK42" s="10"/>
-      <c r="AL42" s="6"/>
+      <c r="AK42" s="10" t="s">
+        <v>181</v>
+      </c>
+      <c r="AL42" s="6" t="s">
+        <v>182</v>
+      </c>
       <c r="AM42" s="8"/>
       <c r="AN42" s="6"/>
       <c r="AO42" s="6"/>
@@ -5701,8 +5986,12 @@
         <v>209</v>
       </c>
       <c r="AJ43" s="8"/>
-      <c r="AK43" s="10"/>
-      <c r="AL43" s="6"/>
+      <c r="AK43" s="10" t="s">
+        <v>181</v>
+      </c>
+      <c r="AL43" s="6" t="s">
+        <v>182</v>
+      </c>
       <c r="AM43" s="8"/>
       <c r="AN43" s="6"/>
       <c r="AO43" s="6"/>
@@ -5791,8 +6080,12 @@
         <v>217</v>
       </c>
       <c r="AJ44" s="8"/>
-      <c r="AK44" s="10"/>
-      <c r="AL44" s="6"/>
+      <c r="AK44" s="10" t="s">
+        <v>230</v>
+      </c>
+      <c r="AL44" s="6" t="s">
+        <v>231</v>
+      </c>
       <c r="AM44" s="8"/>
       <c r="AN44" s="6"/>
       <c r="AO44" s="6"/>
@@ -5883,8 +6176,12 @@
       <c r="AT45" s="10"/>
       <c r="AU45" s="6"/>
       <c r="AV45" s="8"/>
-      <c r="AW45" s="6"/>
-      <c r="AX45" s="6"/>
+      <c r="AW45" s="6" t="s">
+        <v>190</v>
+      </c>
+      <c r="AX45" s="6" t="s">
+        <v>140</v>
+      </c>
       <c r="AY45" s="9"/>
       <c r="AZ45" s="7"/>
       <c r="BA45" s="6"/>
@@ -6034,8 +6331,12 @@
         <v>147</v>
       </c>
       <c r="AJ47" s="8"/>
-      <c r="AK47" s="10"/>
-      <c r="AL47" s="6"/>
+      <c r="AK47" s="10" t="s">
+        <v>181</v>
+      </c>
+      <c r="AL47" s="6" t="s">
+        <v>182</v>
+      </c>
       <c r="AM47" s="8"/>
       <c r="AN47" s="6"/>
       <c r="AO47" s="6"/>
@@ -6130,8 +6431,12 @@
         <v>147</v>
       </c>
       <c r="AJ48" s="8"/>
-      <c r="AK48" s="10"/>
-      <c r="AL48" s="6"/>
+      <c r="AK48" s="10" t="s">
+        <v>230</v>
+      </c>
+      <c r="AL48" s="6" t="s">
+        <v>231</v>
+      </c>
       <c r="AM48" s="8"/>
       <c r="AN48" s="6"/>
       <c r="AO48" s="6"/>
@@ -6226,12 +6531,19 @@
         <v>147</v>
       </c>
       <c r="AJ49" s="8"/>
-      <c r="AK49" s="10"/>
-      <c r="AL49" s="6"/>
+      <c r="AK49" s="10" t="s">
+        <v>230</v>
+      </c>
+      <c r="AL49" s="6" t="s">
+        <v>231</v>
+      </c>
       <c r="AM49" s="8"/>
-      <c r="AN49" s="6"/>
-      <c r="AO49" s="6"/>
-      <c r="AP49" s="9"/>
+      <c r="AN49" s="6" t="s">
+        <v>244</v>
+      </c>
+      <c r="AO49" s="6" t="s">
+        <v>195</v>
+      </c>
       <c r="AQ49" s="7"/>
       <c r="AR49" s="6"/>
       <c r="AS49" s="8"/>
@@ -6313,9 +6625,12 @@
       <c r="AK50" s="53"/>
       <c r="AL50" s="16"/>
       <c r="AM50" s="17"/>
-      <c r="AN50" s="16"/>
-      <c r="AO50" s="16"/>
-      <c r="AP50" s="18"/>
+      <c r="AN50" s="6" t="s">
+        <v>240</v>
+      </c>
+      <c r="AO50" s="6" t="s">
+        <v>195</v>
+      </c>
       <c r="AQ50" s="15"/>
       <c r="AR50" s="16"/>
       <c r="AS50" s="17"/>
@@ -6458,21 +6773,25 @@
       <c r="AT52" s="6"/>
       <c r="AU52" s="6"/>
       <c r="AV52" s="6"/>
-      <c r="AW52" s="6"/>
-      <c r="AX52" s="6"/>
+      <c r="AW52" s="6" t="s">
+        <v>258</v>
+      </c>
+      <c r="AX52" s="6" t="s">
+        <v>257</v>
+      </c>
       <c r="AY52" s="6"/>
-      <c r="AZ52" s="74"/>
-      <c r="BA52" s="74"/>
-      <c r="BB52" s="74"/>
-      <c r="BC52" s="74"/>
-      <c r="BD52" s="74"/>
-      <c r="BE52" s="74"/>
-      <c r="BF52" s="74"/>
-      <c r="BG52" s="74"/>
-      <c r="BH52" s="74"/>
-      <c r="BI52" s="74"/>
-      <c r="BJ52" s="74"/>
-      <c r="BK52" s="74"/>
+      <c r="AZ52" s="72"/>
+      <c r="BA52" s="72"/>
+      <c r="BB52" s="72"/>
+      <c r="BC52" s="72"/>
+      <c r="BD52" s="72"/>
+      <c r="BE52" s="72"/>
+      <c r="BF52" s="72"/>
+      <c r="BG52" s="72"/>
+      <c r="BH52" s="72"/>
+      <c r="BI52" s="72"/>
+      <c r="BJ52" s="72"/>
+      <c r="BK52" s="72"/>
       <c r="BL52" s="6"/>
       <c r="BM52" s="6"/>
       <c r="BN52" s="6"/>
@@ -6488,12 +6807,12 @@
       <c r="D53" s="6"/>
       <c r="E53" s="6"/>
       <c r="F53" s="6"/>
-      <c r="G53" s="74"/>
-      <c r="H53" s="74"/>
-      <c r="I53" s="74"/>
-      <c r="J53" s="74"/>
-      <c r="K53" s="74"/>
-      <c r="L53" s="74"/>
+      <c r="G53" s="72"/>
+      <c r="H53" s="72"/>
+      <c r="I53" s="72"/>
+      <c r="J53" s="72"/>
+      <c r="K53" s="72"/>
+      <c r="L53" s="72"/>
       <c r="M53" s="6"/>
       <c r="N53" s="6"/>
       <c r="O53" s="6"/>
@@ -6527,20 +6846,28 @@
         <v>147</v>
       </c>
       <c r="AJ53" s="6"/>
-      <c r="AK53" s="74"/>
-      <c r="AL53" s="74"/>
-      <c r="AM53" s="74"/>
-      <c r="AN53" s="74"/>
-      <c r="AO53" s="74"/>
-      <c r="AP53" s="74"/>
+      <c r="AK53" s="6"/>
+      <c r="AL53" s="6"/>
+      <c r="AM53" s="6"/>
+      <c r="AN53" s="6" t="s">
+        <v>234</v>
+      </c>
+      <c r="AO53" s="3" t="s">
+        <v>80</v>
+      </c>
+      <c r="AP53" s="6"/>
       <c r="AQ53" s="6"/>
       <c r="AR53" s="6"/>
       <c r="AS53" s="6"/>
       <c r="AT53" s="6"/>
       <c r="AU53" s="6"/>
       <c r="AV53" s="6"/>
-      <c r="AW53" s="6"/>
-      <c r="AX53" s="6"/>
+      <c r="AW53" s="6" t="s">
+        <v>259</v>
+      </c>
+      <c r="AX53" s="6" t="s">
+        <v>257</v>
+      </c>
       <c r="AY53" s="6"/>
       <c r="AZ53" s="6"/>
       <c r="BA53" s="6"/>
@@ -6548,12 +6875,12 @@
       <c r="BC53" s="6"/>
       <c r="BD53" s="6"/>
       <c r="BE53" s="6"/>
-      <c r="BF53" s="74"/>
-      <c r="BG53" s="74"/>
-      <c r="BH53" s="74"/>
-      <c r="BI53" s="74"/>
-      <c r="BJ53" s="74"/>
-      <c r="BK53" s="74"/>
+      <c r="BF53" s="72"/>
+      <c r="BG53" s="72"/>
+      <c r="BH53" s="72"/>
+      <c r="BI53" s="72"/>
+      <c r="BJ53" s="72"/>
+      <c r="BK53" s="72"/>
       <c r="BL53" s="6"/>
       <c r="BM53" s="6"/>
       <c r="BN53" s="6"/>
@@ -6569,12 +6896,12 @@
       <c r="D54" s="6"/>
       <c r="E54" s="6"/>
       <c r="F54" s="6"/>
-      <c r="G54" s="74"/>
-      <c r="H54" s="74"/>
-      <c r="I54" s="74"/>
-      <c r="J54" s="74"/>
-      <c r="K54" s="74"/>
-      <c r="L54" s="74"/>
+      <c r="G54" s="72"/>
+      <c r="H54" s="72"/>
+      <c r="I54" s="72"/>
+      <c r="J54" s="72"/>
+      <c r="K54" s="72"/>
+      <c r="L54" s="72"/>
       <c r="M54" s="6"/>
       <c r="N54" s="6"/>
       <c r="O54" s="6"/>
@@ -6614,8 +6941,12 @@
       <c r="AK54" s="6"/>
       <c r="AL54" s="6"/>
       <c r="AM54" s="6"/>
-      <c r="AN54" s="6"/>
-      <c r="AO54" s="6"/>
+      <c r="AN54" s="6" t="s">
+        <v>237</v>
+      </c>
+      <c r="AO54" s="6" t="s">
+        <v>236</v>
+      </c>
       <c r="AP54" s="6"/>
       <c r="AQ54" s="6"/>
       <c r="AR54" s="6"/>
@@ -6632,12 +6963,12 @@
       <c r="BC54" s="6"/>
       <c r="BD54" s="6"/>
       <c r="BE54" s="6"/>
-      <c r="BF54" s="74"/>
-      <c r="BG54" s="74"/>
-      <c r="BH54" s="74"/>
-      <c r="BI54" s="74"/>
-      <c r="BJ54" s="74"/>
-      <c r="BK54" s="74"/>
+      <c r="BF54" s="72"/>
+      <c r="BG54" s="72"/>
+      <c r="BH54" s="72"/>
+      <c r="BI54" s="72"/>
+      <c r="BJ54" s="72"/>
+      <c r="BK54" s="72"/>
       <c r="BL54" s="6"/>
       <c r="BM54" s="6"/>
       <c r="BN54" s="6"/>
@@ -6704,12 +7035,12 @@
       <c r="BC55" s="6"/>
       <c r="BD55" s="6"/>
       <c r="BE55" s="6"/>
-      <c r="BF55" s="74"/>
-      <c r="BG55" s="74"/>
-      <c r="BH55" s="74"/>
-      <c r="BI55" s="74"/>
-      <c r="BJ55" s="74"/>
-      <c r="BK55" s="74"/>
+      <c r="BF55" s="72"/>
+      <c r="BG55" s="72"/>
+      <c r="BH55" s="72"/>
+      <c r="BI55" s="72"/>
+      <c r="BJ55" s="72"/>
+      <c r="BK55" s="72"/>
       <c r="BL55" s="6"/>
       <c r="BM55" s="6"/>
       <c r="BN55" s="6"/>
@@ -6721,12 +7052,12 @@
       <c r="D56" s="6"/>
       <c r="E56" s="6"/>
       <c r="F56" s="6"/>
-      <c r="G56" s="74"/>
-      <c r="H56" s="74"/>
-      <c r="I56" s="74"/>
-      <c r="J56" s="74"/>
-      <c r="K56" s="74"/>
-      <c r="L56" s="74"/>
+      <c r="G56" s="72"/>
+      <c r="H56" s="72"/>
+      <c r="I56" s="72"/>
+      <c r="J56" s="72"/>
+      <c r="K56" s="72"/>
+      <c r="L56" s="72"/>
       <c r="M56" s="6"/>
       <c r="N56" s="6"/>
       <c r="O56" s="6"/>
@@ -6795,12 +7126,12 @@
       <c r="D57" s="6"/>
       <c r="E57" s="6"/>
       <c r="F57" s="6"/>
-      <c r="G57" s="74"/>
-      <c r="H57" s="74"/>
-      <c r="I57" s="74"/>
-      <c r="J57" s="74"/>
-      <c r="K57" s="74"/>
-      <c r="L57" s="74"/>
+      <c r="G57" s="72"/>
+      <c r="H57" s="72"/>
+      <c r="I57" s="72"/>
+      <c r="J57" s="72"/>
+      <c r="K57" s="72"/>
+      <c r="L57" s="72"/>
       <c r="M57" s="6"/>
       <c r="N57" s="6"/>
       <c r="O57" s="6"/>
@@ -6864,12 +7195,12 @@
       <c r="C58" s="68" t="s">
         <v>21</v>
       </c>
-      <c r="D58" s="92"/>
-      <c r="E58" s="92"/>
-      <c r="F58" s="92"/>
-      <c r="G58" s="92"/>
-      <c r="H58" s="92"/>
-      <c r="I58" s="92"/>
+      <c r="D58" s="79"/>
+      <c r="E58" s="79"/>
+      <c r="F58" s="79"/>
+      <c r="G58" s="79"/>
+      <c r="H58" s="79"/>
+      <c r="I58" s="79"/>
       <c r="J58" s="6"/>
       <c r="K58" s="6"/>
       <c r="L58" s="6"/>
@@ -6909,7 +7240,6 @@
       <c r="AL58" s="6"/>
       <c r="AM58" s="6"/>
       <c r="AN58" s="6"/>
-      <c r="AO58" s="6"/>
       <c r="AP58" s="6"/>
       <c r="AQ58" s="6"/>
       <c r="AR58" s="6"/>
@@ -6917,15 +7247,19 @@
       <c r="AT58" s="6"/>
       <c r="AU58" s="6"/>
       <c r="AV58" s="6"/>
-      <c r="AW58" s="6"/>
-      <c r="AX58" s="6"/>
+      <c r="AW58" s="6" t="s">
+        <v>262</v>
+      </c>
+      <c r="AX58" s="6" t="s">
+        <v>80</v>
+      </c>
       <c r="AY58" s="6"/>
-      <c r="AZ58" s="74"/>
-      <c r="BA58" s="74"/>
-      <c r="BB58" s="74"/>
-      <c r="BC58" s="74"/>
-      <c r="BD58" s="74"/>
-      <c r="BE58" s="74"/>
+      <c r="AZ58" s="72"/>
+      <c r="BA58" s="72"/>
+      <c r="BB58" s="72"/>
+      <c r="BC58" s="72"/>
+      <c r="BD58" s="72"/>
+      <c r="BE58" s="72"/>
       <c r="BF58" s="6"/>
       <c r="BG58" s="6"/>
       <c r="BH58" s="6"/>
@@ -6944,12 +7278,12 @@
       <c r="C59" s="68" t="s">
         <v>22</v>
       </c>
-      <c r="D59" s="92"/>
-      <c r="E59" s="92"/>
-      <c r="F59" s="92"/>
-      <c r="G59" s="92"/>
-      <c r="H59" s="92"/>
-      <c r="I59" s="92"/>
+      <c r="D59" s="79"/>
+      <c r="E59" s="79"/>
+      <c r="F59" s="79"/>
+      <c r="G59" s="79"/>
+      <c r="H59" s="79"/>
+      <c r="I59" s="79"/>
       <c r="J59" s="6"/>
       <c r="K59" s="6"/>
       <c r="L59" s="6"/>
@@ -6988,8 +7322,12 @@
       <c r="AK59" s="6"/>
       <c r="AL59" s="6"/>
       <c r="AM59" s="6"/>
-      <c r="AN59" s="6"/>
-      <c r="AO59" s="6"/>
+      <c r="AN59" s="6" t="s">
+        <v>243</v>
+      </c>
+      <c r="AO59" s="6" t="s">
+        <v>195</v>
+      </c>
       <c r="AP59" s="6"/>
       <c r="AQ59" s="6"/>
       <c r="AR59" s="6"/>
@@ -7000,18 +7338,18 @@
       <c r="AW59" s="6"/>
       <c r="AX59" s="6"/>
       <c r="AY59" s="6"/>
-      <c r="AZ59" s="74"/>
-      <c r="BA59" s="74"/>
-      <c r="BB59" s="74"/>
-      <c r="BC59" s="74"/>
-      <c r="BD59" s="74"/>
-      <c r="BE59" s="74"/>
-      <c r="BF59" s="74"/>
-      <c r="BG59" s="74"/>
-      <c r="BH59" s="74"/>
-      <c r="BI59" s="74"/>
-      <c r="BJ59" s="74"/>
-      <c r="BK59" s="74"/>
+      <c r="AZ59" s="72"/>
+      <c r="BA59" s="72"/>
+      <c r="BB59" s="72"/>
+      <c r="BC59" s="72"/>
+      <c r="BD59" s="72"/>
+      <c r="BE59" s="72"/>
+      <c r="BF59" s="72"/>
+      <c r="BG59" s="72"/>
+      <c r="BH59" s="72"/>
+      <c r="BI59" s="72"/>
+      <c r="BJ59" s="72"/>
+      <c r="BK59" s="72"/>
       <c r="BL59" s="6"/>
       <c r="BM59" s="6"/>
       <c r="BN59" s="6"/>
@@ -7064,8 +7402,12 @@
       <c r="AK60" s="6"/>
       <c r="AL60" s="6"/>
       <c r="AM60" s="6"/>
-      <c r="AN60" s="6"/>
-      <c r="AO60" s="6"/>
+      <c r="AN60" s="6" t="s">
+        <v>244</v>
+      </c>
+      <c r="AO60" s="6" t="s">
+        <v>195</v>
+      </c>
       <c r="AP60" s="6"/>
       <c r="AQ60" s="6"/>
       <c r="AR60" s="6"/>
@@ -7082,12 +7424,12 @@
       <c r="BC60" s="6"/>
       <c r="BD60" s="6"/>
       <c r="BE60" s="6"/>
-      <c r="BF60" s="74"/>
-      <c r="BG60" s="74"/>
-      <c r="BH60" s="74"/>
-      <c r="BI60" s="74"/>
-      <c r="BJ60" s="74"/>
-      <c r="BK60" s="74"/>
+      <c r="BF60" s="72"/>
+      <c r="BG60" s="72"/>
+      <c r="BH60" s="72"/>
+      <c r="BI60" s="72"/>
+      <c r="BJ60" s="72"/>
+      <c r="BK60" s="72"/>
       <c r="BL60" s="6"/>
       <c r="BM60" s="6"/>
       <c r="BN60" s="6"/>
@@ -7173,12 +7515,12 @@
       <c r="D62" s="6"/>
       <c r="E62" s="6"/>
       <c r="F62" s="6"/>
-      <c r="G62" s="74"/>
-      <c r="H62" s="74"/>
-      <c r="I62" s="74"/>
-      <c r="J62" s="74"/>
-      <c r="K62" s="74"/>
-      <c r="L62" s="74"/>
+      <c r="G62" s="72"/>
+      <c r="H62" s="72"/>
+      <c r="I62" s="72"/>
+      <c r="J62" s="72"/>
+      <c r="K62" s="72"/>
+      <c r="L62" s="72"/>
       <c r="M62" s="6"/>
       <c r="N62" s="6"/>
       <c r="O62" s="6"/>
@@ -7224,12 +7566,12 @@
       <c r="BC62" s="6"/>
       <c r="BD62" s="6"/>
       <c r="BE62" s="6"/>
-      <c r="BF62" s="74"/>
-      <c r="BG62" s="74"/>
-      <c r="BH62" s="74"/>
-      <c r="BI62" s="74"/>
-      <c r="BJ62" s="74"/>
-      <c r="BK62" s="74"/>
+      <c r="BF62" s="72"/>
+      <c r="BG62" s="72"/>
+      <c r="BH62" s="72"/>
+      <c r="BI62" s="72"/>
+      <c r="BJ62" s="72"/>
+      <c r="BK62" s="72"/>
       <c r="BL62" s="6"/>
       <c r="BM62" s="6"/>
       <c r="BN62" s="6"/>
@@ -7245,12 +7587,12 @@
       <c r="D63" s="6"/>
       <c r="E63" s="6"/>
       <c r="F63" s="6"/>
-      <c r="G63" s="74"/>
-      <c r="H63" s="74"/>
-      <c r="I63" s="74"/>
-      <c r="J63" s="74"/>
-      <c r="K63" s="74"/>
-      <c r="L63" s="74"/>
+      <c r="G63" s="72"/>
+      <c r="H63" s="72"/>
+      <c r="I63" s="72"/>
+      <c r="J63" s="72"/>
+      <c r="K63" s="72"/>
+      <c r="L63" s="72"/>
       <c r="M63" s="6"/>
       <c r="N63" s="6"/>
       <c r="O63" s="6"/>
@@ -7286,8 +7628,12 @@
       <c r="AK63" s="6"/>
       <c r="AL63" s="6"/>
       <c r="AM63" s="6"/>
-      <c r="AN63" s="6"/>
-      <c r="AO63" s="6"/>
+      <c r="AN63" s="6" t="s">
+        <v>243</v>
+      </c>
+      <c r="AO63" s="6" t="s">
+        <v>195</v>
+      </c>
       <c r="AP63" s="6"/>
       <c r="AQ63" s="6"/>
       <c r="AR63" s="6"/>
@@ -7304,12 +7650,12 @@
       <c r="BC63" s="6"/>
       <c r="BD63" s="6"/>
       <c r="BE63" s="6"/>
-      <c r="BF63" s="74"/>
-      <c r="BG63" s="74"/>
-      <c r="BH63" s="74"/>
-      <c r="BI63" s="74"/>
-      <c r="BJ63" s="74"/>
-      <c r="BK63" s="74"/>
+      <c r="BF63" s="72"/>
+      <c r="BG63" s="72"/>
+      <c r="BH63" s="72"/>
+      <c r="BI63" s="72"/>
+      <c r="BJ63" s="72"/>
+      <c r="BK63" s="72"/>
       <c r="BL63" s="6"/>
       <c r="BM63" s="6"/>
       <c r="BN63" s="6"/>
@@ -7322,12 +7668,12 @@
       <c r="C64" s="68" t="s">
         <v>22</v>
       </c>
-      <c r="D64" s="74"/>
-      <c r="E64" s="74"/>
-      <c r="F64" s="74"/>
-      <c r="G64" s="74"/>
-      <c r="H64" s="74"/>
-      <c r="I64" s="74"/>
+      <c r="D64" s="72"/>
+      <c r="E64" s="72"/>
+      <c r="F64" s="72"/>
+      <c r="G64" s="72"/>
+      <c r="H64" s="72"/>
+      <c r="I64" s="72"/>
       <c r="J64" s="6"/>
       <c r="K64" s="6"/>
       <c r="L64" s="6"/>
@@ -7362,8 +7708,12 @@
       <c r="AK64" s="6"/>
       <c r="AL64" s="6"/>
       <c r="AM64" s="6"/>
-      <c r="AN64" s="6"/>
-      <c r="AO64" s="6"/>
+      <c r="AN64" s="3" t="s">
+        <v>243</v>
+      </c>
+      <c r="AO64" s="6" t="s">
+        <v>195</v>
+      </c>
       <c r="AP64" s="6"/>
       <c r="AQ64" s="6"/>
       <c r="AR64" s="6"/>
@@ -7380,12 +7730,12 @@
       <c r="BC64" s="6"/>
       <c r="BD64" s="6"/>
       <c r="BE64" s="6"/>
-      <c r="BF64" s="74"/>
-      <c r="BG64" s="74"/>
-      <c r="BH64" s="74"/>
-      <c r="BI64" s="74"/>
-      <c r="BJ64" s="74"/>
-      <c r="BK64" s="74"/>
+      <c r="BF64" s="72"/>
+      <c r="BG64" s="72"/>
+      <c r="BH64" s="72"/>
+      <c r="BI64" s="72"/>
+      <c r="BJ64" s="72"/>
+      <c r="BK64" s="72"/>
       <c r="BL64" s="6"/>
       <c r="BM64" s="6"/>
       <c r="BN64" s="6"/>
@@ -7443,8 +7793,12 @@
       <c r="AT65" s="6"/>
       <c r="AU65" s="6"/>
       <c r="AV65" s="6"/>
-      <c r="AW65" s="6"/>
-      <c r="AX65" s="6"/>
+      <c r="AW65" s="6" t="s">
+        <v>263</v>
+      </c>
+      <c r="AX65" s="6" t="s">
+        <v>195</v>
+      </c>
       <c r="AY65" s="6"/>
       <c r="AZ65" s="6"/>
       <c r="BA65" s="6"/>
@@ -7452,12 +7806,12 @@
       <c r="BC65" s="6"/>
       <c r="BD65" s="6"/>
       <c r="BE65" s="6"/>
-      <c r="BF65" s="74"/>
-      <c r="BG65" s="74"/>
-      <c r="BH65" s="74"/>
-      <c r="BI65" s="74"/>
-      <c r="BJ65" s="74"/>
-      <c r="BK65" s="74"/>
+      <c r="BF65" s="72"/>
+      <c r="BG65" s="72"/>
+      <c r="BH65" s="72"/>
+      <c r="BI65" s="72"/>
+      <c r="BJ65" s="72"/>
+      <c r="BK65" s="72"/>
       <c r="BL65" s="6"/>
       <c r="BM65" s="6"/>
       <c r="BN65" s="6"/>
@@ -7544,12 +7898,12 @@
       <c r="C67" s="68" t="s">
         <v>21</v>
       </c>
-      <c r="D67" s="74"/>
-      <c r="E67" s="74"/>
-      <c r="F67" s="74"/>
-      <c r="G67" s="74"/>
-      <c r="H67" s="74"/>
-      <c r="I67" s="74"/>
+      <c r="D67" s="72"/>
+      <c r="E67" s="72"/>
+      <c r="F67" s="72"/>
+      <c r="G67" s="72"/>
+      <c r="H67" s="72"/>
+      <c r="I67" s="72"/>
       <c r="J67" s="6"/>
       <c r="K67" s="6"/>
       <c r="L67" s="6"/>
@@ -7589,15 +7943,19 @@
       <c r="AT67" s="6"/>
       <c r="AU67" s="6"/>
       <c r="AV67" s="6"/>
-      <c r="AW67" s="6"/>
-      <c r="AX67" s="6"/>
+      <c r="AW67" s="6" t="s">
+        <v>264</v>
+      </c>
+      <c r="AX67" s="6" t="s">
+        <v>195</v>
+      </c>
       <c r="AY67" s="6"/>
-      <c r="AZ67" s="74"/>
-      <c r="BA67" s="74"/>
-      <c r="BB67" s="74"/>
-      <c r="BC67" s="74"/>
-      <c r="BD67" s="74"/>
-      <c r="BE67" s="74"/>
+      <c r="AZ67" s="72"/>
+      <c r="BA67" s="72"/>
+      <c r="BB67" s="72"/>
+      <c r="BC67" s="72"/>
+      <c r="BD67" s="72"/>
+      <c r="BE67" s="72"/>
       <c r="BF67" s="6"/>
       <c r="BG67" s="6"/>
       <c r="BH67" s="6"/>
@@ -7619,12 +7977,12 @@
       <c r="D68" s="6"/>
       <c r="E68" s="6"/>
       <c r="F68" s="6"/>
-      <c r="G68" s="74"/>
-      <c r="H68" s="74"/>
-      <c r="I68" s="74"/>
-      <c r="J68" s="74"/>
-      <c r="K68" s="74"/>
-      <c r="L68" s="74"/>
+      <c r="G68" s="72"/>
+      <c r="H68" s="72"/>
+      <c r="I68" s="72"/>
+      <c r="J68" s="72"/>
+      <c r="K68" s="72"/>
+      <c r="L68" s="72"/>
       <c r="M68" s="6"/>
       <c r="N68" s="6"/>
       <c r="O68" s="6"/>
@@ -7661,8 +8019,12 @@
       <c r="AT68" s="6"/>
       <c r="AU68" s="6"/>
       <c r="AV68" s="6"/>
-      <c r="AW68" s="6"/>
-      <c r="AX68" s="6"/>
+      <c r="AW68" s="6" t="s">
+        <v>265</v>
+      </c>
+      <c r="AX68" s="6" t="s">
+        <v>195</v>
+      </c>
       <c r="AY68" s="6"/>
       <c r="AZ68" s="6"/>
       <c r="BA68" s="6"/>
@@ -7691,12 +8053,12 @@
       <c r="D69" s="6"/>
       <c r="E69" s="6"/>
       <c r="F69" s="6"/>
-      <c r="G69" s="74"/>
-      <c r="H69" s="74"/>
-      <c r="I69" s="74"/>
-      <c r="J69" s="74"/>
-      <c r="K69" s="74"/>
-      <c r="L69" s="74"/>
+      <c r="G69" s="72"/>
+      <c r="H69" s="72"/>
+      <c r="I69" s="72"/>
+      <c r="J69" s="72"/>
+      <c r="K69" s="72"/>
+      <c r="L69" s="72"/>
       <c r="M69" s="6"/>
       <c r="N69" s="6"/>
       <c r="O69" s="6"/>
@@ -7742,12 +8104,12 @@
       <c r="BC69" s="6"/>
       <c r="BD69" s="6"/>
       <c r="BE69" s="6"/>
-      <c r="BF69" s="87"/>
-      <c r="BG69" s="87"/>
-      <c r="BH69" s="87"/>
-      <c r="BI69" s="87"/>
-      <c r="BJ69" s="87"/>
-      <c r="BK69" s="87"/>
+      <c r="BF69" s="75"/>
+      <c r="BG69" s="75"/>
+      <c r="BH69" s="75"/>
+      <c r="BI69" s="75"/>
+      <c r="BJ69" s="75"/>
+      <c r="BK69" s="75"/>
       <c r="BL69" s="6"/>
       <c r="BM69" s="6"/>
       <c r="BN69" s="6"/>
@@ -7878,12 +8240,12 @@
       <c r="AW71" s="6"/>
       <c r="AX71" s="6"/>
       <c r="AY71" s="6"/>
-      <c r="AZ71" s="87"/>
-      <c r="BA71" s="87"/>
-      <c r="BB71" s="87"/>
-      <c r="BC71" s="87"/>
-      <c r="BD71" s="87"/>
-      <c r="BE71" s="87"/>
+      <c r="AZ71" s="75"/>
+      <c r="BA71" s="75"/>
+      <c r="BB71" s="75"/>
+      <c r="BC71" s="75"/>
+      <c r="BD71" s="75"/>
+      <c r="BE71" s="75"/>
       <c r="BF71" s="6"/>
       <c r="BG71" s="6"/>
       <c r="BH71" s="6"/>
@@ -7902,12 +8264,12 @@
       <c r="C72" s="68" t="s">
         <v>21</v>
       </c>
-      <c r="D72" s="74"/>
-      <c r="E72" s="74"/>
-      <c r="F72" s="74"/>
-      <c r="G72" s="74"/>
-      <c r="H72" s="74"/>
-      <c r="I72" s="74"/>
+      <c r="D72" s="72"/>
+      <c r="E72" s="72"/>
+      <c r="F72" s="72"/>
+      <c r="G72" s="72"/>
+      <c r="H72" s="72"/>
+      <c r="I72" s="72"/>
       <c r="J72" s="6"/>
       <c r="K72" s="6"/>
       <c r="L72" s="6"/>
@@ -7974,12 +8336,12 @@
       <c r="C73" s="68" t="s">
         <v>22</v>
       </c>
-      <c r="D73" s="74"/>
-      <c r="E73" s="74"/>
-      <c r="F73" s="74"/>
-      <c r="G73" s="74"/>
-      <c r="H73" s="74"/>
-      <c r="I73" s="74"/>
+      <c r="D73" s="72"/>
+      <c r="E73" s="72"/>
+      <c r="F73" s="72"/>
+      <c r="G73" s="72"/>
+      <c r="H73" s="72"/>
+      <c r="I73" s="72"/>
       <c r="J73" s="6"/>
       <c r="K73" s="6"/>
       <c r="L73" s="6"/>
@@ -8028,12 +8390,12 @@
       <c r="BC73" s="6"/>
       <c r="BD73" s="6"/>
       <c r="BE73" s="6"/>
-      <c r="BF73" s="74"/>
-      <c r="BG73" s="74"/>
-      <c r="BH73" s="74"/>
-      <c r="BI73" s="74"/>
-      <c r="BJ73" s="74"/>
-      <c r="BK73" s="74"/>
+      <c r="BF73" s="72"/>
+      <c r="BG73" s="72"/>
+      <c r="BH73" s="72"/>
+      <c r="BI73" s="72"/>
+      <c r="BJ73" s="72"/>
+      <c r="BK73" s="72"/>
       <c r="BL73" s="6"/>
       <c r="BM73" s="6"/>
       <c r="BN73" s="6"/>
@@ -8046,12 +8408,12 @@
       <c r="C74" s="68" t="s">
         <v>23</v>
       </c>
-      <c r="D74" s="92"/>
-      <c r="E74" s="92"/>
-      <c r="F74" s="92"/>
-      <c r="G74" s="92"/>
-      <c r="H74" s="92"/>
-      <c r="I74" s="92"/>
+      <c r="D74" s="79"/>
+      <c r="E74" s="79"/>
+      <c r="F74" s="79"/>
+      <c r="G74" s="79"/>
+      <c r="H74" s="79"/>
+      <c r="I74" s="79"/>
       <c r="J74" s="6"/>
       <c r="K74" s="6"/>
       <c r="L74" s="6"/>
@@ -8100,23 +8462,23 @@
       <c r="BC74" s="6"/>
       <c r="BD74" s="6"/>
       <c r="BE74" s="6"/>
-      <c r="BF74" s="74"/>
-      <c r="BG74" s="74"/>
-      <c r="BH74" s="74"/>
-      <c r="BI74" s="74"/>
-      <c r="BJ74" s="74"/>
-      <c r="BK74" s="74"/>
+      <c r="BF74" s="72"/>
+      <c r="BG74" s="72"/>
+      <c r="BH74" s="72"/>
+      <c r="BI74" s="72"/>
+      <c r="BJ74" s="72"/>
+      <c r="BK74" s="72"/>
       <c r="BL74" s="6"/>
       <c r="BM74" s="6"/>
       <c r="BN74" s="6"/>
     </row>
     <row r="75" spans="1:66" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D75" s="92"/>
-      <c r="E75" s="92"/>
-      <c r="F75" s="92"/>
-      <c r="G75" s="92"/>
-      <c r="H75" s="92"/>
-      <c r="I75" s="92"/>
+      <c r="D75" s="79"/>
+      <c r="E75" s="79"/>
+      <c r="F75" s="79"/>
+      <c r="G75" s="79"/>
+      <c r="H75" s="79"/>
+      <c r="I75" s="79"/>
       <c r="J75" s="6"/>
       <c r="K75" s="6"/>
       <c r="L75" s="6"/>
@@ -8165,12 +8527,12 @@
       <c r="BC75" s="6"/>
       <c r="BD75" s="6"/>
       <c r="BE75" s="6"/>
-      <c r="BF75" s="74"/>
-      <c r="BG75" s="74"/>
-      <c r="BH75" s="74"/>
-      <c r="BI75" s="74"/>
-      <c r="BJ75" s="74"/>
-      <c r="BK75" s="74"/>
+      <c r="BF75" s="72"/>
+      <c r="BG75" s="72"/>
+      <c r="BH75" s="72"/>
+      <c r="BI75" s="72"/>
+      <c r="BJ75" s="72"/>
+      <c r="BK75" s="72"/>
       <c r="BL75" s="6"/>
       <c r="BM75" s="6"/>
       <c r="BN75" s="6"/>
@@ -8247,12 +8609,12 @@
       <c r="A77" s="68"/>
       <c r="B77" s="68"/>
       <c r="C77" s="68"/>
-      <c r="D77" s="92"/>
-      <c r="E77" s="92"/>
-      <c r="F77" s="92"/>
-      <c r="G77" s="92"/>
-      <c r="H77" s="92"/>
-      <c r="I77" s="92"/>
+      <c r="D77" s="79"/>
+      <c r="E77" s="79"/>
+      <c r="F77" s="79"/>
+      <c r="G77" s="79"/>
+      <c r="H77" s="79"/>
+      <c r="I77" s="79"/>
       <c r="J77" s="6"/>
       <c r="K77" s="6"/>
       <c r="L77" s="6"/>
@@ -8301,12 +8663,12 @@
       <c r="BC77" s="6"/>
       <c r="BD77" s="6"/>
       <c r="BE77" s="6"/>
-      <c r="BF77" s="74"/>
-      <c r="BG77" s="74"/>
-      <c r="BH77" s="74"/>
-      <c r="BI77" s="74"/>
-      <c r="BJ77" s="74"/>
-      <c r="BK77" s="74"/>
+      <c r="BF77" s="72"/>
+      <c r="BG77" s="72"/>
+      <c r="BH77" s="72"/>
+      <c r="BI77" s="72"/>
+      <c r="BJ77" s="72"/>
+      <c r="BK77" s="72"/>
       <c r="BL77" s="6"/>
       <c r="BM77" s="6"/>
       <c r="BN77" s="6"/>
@@ -8315,12 +8677,12 @@
       <c r="A78" s="68"/>
       <c r="B78" s="68"/>
       <c r="C78" s="68"/>
-      <c r="D78" s="92"/>
-      <c r="E78" s="92"/>
-      <c r="F78" s="92"/>
-      <c r="G78" s="92"/>
-      <c r="H78" s="92"/>
-      <c r="I78" s="92"/>
+      <c r="D78" s="79"/>
+      <c r="E78" s="79"/>
+      <c r="F78" s="79"/>
+      <c r="G78" s="79"/>
+      <c r="H78" s="79"/>
+      <c r="I78" s="79"/>
       <c r="J78" s="6"/>
       <c r="K78" s="6"/>
       <c r="L78" s="6"/>
@@ -8369,12 +8731,12 @@
       <c r="BC78" s="6"/>
       <c r="BD78" s="6"/>
       <c r="BE78" s="6"/>
-      <c r="BF78" s="74"/>
-      <c r="BG78" s="74"/>
-      <c r="BH78" s="74"/>
-      <c r="BI78" s="74"/>
-      <c r="BJ78" s="74"/>
-      <c r="BK78" s="74"/>
+      <c r="BF78" s="72"/>
+      <c r="BG78" s="72"/>
+      <c r="BH78" s="72"/>
+      <c r="BI78" s="72"/>
+      <c r="BJ78" s="72"/>
+      <c r="BK78" s="72"/>
       <c r="BL78" s="6"/>
       <c r="BM78" s="6"/>
       <c r="BN78" s="6"/>
@@ -8383,12 +8745,12 @@
       <c r="A79" s="68"/>
       <c r="B79" s="68"/>
       <c r="C79" s="68"/>
-      <c r="D79" s="92"/>
-      <c r="E79" s="92"/>
-      <c r="F79" s="92"/>
-      <c r="G79" s="92"/>
-      <c r="H79" s="92"/>
-      <c r="I79" s="92"/>
+      <c r="D79" s="79"/>
+      <c r="E79" s="79"/>
+      <c r="F79" s="79"/>
+      <c r="G79" s="79"/>
+      <c r="H79" s="79"/>
+      <c r="I79" s="79"/>
       <c r="J79" s="6"/>
       <c r="K79" s="6"/>
       <c r="L79" s="6"/>
@@ -8437,23 +8799,23 @@
       <c r="BC79" s="6"/>
       <c r="BD79" s="6"/>
       <c r="BE79" s="6"/>
-      <c r="BF79" s="74"/>
-      <c r="BG79" s="74"/>
-      <c r="BH79" s="74"/>
-      <c r="BI79" s="74"/>
-      <c r="BJ79" s="74"/>
-      <c r="BK79" s="74"/>
+      <c r="BF79" s="72"/>
+      <c r="BG79" s="72"/>
+      <c r="BH79" s="72"/>
+      <c r="BI79" s="72"/>
+      <c r="BJ79" s="72"/>
+      <c r="BK79" s="72"/>
       <c r="BL79" s="6"/>
       <c r="BM79" s="6"/>
       <c r="BN79" s="6"/>
     </row>
     <row r="80" spans="1:66" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D80" s="74"/>
-      <c r="E80" s="74"/>
-      <c r="F80" s="74"/>
-      <c r="G80" s="74"/>
-      <c r="H80" s="74"/>
-      <c r="I80" s="74"/>
+      <c r="D80" s="72"/>
+      <c r="E80" s="72"/>
+      <c r="F80" s="72"/>
+      <c r="G80" s="72"/>
+      <c r="H80" s="72"/>
+      <c r="I80" s="72"/>
       <c r="J80" s="6"/>
       <c r="K80" s="6"/>
       <c r="L80" s="6"/>
@@ -8584,12 +8946,12 @@
       <c r="A82" s="68"/>
       <c r="B82" s="68"/>
       <c r="C82" s="68"/>
-      <c r="D82" s="92"/>
-      <c r="E82" s="92"/>
-      <c r="F82" s="92"/>
-      <c r="G82" s="92"/>
-      <c r="H82" s="92"/>
-      <c r="I82" s="92"/>
+      <c r="D82" s="79"/>
+      <c r="E82" s="79"/>
+      <c r="F82" s="79"/>
+      <c r="G82" s="79"/>
+      <c r="H82" s="79"/>
+      <c r="I82" s="79"/>
       <c r="J82" s="6"/>
       <c r="K82" s="6"/>
       <c r="L82" s="6"/>
@@ -8638,12 +9000,12 @@
       <c r="BC82" s="6"/>
       <c r="BD82" s="6"/>
       <c r="BE82" s="6"/>
-      <c r="BF82" s="74"/>
-      <c r="BG82" s="74"/>
-      <c r="BH82" s="74"/>
-      <c r="BI82" s="74"/>
-      <c r="BJ82" s="74"/>
-      <c r="BK82" s="74"/>
+      <c r="BF82" s="72"/>
+      <c r="BG82" s="72"/>
+      <c r="BH82" s="72"/>
+      <c r="BI82" s="72"/>
+      <c r="BJ82" s="72"/>
+      <c r="BK82" s="72"/>
       <c r="BL82" s="6"/>
       <c r="BM82" s="6"/>
       <c r="BN82" s="6"/>
@@ -8652,12 +9014,12 @@
       <c r="A83" s="68"/>
       <c r="B83" s="68"/>
       <c r="C83" s="68"/>
-      <c r="D83" s="74"/>
-      <c r="E83" s="74"/>
-      <c r="F83" s="74"/>
-      <c r="G83" s="74"/>
-      <c r="H83" s="74"/>
-      <c r="I83" s="74"/>
+      <c r="D83" s="72"/>
+      <c r="E83" s="72"/>
+      <c r="F83" s="72"/>
+      <c r="G83" s="72"/>
+      <c r="H83" s="72"/>
+      <c r="I83" s="72"/>
       <c r="J83" s="6"/>
       <c r="K83" s="6"/>
       <c r="L83" s="6"/>
@@ -8720,12 +9082,12 @@
       <c r="A84" s="68"/>
       <c r="B84" s="68"/>
       <c r="C84" s="68"/>
-      <c r="D84" s="74"/>
-      <c r="E84" s="74"/>
-      <c r="F84" s="74"/>
-      <c r="G84" s="74"/>
-      <c r="H84" s="74"/>
-      <c r="I84" s="74"/>
+      <c r="D84" s="72"/>
+      <c r="E84" s="72"/>
+      <c r="F84" s="72"/>
+      <c r="G84" s="72"/>
+      <c r="H84" s="72"/>
+      <c r="I84" s="72"/>
       <c r="J84" s="6"/>
       <c r="K84" s="6"/>
       <c r="L84" s="6"/>
@@ -8788,12 +9150,12 @@
       <c r="A85" s="21"/>
       <c r="B85" s="21"/>
       <c r="C85" s="21"/>
-      <c r="D85" s="92"/>
-      <c r="E85" s="92"/>
-      <c r="F85" s="92"/>
-      <c r="G85" s="92"/>
-      <c r="H85" s="92"/>
-      <c r="I85" s="92"/>
+      <c r="D85" s="79"/>
+      <c r="E85" s="79"/>
+      <c r="F85" s="79"/>
+      <c r="G85" s="79"/>
+      <c r="H85" s="79"/>
+      <c r="I85" s="79"/>
       <c r="J85" s="6"/>
       <c r="K85" s="6"/>
       <c r="L85" s="6"/>
@@ -8842,12 +9204,12 @@
       <c r="BC85" s="6"/>
       <c r="BD85" s="6"/>
       <c r="BE85" s="6"/>
-      <c r="BF85" s="74"/>
-      <c r="BG85" s="74"/>
-      <c r="BH85" s="74"/>
-      <c r="BI85" s="74"/>
-      <c r="BJ85" s="74"/>
-      <c r="BK85" s="74"/>
+      <c r="BF85" s="72"/>
+      <c r="BG85" s="72"/>
+      <c r="BH85" s="72"/>
+      <c r="BI85" s="72"/>
+      <c r="BJ85" s="72"/>
+      <c r="BK85" s="72"/>
       <c r="BL85" s="6"/>
       <c r="BM85" s="6"/>
       <c r="BN85" s="6"/>
@@ -9264,79 +9626,56 @@
       <c r="AB92" s="4"/>
     </row>
   </sheetData>
-  <mergeCells count="145">
-    <mergeCell ref="D17:I17"/>
-    <mergeCell ref="D18:I18"/>
-    <mergeCell ref="D9:I9"/>
-    <mergeCell ref="D10:I10"/>
-    <mergeCell ref="D14:I14"/>
-    <mergeCell ref="D15:I15"/>
-    <mergeCell ref="D38:I38"/>
-    <mergeCell ref="D39:I39"/>
-    <mergeCell ref="D24:I24"/>
-    <mergeCell ref="D25:I25"/>
-    <mergeCell ref="D67:I67"/>
-    <mergeCell ref="D72:I72"/>
-    <mergeCell ref="D64:I64"/>
-    <mergeCell ref="G63:L63"/>
-    <mergeCell ref="G56:L56"/>
-    <mergeCell ref="G57:L57"/>
-    <mergeCell ref="D85:I85"/>
-    <mergeCell ref="D58:I58"/>
-    <mergeCell ref="D59:I59"/>
-    <mergeCell ref="D79:I79"/>
-    <mergeCell ref="D73:I73"/>
-    <mergeCell ref="D80:I80"/>
-    <mergeCell ref="D82:I82"/>
-    <mergeCell ref="D83:I83"/>
-    <mergeCell ref="D84:I84"/>
-    <mergeCell ref="D77:I77"/>
-    <mergeCell ref="D78:I78"/>
-    <mergeCell ref="D74:I74"/>
-    <mergeCell ref="D75:I75"/>
-    <mergeCell ref="G68:L68"/>
-    <mergeCell ref="G69:L69"/>
-    <mergeCell ref="G62:L62"/>
-    <mergeCell ref="G53:L53"/>
-    <mergeCell ref="G54:L54"/>
-    <mergeCell ref="AK53:AP53"/>
-    <mergeCell ref="AQ1:AY1"/>
-    <mergeCell ref="AZ1:BN1"/>
-    <mergeCell ref="AZ3:BB3"/>
-    <mergeCell ref="P1:X1"/>
-    <mergeCell ref="AQ2:AS3"/>
-    <mergeCell ref="AT2:AV3"/>
-    <mergeCell ref="AE2:AG3"/>
-    <mergeCell ref="AH2:AJ3"/>
-    <mergeCell ref="D1:O1"/>
-    <mergeCell ref="AZ2:BE2"/>
-    <mergeCell ref="BF2:BK2"/>
-    <mergeCell ref="BL2:BN2"/>
-    <mergeCell ref="BL3:BN3"/>
-    <mergeCell ref="D12:O12"/>
-    <mergeCell ref="D13:O13"/>
-    <mergeCell ref="D23:O23"/>
-    <mergeCell ref="D22:O22"/>
-    <mergeCell ref="D37:O37"/>
-    <mergeCell ref="P18:X18"/>
-    <mergeCell ref="P19:X19"/>
-    <mergeCell ref="P33:X33"/>
-    <mergeCell ref="BR3:BT3"/>
-    <mergeCell ref="D2:F3"/>
-    <mergeCell ref="G2:I3"/>
-    <mergeCell ref="J2:L3"/>
-    <mergeCell ref="M2:O3"/>
-    <mergeCell ref="P2:R3"/>
-    <mergeCell ref="S2:U3"/>
-    <mergeCell ref="V2:X3"/>
-    <mergeCell ref="Y2:AA3"/>
-    <mergeCell ref="AB2:AD3"/>
-    <mergeCell ref="BC3:BE3"/>
-    <mergeCell ref="BF3:BH3"/>
-    <mergeCell ref="BI3:BK3"/>
-    <mergeCell ref="BO3:BQ3"/>
-    <mergeCell ref="AK2:AM3"/>
-    <mergeCell ref="AN2:AP3"/>
+  <mergeCells count="144">
+    <mergeCell ref="D7:O7"/>
+    <mergeCell ref="D8:O8"/>
+    <mergeCell ref="P9:X9"/>
+    <mergeCell ref="P42:X42"/>
+    <mergeCell ref="BF4:BH4"/>
+    <mergeCell ref="BC4:BE4"/>
+    <mergeCell ref="BI4:BK4"/>
+    <mergeCell ref="AQ4:AS4"/>
+    <mergeCell ref="S4:U4"/>
+    <mergeCell ref="AB4:AD4"/>
+    <mergeCell ref="AK4:AM4"/>
+    <mergeCell ref="AT4:AV4"/>
+    <mergeCell ref="V4:X4"/>
+    <mergeCell ref="AE4:AG4"/>
+    <mergeCell ref="AN4:AP4"/>
+    <mergeCell ref="P4:R4"/>
+    <mergeCell ref="AH4:AJ4"/>
+    <mergeCell ref="Y4:AA4"/>
+    <mergeCell ref="BF5:BH5"/>
+    <mergeCell ref="BI5:BK5"/>
+    <mergeCell ref="D4:F4"/>
+    <mergeCell ref="G4:I4"/>
+    <mergeCell ref="J4:L4"/>
+    <mergeCell ref="M4:O4"/>
+    <mergeCell ref="D5:F5"/>
+    <mergeCell ref="G5:I5"/>
+    <mergeCell ref="Y5:AA5"/>
+    <mergeCell ref="S5:U5"/>
+    <mergeCell ref="V5:X5"/>
+    <mergeCell ref="AH5:AJ5"/>
+    <mergeCell ref="AB5:AD5"/>
+    <mergeCell ref="AE5:AG5"/>
+    <mergeCell ref="J5:L5"/>
+    <mergeCell ref="M5:O5"/>
+    <mergeCell ref="P5:R5"/>
+    <mergeCell ref="BL4:BN4"/>
+    <mergeCell ref="AW4:AY4"/>
+    <mergeCell ref="AZ4:BB4"/>
+    <mergeCell ref="BF79:BK79"/>
+    <mergeCell ref="BF77:BK77"/>
+    <mergeCell ref="BF78:BK78"/>
+    <mergeCell ref="BF69:BK69"/>
+    <mergeCell ref="BF53:BK53"/>
+    <mergeCell ref="BF64:BK64"/>
+    <mergeCell ref="BF73:BK73"/>
+    <mergeCell ref="BF63:BK63"/>
+    <mergeCell ref="BF62:BK62"/>
+    <mergeCell ref="BF54:BK54"/>
+    <mergeCell ref="BL5:BN5"/>
     <mergeCell ref="BF85:BK85"/>
     <mergeCell ref="BF75:BK75"/>
     <mergeCell ref="BF74:BK74"/>
@@ -9361,55 +9700,77 @@
     <mergeCell ref="BC5:BE5"/>
     <mergeCell ref="BF52:BK52"/>
     <mergeCell ref="BF82:BK82"/>
-    <mergeCell ref="BL4:BN4"/>
-    <mergeCell ref="AW4:AY4"/>
-    <mergeCell ref="AZ4:BB4"/>
-    <mergeCell ref="BF79:BK79"/>
-    <mergeCell ref="BF77:BK77"/>
-    <mergeCell ref="BF78:BK78"/>
-    <mergeCell ref="BF69:BK69"/>
-    <mergeCell ref="BF53:BK53"/>
-    <mergeCell ref="BF64:BK64"/>
-    <mergeCell ref="BF73:BK73"/>
-    <mergeCell ref="BF63:BK63"/>
-    <mergeCell ref="BF62:BK62"/>
-    <mergeCell ref="BF54:BK54"/>
-    <mergeCell ref="BL5:BN5"/>
-    <mergeCell ref="D5:F5"/>
-    <mergeCell ref="G5:I5"/>
-    <mergeCell ref="Y5:AA5"/>
-    <mergeCell ref="S5:U5"/>
-    <mergeCell ref="V5:X5"/>
-    <mergeCell ref="AH5:AJ5"/>
-    <mergeCell ref="AB5:AD5"/>
-    <mergeCell ref="AE5:AG5"/>
-    <mergeCell ref="J5:L5"/>
-    <mergeCell ref="M5:O5"/>
-    <mergeCell ref="P5:R5"/>
-    <mergeCell ref="D7:O7"/>
-    <mergeCell ref="D8:O8"/>
-    <mergeCell ref="P9:X9"/>
-    <mergeCell ref="P42:X42"/>
-    <mergeCell ref="BF4:BH4"/>
-    <mergeCell ref="BC4:BE4"/>
-    <mergeCell ref="BI4:BK4"/>
-    <mergeCell ref="AQ4:AS4"/>
-    <mergeCell ref="S4:U4"/>
-    <mergeCell ref="AB4:AD4"/>
-    <mergeCell ref="AK4:AM4"/>
-    <mergeCell ref="AT4:AV4"/>
-    <mergeCell ref="V4:X4"/>
-    <mergeCell ref="AE4:AG4"/>
-    <mergeCell ref="AN4:AP4"/>
-    <mergeCell ref="P4:R4"/>
-    <mergeCell ref="AH4:AJ4"/>
-    <mergeCell ref="Y4:AA4"/>
-    <mergeCell ref="BF5:BH5"/>
-    <mergeCell ref="BI5:BK5"/>
-    <mergeCell ref="D4:F4"/>
-    <mergeCell ref="G4:I4"/>
-    <mergeCell ref="J4:L4"/>
-    <mergeCell ref="M4:O4"/>
+    <mergeCell ref="BR3:BT3"/>
+    <mergeCell ref="D2:F3"/>
+    <mergeCell ref="G2:I3"/>
+    <mergeCell ref="J2:L3"/>
+    <mergeCell ref="M2:O3"/>
+    <mergeCell ref="P2:R3"/>
+    <mergeCell ref="S2:U3"/>
+    <mergeCell ref="V2:X3"/>
+    <mergeCell ref="Y2:AA3"/>
+    <mergeCell ref="AB2:AD3"/>
+    <mergeCell ref="BC3:BE3"/>
+    <mergeCell ref="BF3:BH3"/>
+    <mergeCell ref="BI3:BK3"/>
+    <mergeCell ref="BO3:BQ3"/>
+    <mergeCell ref="AK2:AM3"/>
+    <mergeCell ref="AN2:AP3"/>
+    <mergeCell ref="G53:L53"/>
+    <mergeCell ref="G54:L54"/>
+    <mergeCell ref="AQ1:AY1"/>
+    <mergeCell ref="AZ1:BN1"/>
+    <mergeCell ref="AZ3:BB3"/>
+    <mergeCell ref="P1:X1"/>
+    <mergeCell ref="AQ2:AS3"/>
+    <mergeCell ref="AT2:AV3"/>
+    <mergeCell ref="AE2:AG3"/>
+    <mergeCell ref="AH2:AJ3"/>
+    <mergeCell ref="D1:O1"/>
+    <mergeCell ref="AZ2:BE2"/>
+    <mergeCell ref="BF2:BK2"/>
+    <mergeCell ref="BL2:BN2"/>
+    <mergeCell ref="BL3:BN3"/>
+    <mergeCell ref="D12:O12"/>
+    <mergeCell ref="D13:O13"/>
+    <mergeCell ref="D23:O23"/>
+    <mergeCell ref="D22:O22"/>
+    <mergeCell ref="D37:O37"/>
+    <mergeCell ref="P18:X18"/>
+    <mergeCell ref="P19:X19"/>
+    <mergeCell ref="P33:X33"/>
+    <mergeCell ref="D67:I67"/>
+    <mergeCell ref="D72:I72"/>
+    <mergeCell ref="D64:I64"/>
+    <mergeCell ref="G63:L63"/>
+    <mergeCell ref="G56:L56"/>
+    <mergeCell ref="G57:L57"/>
+    <mergeCell ref="D85:I85"/>
+    <mergeCell ref="D58:I58"/>
+    <mergeCell ref="D59:I59"/>
+    <mergeCell ref="D79:I79"/>
+    <mergeCell ref="D73:I73"/>
+    <mergeCell ref="D80:I80"/>
+    <mergeCell ref="D82:I82"/>
+    <mergeCell ref="D83:I83"/>
+    <mergeCell ref="D84:I84"/>
+    <mergeCell ref="D77:I77"/>
+    <mergeCell ref="D78:I78"/>
+    <mergeCell ref="D74:I74"/>
+    <mergeCell ref="D75:I75"/>
+    <mergeCell ref="G68:L68"/>
+    <mergeCell ref="G69:L69"/>
+    <mergeCell ref="G62:L62"/>
+    <mergeCell ref="D17:I17"/>
+    <mergeCell ref="D18:I18"/>
+    <mergeCell ref="D9:I9"/>
+    <mergeCell ref="D10:I10"/>
+    <mergeCell ref="D14:I14"/>
+    <mergeCell ref="D15:I15"/>
+    <mergeCell ref="D38:I38"/>
+    <mergeCell ref="D39:I39"/>
+    <mergeCell ref="D24:I24"/>
+    <mergeCell ref="D25:I25"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Finished up to 6th grade
</commit_message>
<xml_diff>
--- a/Rozklad_3zaizd.xlsx
+++ b/Rozklad_3zaizd.xlsx
@@ -55,7 +55,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="877" uniqueCount="267">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="919" uniqueCount="281">
   <si>
     <t>І</t>
   </si>
@@ -856,6 +856,48 @@
   </si>
   <si>
     <t>Лісівництво в т.ч. рекреаційне</t>
+  </si>
+  <si>
+    <t>Регіональна економічна та соціальна географія світу</t>
+  </si>
+  <si>
+    <t>Регіональна економічна та соціальна географія світу (іспит)</t>
+  </si>
+  <si>
+    <t>Інформаційні технології в географії (іспит)</t>
+  </si>
+  <si>
+    <t>Картографічне моделювання</t>
+  </si>
+  <si>
+    <t>Картографічне моделювання (іспит)</t>
+  </si>
+  <si>
+    <t>Моніторинг навколишнього природного середовища</t>
+  </si>
+  <si>
+    <t>Моніторинг навколишнього природного середовища (залік)</t>
+  </si>
+  <si>
+    <t>Управління природокористуванням</t>
+  </si>
+  <si>
+    <t>Управління природокористуванням (залік)</t>
+  </si>
+  <si>
+    <t>Галузеві кадастри</t>
+  </si>
+  <si>
+    <t>Галузеві кадастри (іспит)</t>
+  </si>
+  <si>
+    <t>проф. Перович Л.М.</t>
+  </si>
+  <si>
+    <t>Конструктивно-географічні основи раціонального природокористування</t>
+  </si>
+  <si>
+    <t>Конструктивно-географічні основи раціонального природокористування (залік)</t>
   </si>
 </sst>
 </file>
@@ -1115,7 +1157,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="98">
+  <cellXfs count="104">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -1219,9 +1261,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
@@ -1327,86 +1366,107 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1468,7 +1528,7 @@
     </a:clrScheme>
     <a:fontScheme name="Офіс">
       <a:majorFont>
-        <a:latin typeface="Calibri Light"/>
+        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック Light"/>
@@ -1503,7 +1563,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック"/>
@@ -1691,10 +1751,10 @@
   <dimension ref="A1:BT92"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <pane xSplit="3" ySplit="3" topLeftCell="D22" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="3" ySplit="3" topLeftCell="D13" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="AT20" sqref="AT20"/>
+      <selection pane="bottomRight" activeCell="X26" sqref="X26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1775,372 +1835,372 @@
       <c r="A1" s="1"/>
       <c r="B1" s="1"/>
       <c r="C1" s="1"/>
-      <c r="D1" s="80" t="s">
+      <c r="D1" s="90" t="s">
         <v>14</v>
       </c>
-      <c r="E1" s="81"/>
-      <c r="F1" s="81"/>
-      <c r="G1" s="81"/>
-      <c r="H1" s="81"/>
-      <c r="I1" s="81"/>
-      <c r="J1" s="81"/>
-      <c r="K1" s="81"/>
-      <c r="L1" s="81"/>
-      <c r="M1" s="81"/>
-      <c r="N1" s="81"/>
-      <c r="O1" s="82"/>
-      <c r="P1" s="80" t="s">
+      <c r="E1" s="91"/>
+      <c r="F1" s="91"/>
+      <c r="G1" s="91"/>
+      <c r="H1" s="91"/>
+      <c r="I1" s="91"/>
+      <c r="J1" s="91"/>
+      <c r="K1" s="91"/>
+      <c r="L1" s="91"/>
+      <c r="M1" s="91"/>
+      <c r="N1" s="91"/>
+      <c r="O1" s="92"/>
+      <c r="P1" s="90" t="s">
         <v>15</v>
       </c>
-      <c r="Q1" s="81"/>
-      <c r="R1" s="81"/>
-      <c r="S1" s="81"/>
-      <c r="T1" s="81"/>
-      <c r="U1" s="81"/>
-      <c r="V1" s="81"/>
-      <c r="W1" s="81"/>
-      <c r="X1" s="82"/>
-      <c r="Y1" s="80" t="s">
+      <c r="Q1" s="91"/>
+      <c r="R1" s="91"/>
+      <c r="S1" s="91"/>
+      <c r="T1" s="91"/>
+      <c r="U1" s="91"/>
+      <c r="V1" s="91"/>
+      <c r="W1" s="91"/>
+      <c r="X1" s="92"/>
+      <c r="Y1" s="90" t="s">
         <v>16</v>
       </c>
-      <c r="Z1" s="81"/>
-      <c r="AA1" s="81"/>
-      <c r="AB1" s="81"/>
-      <c r="AC1" s="81"/>
-      <c r="AD1" s="81"/>
-      <c r="AE1" s="81"/>
-      <c r="AF1" s="81"/>
-      <c r="AG1" s="82"/>
-      <c r="AH1" s="80" t="s">
+      <c r="Z1" s="91"/>
+      <c r="AA1" s="91"/>
+      <c r="AB1" s="91"/>
+      <c r="AC1" s="91"/>
+      <c r="AD1" s="91"/>
+      <c r="AE1" s="91"/>
+      <c r="AF1" s="91"/>
+      <c r="AG1" s="92"/>
+      <c r="AH1" s="90" t="s">
         <v>17</v>
       </c>
-      <c r="AI1" s="81"/>
-      <c r="AJ1" s="81"/>
-      <c r="AK1" s="81"/>
-      <c r="AL1" s="81"/>
-      <c r="AM1" s="81"/>
-      <c r="AN1" s="81"/>
-      <c r="AO1" s="81"/>
-      <c r="AP1" s="82"/>
-      <c r="AQ1" s="80" t="s">
+      <c r="AI1" s="91"/>
+      <c r="AJ1" s="91"/>
+      <c r="AK1" s="91"/>
+      <c r="AL1" s="91"/>
+      <c r="AM1" s="91"/>
+      <c r="AN1" s="91"/>
+      <c r="AO1" s="91"/>
+      <c r="AP1" s="92"/>
+      <c r="AQ1" s="90" t="s">
         <v>18</v>
       </c>
-      <c r="AR1" s="81"/>
-      <c r="AS1" s="81"/>
-      <c r="AT1" s="81"/>
-      <c r="AU1" s="81"/>
-      <c r="AV1" s="81"/>
-      <c r="AW1" s="81"/>
-      <c r="AX1" s="81"/>
-      <c r="AY1" s="82"/>
-      <c r="AZ1" s="81" t="s">
+      <c r="AR1" s="91"/>
+      <c r="AS1" s="91"/>
+      <c r="AT1" s="91"/>
+      <c r="AU1" s="91"/>
+      <c r="AV1" s="91"/>
+      <c r="AW1" s="91"/>
+      <c r="AX1" s="91"/>
+      <c r="AY1" s="92"/>
+      <c r="AZ1" s="91" t="s">
         <v>19</v>
       </c>
-      <c r="BA1" s="81"/>
-      <c r="BB1" s="81"/>
-      <c r="BC1" s="81"/>
-      <c r="BD1" s="81"/>
-      <c r="BE1" s="81"/>
-      <c r="BF1" s="81"/>
-      <c r="BG1" s="81"/>
-      <c r="BH1" s="81"/>
-      <c r="BI1" s="81"/>
-      <c r="BJ1" s="81"/>
-      <c r="BK1" s="81"/>
-      <c r="BL1" s="81"/>
-      <c r="BM1" s="81"/>
-      <c r="BN1" s="82"/>
+      <c r="BA1" s="91"/>
+      <c r="BB1" s="91"/>
+      <c r="BC1" s="91"/>
+      <c r="BD1" s="91"/>
+      <c r="BE1" s="91"/>
+      <c r="BF1" s="91"/>
+      <c r="BG1" s="91"/>
+      <c r="BH1" s="91"/>
+      <c r="BI1" s="91"/>
+      <c r="BJ1" s="91"/>
+      <c r="BK1" s="91"/>
+      <c r="BL1" s="91"/>
+      <c r="BM1" s="91"/>
+      <c r="BN1" s="92"/>
     </row>
     <row r="2" spans="1:72" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="1"/>
       <c r="B2" s="1"/>
       <c r="C2" s="1"/>
-      <c r="D2" s="83" t="s">
+      <c r="D2" s="81" t="s">
         <v>24</v>
       </c>
-      <c r="E2" s="84"/>
-      <c r="F2" s="86"/>
-      <c r="G2" s="87" t="s">
+      <c r="E2" s="79"/>
+      <c r="F2" s="82"/>
+      <c r="G2" s="78" t="s">
         <v>25</v>
       </c>
-      <c r="H2" s="84"/>
-      <c r="I2" s="86"/>
-      <c r="J2" s="87" t="s">
+      <c r="H2" s="79"/>
+      <c r="I2" s="82"/>
+      <c r="J2" s="78" t="s">
         <v>26</v>
       </c>
-      <c r="K2" s="84"/>
-      <c r="L2" s="86"/>
-      <c r="M2" s="84" t="s">
+      <c r="K2" s="79"/>
+      <c r="L2" s="82"/>
+      <c r="M2" s="79" t="s">
         <v>27</v>
       </c>
-      <c r="N2" s="84"/>
+      <c r="N2" s="79"/>
       <c r="O2" s="88"/>
-      <c r="P2" s="83" t="s">
+      <c r="P2" s="81" t="s">
         <v>28</v>
       </c>
-      <c r="Q2" s="84"/>
-      <c r="R2" s="86"/>
-      <c r="S2" s="87" t="s">
+      <c r="Q2" s="79"/>
+      <c r="R2" s="82"/>
+      <c r="S2" s="78" t="s">
         <v>26</v>
       </c>
-      <c r="T2" s="84"/>
-      <c r="U2" s="86"/>
-      <c r="V2" s="84" t="s">
+      <c r="T2" s="79"/>
+      <c r="U2" s="82"/>
+      <c r="V2" s="79" t="s">
         <v>29</v>
       </c>
-      <c r="W2" s="84"/>
+      <c r="W2" s="79"/>
       <c r="X2" s="88"/>
-      <c r="Y2" s="83" t="s">
+      <c r="Y2" s="81" t="s">
         <v>28</v>
       </c>
-      <c r="Z2" s="84"/>
-      <c r="AA2" s="86"/>
-      <c r="AB2" s="87" t="s">
+      <c r="Z2" s="79"/>
+      <c r="AA2" s="82"/>
+      <c r="AB2" s="78" t="s">
         <v>26</v>
       </c>
-      <c r="AC2" s="84"/>
-      <c r="AD2" s="86"/>
-      <c r="AE2" s="84" t="s">
+      <c r="AC2" s="79"/>
+      <c r="AD2" s="82"/>
+      <c r="AE2" s="79" t="s">
         <v>29</v>
       </c>
-      <c r="AF2" s="84"/>
+      <c r="AF2" s="79"/>
       <c r="AG2" s="88"/>
-      <c r="AH2" s="83" t="s">
+      <c r="AH2" s="81" t="s">
         <v>28</v>
       </c>
-      <c r="AI2" s="84"/>
-      <c r="AJ2" s="86"/>
-      <c r="AK2" s="87" t="s">
+      <c r="AI2" s="79"/>
+      <c r="AJ2" s="82"/>
+      <c r="AK2" s="78" t="s">
         <v>26</v>
       </c>
-      <c r="AL2" s="84"/>
-      <c r="AM2" s="86"/>
-      <c r="AN2" s="84" t="s">
+      <c r="AL2" s="79"/>
+      <c r="AM2" s="82"/>
+      <c r="AN2" s="79" t="s">
         <v>29</v>
       </c>
-      <c r="AO2" s="84"/>
+      <c r="AO2" s="79"/>
       <c r="AP2" s="88"/>
-      <c r="AQ2" s="83" t="s">
+      <c r="AQ2" s="81" t="s">
         <v>28</v>
       </c>
-      <c r="AR2" s="84"/>
-      <c r="AS2" s="86"/>
-      <c r="AT2" s="87" t="s">
+      <c r="AR2" s="79"/>
+      <c r="AS2" s="82"/>
+      <c r="AT2" s="78" t="s">
         <v>26</v>
       </c>
-      <c r="AU2" s="84"/>
-      <c r="AV2" s="86"/>
-      <c r="AW2" s="84" t="s">
+      <c r="AU2" s="79"/>
+      <c r="AV2" s="82"/>
+      <c r="AW2" s="79" t="s">
         <v>29</v>
       </c>
-      <c r="AX2" s="84"/>
+      <c r="AX2" s="79"/>
       <c r="AY2" s="88"/>
-      <c r="AZ2" s="83" t="s">
+      <c r="AZ2" s="81" t="s">
         <v>30</v>
       </c>
-      <c r="BA2" s="84"/>
-      <c r="BB2" s="84"/>
-      <c r="BC2" s="84"/>
-      <c r="BD2" s="84"/>
-      <c r="BE2" s="86"/>
-      <c r="BF2" s="87" t="s">
+      <c r="BA2" s="79"/>
+      <c r="BB2" s="79"/>
+      <c r="BC2" s="79"/>
+      <c r="BD2" s="79"/>
+      <c r="BE2" s="82"/>
+      <c r="BF2" s="78" t="s">
         <v>26</v>
       </c>
-      <c r="BG2" s="84"/>
-      <c r="BH2" s="84"/>
-      <c r="BI2" s="84"/>
-      <c r="BJ2" s="84"/>
-      <c r="BK2" s="86"/>
-      <c r="BL2" s="84" t="s">
+      <c r="BG2" s="79"/>
+      <c r="BH2" s="79"/>
+      <c r="BI2" s="79"/>
+      <c r="BJ2" s="79"/>
+      <c r="BK2" s="82"/>
+      <c r="BL2" s="79" t="s">
         <v>35</v>
       </c>
-      <c r="BM2" s="84"/>
+      <c r="BM2" s="79"/>
       <c r="BN2" s="88"/>
     </row>
     <row r="3" spans="1:72" x14ac:dyDescent="0.25">
-      <c r="D3" s="83"/>
-      <c r="E3" s="84"/>
-      <c r="F3" s="86"/>
-      <c r="G3" s="87"/>
-      <c r="H3" s="84"/>
-      <c r="I3" s="86"/>
-      <c r="J3" s="87"/>
-      <c r="K3" s="84"/>
-      <c r="L3" s="86"/>
-      <c r="M3" s="84"/>
-      <c r="N3" s="84"/>
+      <c r="D3" s="81"/>
+      <c r="E3" s="79"/>
+      <c r="F3" s="82"/>
+      <c r="G3" s="78"/>
+      <c r="H3" s="79"/>
+      <c r="I3" s="82"/>
+      <c r="J3" s="78"/>
+      <c r="K3" s="79"/>
+      <c r="L3" s="82"/>
+      <c r="M3" s="79"/>
+      <c r="N3" s="79"/>
       <c r="O3" s="88"/>
-      <c r="P3" s="83"/>
-      <c r="Q3" s="84"/>
-      <c r="R3" s="86"/>
-      <c r="S3" s="87"/>
-      <c r="T3" s="84"/>
-      <c r="U3" s="86"/>
-      <c r="V3" s="84"/>
-      <c r="W3" s="84"/>
+      <c r="P3" s="81"/>
+      <c r="Q3" s="79"/>
+      <c r="R3" s="82"/>
+      <c r="S3" s="78"/>
+      <c r="T3" s="79"/>
+      <c r="U3" s="82"/>
+      <c r="V3" s="79"/>
+      <c r="W3" s="79"/>
       <c r="X3" s="88"/>
-      <c r="Y3" s="83"/>
-      <c r="Z3" s="84"/>
-      <c r="AA3" s="86"/>
-      <c r="AB3" s="87"/>
-      <c r="AC3" s="84"/>
-      <c r="AD3" s="86"/>
-      <c r="AE3" s="84"/>
-      <c r="AF3" s="84"/>
+      <c r="Y3" s="81"/>
+      <c r="Z3" s="79"/>
+      <c r="AA3" s="82"/>
+      <c r="AB3" s="78"/>
+      <c r="AC3" s="79"/>
+      <c r="AD3" s="82"/>
+      <c r="AE3" s="79"/>
+      <c r="AF3" s="79"/>
       <c r="AG3" s="88"/>
-      <c r="AH3" s="83"/>
-      <c r="AI3" s="84"/>
-      <c r="AJ3" s="86"/>
-      <c r="AK3" s="87"/>
-      <c r="AL3" s="84"/>
-      <c r="AM3" s="86"/>
-      <c r="AN3" s="84"/>
-      <c r="AO3" s="84"/>
+      <c r="AH3" s="81"/>
+      <c r="AI3" s="79"/>
+      <c r="AJ3" s="82"/>
+      <c r="AK3" s="78"/>
+      <c r="AL3" s="79"/>
+      <c r="AM3" s="82"/>
+      <c r="AN3" s="79"/>
+      <c r="AO3" s="79"/>
       <c r="AP3" s="88"/>
-      <c r="AQ3" s="83"/>
-      <c r="AR3" s="84"/>
-      <c r="AS3" s="86"/>
-      <c r="AT3" s="87"/>
-      <c r="AU3" s="84"/>
-      <c r="AV3" s="86"/>
-      <c r="AW3" s="84"/>
-      <c r="AX3" s="84"/>
+      <c r="AQ3" s="81"/>
+      <c r="AR3" s="79"/>
+      <c r="AS3" s="82"/>
+      <c r="AT3" s="78"/>
+      <c r="AU3" s="79"/>
+      <c r="AV3" s="82"/>
+      <c r="AW3" s="79"/>
+      <c r="AX3" s="79"/>
       <c r="AY3" s="88"/>
-      <c r="AZ3" s="83" t="s">
+      <c r="AZ3" s="81" t="s">
         <v>31</v>
       </c>
-      <c r="BA3" s="84"/>
-      <c r="BB3" s="85"/>
-      <c r="BC3" s="84" t="s">
+      <c r="BA3" s="79"/>
+      <c r="BB3" s="80"/>
+      <c r="BC3" s="79" t="s">
         <v>32</v>
       </c>
-      <c r="BD3" s="84"/>
-      <c r="BE3" s="86"/>
-      <c r="BF3" s="87" t="s">
+      <c r="BD3" s="79"/>
+      <c r="BE3" s="82"/>
+      <c r="BF3" s="78" t="s">
         <v>33</v>
       </c>
-      <c r="BG3" s="84"/>
-      <c r="BH3" s="85"/>
-      <c r="BI3" s="84" t="s">
+      <c r="BG3" s="79"/>
+      <c r="BH3" s="80"/>
+      <c r="BI3" s="79" t="s">
         <v>34</v>
       </c>
-      <c r="BJ3" s="84"/>
-      <c r="BK3" s="86"/>
-      <c r="BL3" s="84" t="s">
+      <c r="BJ3" s="79"/>
+      <c r="BK3" s="82"/>
+      <c r="BL3" s="79" t="s">
         <v>34</v>
       </c>
-      <c r="BM3" s="84"/>
+      <c r="BM3" s="79"/>
       <c r="BN3" s="88"/>
-      <c r="BO3" s="90"/>
-      <c r="BP3" s="90"/>
-      <c r="BQ3" s="90"/>
-      <c r="BR3" s="90"/>
-      <c r="BS3" s="90"/>
-      <c r="BT3" s="90"/>
+      <c r="BO3" s="93"/>
+      <c r="BP3" s="93"/>
+      <c r="BQ3" s="93"/>
+      <c r="BR3" s="93"/>
+      <c r="BS3" s="93"/>
+      <c r="BT3" s="93"/>
     </row>
     <row r="4" spans="1:72" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D4" s="83" t="s">
+      <c r="D4" s="81" t="s">
         <v>41</v>
       </c>
-      <c r="E4" s="84"/>
-      <c r="F4" s="86"/>
-      <c r="G4" s="83" t="s">
+      <c r="E4" s="79"/>
+      <c r="F4" s="82"/>
+      <c r="G4" s="81" t="s">
         <v>41</v>
       </c>
-      <c r="H4" s="84"/>
-      <c r="I4" s="86"/>
-      <c r="J4" s="83" t="s">
+      <c r="H4" s="79"/>
+      <c r="I4" s="82"/>
+      <c r="J4" s="81" t="s">
         <v>41</v>
       </c>
-      <c r="K4" s="84"/>
-      <c r="L4" s="86"/>
-      <c r="M4" s="83" t="s">
+      <c r="K4" s="79"/>
+      <c r="L4" s="82"/>
+      <c r="M4" s="81" t="s">
         <v>41</v>
       </c>
-      <c r="N4" s="84"/>
-      <c r="O4" s="86"/>
-      <c r="P4" s="83" t="s">
+      <c r="N4" s="79"/>
+      <c r="O4" s="82"/>
+      <c r="P4" s="81" t="s">
         <v>50</v>
       </c>
-      <c r="Q4" s="84"/>
-      <c r="R4" s="86"/>
-      <c r="S4" s="83" t="s">
+      <c r="Q4" s="79"/>
+      <c r="R4" s="82"/>
+      <c r="S4" s="81" t="s">
         <v>50</v>
       </c>
-      <c r="T4" s="84"/>
-      <c r="U4" s="86"/>
-      <c r="V4" s="83" t="s">
+      <c r="T4" s="79"/>
+      <c r="U4" s="82"/>
+      <c r="V4" s="81" t="s">
         <v>50</v>
       </c>
-      <c r="W4" s="84"/>
-      <c r="X4" s="86"/>
-      <c r="Y4" s="83" t="s">
+      <c r="W4" s="79"/>
+      <c r="X4" s="82"/>
+      <c r="Y4" s="81" t="s">
         <v>52</v>
       </c>
-      <c r="Z4" s="84"/>
-      <c r="AA4" s="86"/>
-      <c r="AB4" s="83" t="s">
+      <c r="Z4" s="79"/>
+      <c r="AA4" s="82"/>
+      <c r="AB4" s="81" t="s">
         <v>50</v>
       </c>
-      <c r="AC4" s="84"/>
-      <c r="AD4" s="86"/>
-      <c r="AE4" s="83" t="s">
+      <c r="AC4" s="79"/>
+      <c r="AD4" s="82"/>
+      <c r="AE4" s="81" t="s">
         <v>52</v>
       </c>
-      <c r="AF4" s="84"/>
-      <c r="AG4" s="86"/>
-      <c r="AH4" s="83" t="s">
+      <c r="AF4" s="79"/>
+      <c r="AG4" s="82"/>
+      <c r="AH4" s="81" t="s">
         <v>52</v>
       </c>
-      <c r="AI4" s="84"/>
-      <c r="AJ4" s="86"/>
-      <c r="AK4" s="83" t="s">
+      <c r="AI4" s="79"/>
+      <c r="AJ4" s="82"/>
+      <c r="AK4" s="81" t="s">
         <v>50</v>
       </c>
-      <c r="AL4" s="84"/>
-      <c r="AM4" s="86"/>
-      <c r="AN4" s="83" t="s">
+      <c r="AL4" s="79"/>
+      <c r="AM4" s="82"/>
+      <c r="AN4" s="81" t="s">
         <v>52</v>
       </c>
-      <c r="AO4" s="84"/>
-      <c r="AP4" s="86"/>
-      <c r="AQ4" s="83"/>
-      <c r="AR4" s="84"/>
-      <c r="AS4" s="86"/>
-      <c r="AT4" s="83" t="s">
+      <c r="AO4" s="79"/>
+      <c r="AP4" s="82"/>
+      <c r="AQ4" s="81"/>
+      <c r="AR4" s="79"/>
+      <c r="AS4" s="82"/>
+      <c r="AT4" s="81" t="s">
         <v>50</v>
       </c>
-      <c r="AU4" s="84"/>
-      <c r="AV4" s="86"/>
-      <c r="AW4" s="87" t="s">
+      <c r="AU4" s="79"/>
+      <c r="AV4" s="82"/>
+      <c r="AW4" s="78" t="s">
         <v>58</v>
       </c>
-      <c r="AX4" s="84"/>
+      <c r="AX4" s="79"/>
       <c r="AY4" s="88"/>
-      <c r="AZ4" s="83" t="s">
+      <c r="AZ4" s="81" t="s">
         <v>52</v>
       </c>
-      <c r="BA4" s="84"/>
-      <c r="BB4" s="86"/>
-      <c r="BC4" s="83" t="s">
+      <c r="BA4" s="79"/>
+      <c r="BB4" s="82"/>
+      <c r="BC4" s="81" t="s">
         <v>52</v>
       </c>
-      <c r="BD4" s="84"/>
-      <c r="BE4" s="86"/>
-      <c r="BF4" s="87" t="s">
+      <c r="BD4" s="79"/>
+      <c r="BE4" s="82"/>
+      <c r="BF4" s="78" t="s">
         <v>54</v>
       </c>
-      <c r="BG4" s="84"/>
-      <c r="BH4" s="85"/>
-      <c r="BI4" s="95" t="s">
+      <c r="BG4" s="79"/>
+      <c r="BH4" s="80"/>
+      <c r="BI4" s="83" t="s">
         <v>55</v>
       </c>
-      <c r="BJ4" s="96"/>
-      <c r="BK4" s="97"/>
-      <c r="BL4" s="91" t="s">
+      <c r="BJ4" s="84"/>
+      <c r="BK4" s="85"/>
+      <c r="BL4" s="86" t="s">
         <v>56</v>
       </c>
-      <c r="BM4" s="84"/>
+      <c r="BM4" s="79"/>
       <c r="BN4" s="88"/>
       <c r="BO4" s="25"/>
       <c r="BP4" s="25"/>
@@ -2150,102 +2210,102 @@
       <c r="BT4" s="25"/>
     </row>
     <row r="5" spans="1:72" x14ac:dyDescent="0.25">
-      <c r="D5" s="77" t="s">
+      <c r="D5" s="87" t="s">
         <v>40</v>
       </c>
-      <c r="E5" s="77"/>
-      <c r="F5" s="77"/>
-      <c r="G5" s="77" t="s">
+      <c r="E5" s="87"/>
+      <c r="F5" s="87"/>
+      <c r="G5" s="87" t="s">
         <v>40</v>
       </c>
-      <c r="H5" s="77"/>
-      <c r="I5" s="77"/>
-      <c r="J5" s="77" t="s">
+      <c r="H5" s="87"/>
+      <c r="I5" s="87"/>
+      <c r="J5" s="87" t="s">
         <v>40</v>
       </c>
-      <c r="K5" s="77"/>
-      <c r="L5" s="77"/>
-      <c r="M5" s="77" t="s">
+      <c r="K5" s="87"/>
+      <c r="L5" s="87"/>
+      <c r="M5" s="87" t="s">
         <v>40</v>
       </c>
-      <c r="N5" s="77"/>
-      <c r="O5" s="77"/>
-      <c r="P5" s="83" t="s">
+      <c r="N5" s="87"/>
+      <c r="O5" s="87"/>
+      <c r="P5" s="81" t="s">
         <v>51</v>
       </c>
-      <c r="Q5" s="84"/>
-      <c r="R5" s="86"/>
-      <c r="S5" s="83" t="s">
+      <c r="Q5" s="79"/>
+      <c r="R5" s="82"/>
+      <c r="S5" s="81" t="s">
         <v>51</v>
       </c>
-      <c r="T5" s="84"/>
-      <c r="U5" s="86"/>
-      <c r="V5" s="83" t="s">
+      <c r="T5" s="79"/>
+      <c r="U5" s="82"/>
+      <c r="V5" s="81" t="s">
         <v>51</v>
       </c>
-      <c r="W5" s="84"/>
-      <c r="X5" s="86"/>
-      <c r="Y5" s="83" t="s">
+      <c r="W5" s="79"/>
+      <c r="X5" s="82"/>
+      <c r="Y5" s="81" t="s">
         <v>53</v>
       </c>
-      <c r="Z5" s="84"/>
-      <c r="AA5" s="86"/>
-      <c r="AB5" s="83" t="s">
+      <c r="Z5" s="79"/>
+      <c r="AA5" s="82"/>
+      <c r="AB5" s="81" t="s">
         <v>51</v>
       </c>
-      <c r="AC5" s="84"/>
-      <c r="AD5" s="86"/>
-      <c r="AE5" s="83" t="s">
+      <c r="AC5" s="79"/>
+      <c r="AD5" s="82"/>
+      <c r="AE5" s="81" t="s">
         <v>53</v>
       </c>
-      <c r="AF5" s="84"/>
-      <c r="AG5" s="86"/>
-      <c r="AH5" s="83" t="s">
+      <c r="AF5" s="79"/>
+      <c r="AG5" s="82"/>
+      <c r="AH5" s="81" t="s">
         <v>53</v>
       </c>
-      <c r="AI5" s="84"/>
-      <c r="AJ5" s="86"/>
-      <c r="AK5" s="83" t="s">
+      <c r="AI5" s="79"/>
+      <c r="AJ5" s="82"/>
+      <c r="AK5" s="81" t="s">
         <v>51</v>
       </c>
-      <c r="AL5" s="84"/>
-      <c r="AM5" s="86"/>
-      <c r="AN5" s="83" t="s">
+      <c r="AL5" s="79"/>
+      <c r="AM5" s="82"/>
+      <c r="AN5" s="81" t="s">
         <v>53</v>
       </c>
-      <c r="AO5" s="84"/>
-      <c r="AP5" s="86"/>
-      <c r="AQ5" s="83"/>
-      <c r="AR5" s="84"/>
-      <c r="AS5" s="86"/>
-      <c r="AT5" s="83" t="s">
+      <c r="AO5" s="79"/>
+      <c r="AP5" s="82"/>
+      <c r="AQ5" s="81"/>
+      <c r="AR5" s="79"/>
+      <c r="AS5" s="82"/>
+      <c r="AT5" s="81" t="s">
         <v>51</v>
       </c>
-      <c r="AU5" s="84"/>
-      <c r="AV5" s="86"/>
-      <c r="AW5" s="87"/>
-      <c r="AX5" s="84"/>
+      <c r="AU5" s="79"/>
+      <c r="AV5" s="82"/>
+      <c r="AW5" s="78"/>
+      <c r="AX5" s="79"/>
       <c r="AY5" s="88"/>
-      <c r="AZ5" s="83" t="s">
+      <c r="AZ5" s="81" t="s">
         <v>53</v>
       </c>
-      <c r="BA5" s="84"/>
-      <c r="BB5" s="86"/>
-      <c r="BC5" s="83" t="s">
+      <c r="BA5" s="79"/>
+      <c r="BB5" s="82"/>
+      <c r="BC5" s="81" t="s">
         <v>53</v>
       </c>
-      <c r="BD5" s="84"/>
-      <c r="BE5" s="86"/>
-      <c r="BF5" s="87"/>
-      <c r="BG5" s="84"/>
-      <c r="BH5" s="85"/>
-      <c r="BI5" s="91"/>
-      <c r="BJ5" s="84"/>
-      <c r="BK5" s="86"/>
-      <c r="BL5" s="87" t="s">
+      <c r="BD5" s="79"/>
+      <c r="BE5" s="82"/>
+      <c r="BF5" s="78"/>
+      <c r="BG5" s="79"/>
+      <c r="BH5" s="80"/>
+      <c r="BI5" s="86"/>
+      <c r="BJ5" s="79"/>
+      <c r="BK5" s="82"/>
+      <c r="BL5" s="78" t="s">
         <v>57</v>
       </c>
-      <c r="BM5" s="84"/>
+      <c r="BM5" s="79"/>
       <c r="BN5" s="88"/>
       <c r="BO5" s="25"/>
       <c r="BP5" s="25"/>
@@ -2467,119 +2527,114 @@
       <c r="C7" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="D7" s="92" t="s">
+      <c r="D7" s="72" t="s">
         <v>90</v>
       </c>
-      <c r="E7" s="93"/>
-      <c r="F7" s="93"/>
-      <c r="G7" s="93"/>
-      <c r="H7" s="93"/>
-      <c r="I7" s="93"/>
-      <c r="J7" s="93"/>
-      <c r="K7" s="93"/>
-      <c r="L7" s="93"/>
-      <c r="M7" s="93"/>
-      <c r="N7" s="93"/>
-      <c r="O7" s="94"/>
-      <c r="P7" s="44" t="s">
+      <c r="E7" s="73"/>
+      <c r="F7" s="73"/>
+      <c r="G7" s="73"/>
+      <c r="H7" s="73"/>
+      <c r="I7" s="73"/>
+      <c r="J7" s="73"/>
+      <c r="K7" s="73"/>
+      <c r="L7" s="73"/>
+      <c r="M7" s="73"/>
+      <c r="N7" s="73"/>
+      <c r="O7" s="74"/>
+      <c r="P7" s="43" t="s">
         <v>118</v>
       </c>
-      <c r="Q7" s="37" t="s">
+      <c r="Q7" s="36" t="s">
         <v>119</v>
       </c>
-      <c r="R7" s="52"/>
+      <c r="R7" s="51"/>
       <c r="S7" s="10" t="s">
         <v>73</v>
       </c>
       <c r="T7" s="6" t="s">
         <v>98</v>
       </c>
-      <c r="U7" s="52"/>
+      <c r="U7" s="51"/>
       <c r="V7" s="6" t="s">
         <v>138</v>
       </c>
       <c r="W7" s="6" t="s">
         <v>104</v>
       </c>
-      <c r="X7" s="43"/>
-      <c r="Y7" s="45" t="s">
+      <c r="X7" s="42"/>
+      <c r="Y7" s="44" t="s">
         <v>157</v>
       </c>
-      <c r="Z7" s="38" t="s">
+      <c r="Z7" s="37" t="s">
         <v>158</v>
       </c>
-      <c r="AA7" s="52"/>
-      <c r="AB7" s="54" t="s">
+      <c r="AA7" s="51"/>
+      <c r="AB7" s="53" t="s">
         <v>167</v>
       </c>
-      <c r="AC7" s="38" t="s">
+      <c r="AC7" s="37" t="s">
         <v>168</v>
       </c>
-      <c r="AD7" s="38"/>
-      <c r="AE7" s="57" t="s">
+      <c r="AD7" s="37"/>
+      <c r="AE7" s="56" t="s">
         <v>83</v>
       </c>
-      <c r="AF7" s="57" t="s">
+      <c r="AF7" s="56" t="s">
         <v>84</v>
       </c>
-      <c r="AG7" s="43"/>
-      <c r="AH7" s="45" t="s">
+      <c r="AG7" s="42"/>
+      <c r="AH7" s="44" t="s">
         <v>86</v>
       </c>
-      <c r="AI7" s="63" t="s">
+      <c r="AI7" s="62" t="s">
         <v>87</v>
       </c>
-      <c r="AJ7" s="52"/>
-      <c r="AK7" s="57" t="s">
+      <c r="AJ7" s="51"/>
+      <c r="AK7" s="56" t="s">
         <v>83</v>
       </c>
-      <c r="AL7" s="57" t="s">
+      <c r="AL7" s="56" t="s">
         <v>84</v>
       </c>
-      <c r="AM7" s="52"/>
-      <c r="AN7" s="63" t="s">
+      <c r="AM7" s="51"/>
+      <c r="AN7" s="62" t="s">
         <v>100</v>
       </c>
-      <c r="AO7" s="63" t="s">
+      <c r="AO7" s="62" t="s">
         <v>101</v>
       </c>
-      <c r="AP7" s="43"/>
-      <c r="AQ7" s="45"/>
-      <c r="AR7" s="38"/>
-      <c r="AS7" s="52"/>
-      <c r="AT7" s="51" t="s">
+      <c r="AP7" s="42"/>
+      <c r="AQ7" s="44"/>
+      <c r="AR7" s="37"/>
+      <c r="AS7" s="51"/>
+      <c r="AT7" s="50" t="s">
         <v>252</v>
       </c>
-      <c r="AU7" s="38" t="s">
+      <c r="AU7" s="37" t="s">
         <v>254</v>
       </c>
-      <c r="AV7" s="52"/>
-      <c r="AW7" s="37" t="s">
+      <c r="AV7" s="51"/>
+      <c r="AW7" s="36" t="s">
         <v>266</v>
       </c>
-      <c r="AX7" s="37" t="s">
+      <c r="AX7" s="36" t="s">
         <v>195</v>
       </c>
-      <c r="AY7" s="43"/>
-      <c r="AZ7" s="35"/>
-      <c r="BA7" s="36"/>
-      <c r="BB7" s="55"/>
-      <c r="BC7" s="36"/>
-      <c r="BD7" s="36"/>
-      <c r="BE7" s="46"/>
-      <c r="BF7" s="48"/>
-      <c r="BG7" s="36"/>
-      <c r="BH7" s="55"/>
-      <c r="BI7" s="36"/>
-      <c r="BJ7" s="36"/>
-      <c r="BK7" s="46"/>
-      <c r="BL7" s="37" t="s">
+      <c r="AY7" s="42"/>
+      <c r="BE7" s="45"/>
+      <c r="BF7" s="47"/>
+      <c r="BG7" s="35"/>
+      <c r="BH7" s="54"/>
+      <c r="BI7" s="35"/>
+      <c r="BJ7" s="35"/>
+      <c r="BK7" s="45"/>
+      <c r="BL7" s="36" t="s">
         <v>226</v>
       </c>
-      <c r="BM7" s="37" t="s">
+      <c r="BM7" s="36" t="s">
         <v>227</v>
       </c>
-      <c r="BN7" s="39"/>
+      <c r="BN7" s="38"/>
     </row>
     <row r="8" spans="1:72" ht="35.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="1"/>
@@ -2589,20 +2644,20 @@
       <c r="C8" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D8" s="92" t="s">
+      <c r="D8" s="72" t="s">
         <v>90</v>
       </c>
-      <c r="E8" s="93"/>
-      <c r="F8" s="93"/>
-      <c r="G8" s="93"/>
-      <c r="H8" s="93"/>
-      <c r="I8" s="93"/>
-      <c r="J8" s="93"/>
-      <c r="K8" s="93"/>
-      <c r="L8" s="93"/>
-      <c r="M8" s="93"/>
-      <c r="N8" s="93"/>
-      <c r="O8" s="94"/>
+      <c r="E8" s="73"/>
+      <c r="F8" s="73"/>
+      <c r="G8" s="73"/>
+      <c r="H8" s="73"/>
+      <c r="I8" s="73"/>
+      <c r="J8" s="73"/>
+      <c r="K8" s="73"/>
+      <c r="L8" s="73"/>
+      <c r="M8" s="73"/>
+      <c r="N8" s="73"/>
+      <c r="O8" s="74"/>
       <c r="P8" s="7" t="s">
         <v>120</v>
       </c>
@@ -2627,42 +2682,42 @@
       <c r="Y8" s="20" t="s">
         <v>157</v>
       </c>
-      <c r="Z8" s="65" t="s">
+      <c r="Z8" s="64" t="s">
         <v>158</v>
       </c>
       <c r="AA8" s="23"/>
       <c r="AB8" s="24" t="s">
         <v>167</v>
       </c>
-      <c r="AC8" s="65" t="s">
+      <c r="AC8" s="64" t="s">
         <v>168</v>
       </c>
-      <c r="AD8" s="57"/>
-      <c r="AE8" s="57" t="s">
+      <c r="AD8" s="56"/>
+      <c r="AE8" s="56" t="s">
         <v>83</v>
       </c>
-      <c r="AF8" s="57" t="s">
+      <c r="AF8" s="56" t="s">
         <v>84</v>
       </c>
       <c r="AG8" s="22"/>
       <c r="AH8" s="20" t="s">
         <v>86</v>
       </c>
-      <c r="AI8" s="63" t="s">
+      <c r="AI8" s="62" t="s">
         <v>87</v>
       </c>
       <c r="AJ8" s="23"/>
-      <c r="AK8" s="57" t="s">
+      <c r="AK8" s="56" t="s">
         <v>83</v>
       </c>
-      <c r="AL8" s="57" t="s">
+      <c r="AL8" s="56" t="s">
         <v>84</v>
       </c>
       <c r="AM8" s="23"/>
-      <c r="AN8" s="63" t="s">
+      <c r="AN8" s="62" t="s">
         <v>102</v>
       </c>
-      <c r="AO8" s="63" t="s">
+      <c r="AO8" s="62" t="s">
         <v>101</v>
       </c>
       <c r="AP8" s="22"/>
@@ -2683,15 +2738,19 @@
         <v>195</v>
       </c>
       <c r="AY8" s="22"/>
-      <c r="AZ8" s="28"/>
-      <c r="BA8" s="29"/>
-      <c r="BB8" s="56"/>
-      <c r="BC8" s="29"/>
-      <c r="BD8" s="29"/>
+      <c r="AZ8" s="99" t="s">
+        <v>272</v>
+      </c>
+      <c r="BA8" s="87"/>
+      <c r="BB8" s="87"/>
+      <c r="BC8" s="87"/>
+      <c r="BD8" s="71" t="s">
+        <v>211</v>
+      </c>
       <c r="BE8" s="30"/>
       <c r="BF8" s="31"/>
       <c r="BG8" s="29"/>
-      <c r="BH8" s="56"/>
+      <c r="BH8" s="55"/>
       <c r="BI8" s="29"/>
       <c r="BJ8" s="29"/>
       <c r="BK8" s="30"/>
@@ -2711,14 +2770,14 @@
       <c r="C9" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="D9" s="74" t="s">
+      <c r="D9" s="96" t="s">
         <v>108</v>
       </c>
-      <c r="E9" s="75"/>
-      <c r="F9" s="75"/>
-      <c r="G9" s="75"/>
-      <c r="H9" s="75"/>
-      <c r="I9" s="76"/>
+      <c r="E9" s="89"/>
+      <c r="F9" s="89"/>
+      <c r="G9" s="89"/>
+      <c r="H9" s="89"/>
+      <c r="I9" s="97"/>
       <c r="J9" s="24"/>
       <c r="K9" s="21"/>
       <c r="L9" s="23"/>
@@ -2729,38 +2788,38 @@
         <v>104</v>
       </c>
       <c r="O9" s="22"/>
-      <c r="P9" s="92" t="s">
+      <c r="P9" s="72" t="s">
         <v>90</v>
       </c>
-      <c r="Q9" s="93"/>
-      <c r="R9" s="93"/>
-      <c r="S9" s="93"/>
-      <c r="T9" s="93"/>
-      <c r="U9" s="93"/>
-      <c r="V9" s="93"/>
-      <c r="W9" s="93"/>
-      <c r="X9" s="93"/>
-      <c r="Y9" s="36"/>
-      <c r="Z9" s="36"/>
-      <c r="AA9" s="64"/>
+      <c r="Q9" s="73"/>
+      <c r="R9" s="73"/>
+      <c r="S9" s="73"/>
+      <c r="T9" s="73"/>
+      <c r="U9" s="73"/>
+      <c r="V9" s="73"/>
+      <c r="W9" s="73"/>
+      <c r="X9" s="73"/>
+      <c r="Y9" s="35"/>
+      <c r="Z9" s="35"/>
+      <c r="AA9" s="63"/>
       <c r="AB9" s="24" t="s">
         <v>169</v>
       </c>
       <c r="AC9" s="21" t="s">
         <v>142</v>
       </c>
-      <c r="AD9" s="57"/>
-      <c r="AE9" s="57" t="s">
+      <c r="AD9" s="56"/>
+      <c r="AE9" s="56" t="s">
         <v>100</v>
       </c>
-      <c r="AF9" s="57" t="s">
+      <c r="AF9" s="56" t="s">
         <v>101</v>
       </c>
       <c r="AG9" s="22"/>
       <c r="AH9" s="20" t="s">
         <v>86</v>
       </c>
-      <c r="AI9" s="63" t="s">
+      <c r="AI9" s="62" t="s">
         <v>87</v>
       </c>
       <c r="AJ9" s="23"/>
@@ -2791,15 +2850,19 @@
       <c r="AW9" s="21"/>
       <c r="AX9" s="21"/>
       <c r="AY9" s="22"/>
-      <c r="AZ9" s="28"/>
-      <c r="BA9" s="29"/>
-      <c r="BB9" s="56"/>
-      <c r="BC9" s="29"/>
-      <c r="BD9" s="29"/>
+      <c r="AZ9" s="99" t="s">
+        <v>272</v>
+      </c>
+      <c r="BA9" s="87"/>
+      <c r="BB9" s="87"/>
+      <c r="BC9" s="87"/>
+      <c r="BD9" s="71" t="s">
+        <v>211</v>
+      </c>
       <c r="BE9" s="30"/>
       <c r="BF9" s="31"/>
       <c r="BG9" s="29"/>
-      <c r="BH9" s="56"/>
+      <c r="BH9" s="55"/>
       <c r="BI9" s="29"/>
       <c r="BJ9" s="29"/>
       <c r="BK9" s="30"/>
@@ -2815,14 +2878,14 @@
       <c r="C10" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="D10" s="74" t="s">
+      <c r="D10" s="96" t="s">
         <v>108</v>
       </c>
-      <c r="E10" s="75"/>
-      <c r="F10" s="75"/>
-      <c r="G10" s="75"/>
-      <c r="H10" s="75"/>
-      <c r="I10" s="76"/>
+      <c r="E10" s="89"/>
+      <c r="F10" s="89"/>
+      <c r="G10" s="89"/>
+      <c r="H10" s="89"/>
+      <c r="I10" s="97"/>
       <c r="J10" s="31"/>
       <c r="K10" s="29"/>
       <c r="L10" s="30"/>
@@ -2841,23 +2904,23 @@
       <c r="U10" s="23"/>
       <c r="X10" s="22"/>
       <c r="Y10" s="7"/>
-      <c r="Z10" s="36"/>
+      <c r="Z10" s="35"/>
       <c r="AA10" s="23"/>
       <c r="AB10" s="24" t="s">
         <v>169</v>
       </c>
-      <c r="AC10" s="67" t="s">
+      <c r="AC10" s="66" t="s">
         <v>142</v>
       </c>
-      <c r="AD10" s="57"/>
-      <c r="AE10" s="57" t="s">
+      <c r="AD10" s="56"/>
+      <c r="AE10" s="56" t="s">
         <v>102</v>
       </c>
-      <c r="AF10" s="57" t="s">
+      <c r="AF10" s="56" t="s">
         <v>101</v>
       </c>
       <c r="AG10" s="22"/>
-      <c r="AH10" s="69" t="s">
+      <c r="AH10" s="68" t="s">
         <v>210</v>
       </c>
       <c r="AI10" s="21" t="s">
@@ -2867,7 +2930,7 @@
       <c r="AK10" s="24" t="s">
         <v>200</v>
       </c>
-      <c r="AL10" s="67" t="s">
+      <c r="AL10" s="66" t="s">
         <v>201</v>
       </c>
       <c r="AM10" s="23"/>
@@ -2893,13 +2956,13 @@
       <c r="AY10" s="22"/>
       <c r="AZ10" s="28"/>
       <c r="BA10" s="29"/>
-      <c r="BB10" s="56"/>
+      <c r="BB10" s="55"/>
       <c r="BC10" s="29"/>
       <c r="BD10" s="29"/>
       <c r="BE10" s="30"/>
       <c r="BF10" s="31"/>
       <c r="BG10" s="29"/>
-      <c r="BH10" s="56"/>
+      <c r="BH10" s="55"/>
       <c r="BI10" s="29"/>
       <c r="BJ10" s="29"/>
       <c r="BK10" s="30"/>
@@ -2978,20 +3041,20 @@
       <c r="C12" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="D12" s="71" t="s">
+      <c r="D12" s="75" t="s">
         <v>65</v>
       </c>
-      <c r="E12" s="72"/>
-      <c r="F12" s="72"/>
-      <c r="G12" s="72"/>
-      <c r="H12" s="72"/>
-      <c r="I12" s="72"/>
-      <c r="J12" s="72"/>
-      <c r="K12" s="72"/>
-      <c r="L12" s="72"/>
-      <c r="M12" s="72"/>
-      <c r="N12" s="72"/>
-      <c r="O12" s="89"/>
+      <c r="E12" s="76"/>
+      <c r="F12" s="76"/>
+      <c r="G12" s="76"/>
+      <c r="H12" s="76"/>
+      <c r="I12" s="76"/>
+      <c r="J12" s="76"/>
+      <c r="K12" s="76"/>
+      <c r="L12" s="76"/>
+      <c r="M12" s="76"/>
+      <c r="N12" s="76"/>
+      <c r="O12" s="77"/>
       <c r="P12" s="7" t="s">
         <v>120</v>
       </c>
@@ -3025,10 +3088,10 @@
         <v>98</v>
       </c>
       <c r="AD12" s="6"/>
-      <c r="AE12" s="57" t="s">
+      <c r="AE12" s="56" t="s">
         <v>85</v>
       </c>
-      <c r="AF12" s="57" t="s">
+      <c r="AF12" s="56" t="s">
         <v>84</v>
       </c>
       <c r="AG12" s="9"/>
@@ -3039,10 +3102,10 @@
         <v>149</v>
       </c>
       <c r="AJ12" s="8"/>
-      <c r="AK12" s="57" t="s">
+      <c r="AK12" s="56" t="s">
         <v>85</v>
       </c>
-      <c r="AL12" s="57" t="s">
+      <c r="AL12" s="56" t="s">
         <v>84</v>
       </c>
       <c r="AM12" s="8"/>
@@ -3062,15 +3125,15 @@
       <c r="AW12" s="6"/>
       <c r="AX12" s="6"/>
       <c r="AY12" s="9"/>
-      <c r="AZ12" s="7"/>
-      <c r="BA12" s="6"/>
-      <c r="BB12" s="13"/>
-      <c r="BC12" s="6"/>
+      <c r="AZ12" s="75"/>
+      <c r="BA12" s="76"/>
+      <c r="BB12" s="76"/>
+      <c r="BC12" s="76"/>
       <c r="BD12" s="6"/>
       <c r="BE12" s="8"/>
       <c r="BF12" s="31"/>
       <c r="BG12" s="29"/>
-      <c r="BH12" s="56"/>
+      <c r="BH12" s="55"/>
       <c r="BI12" s="29"/>
       <c r="BJ12" s="29"/>
       <c r="BK12" s="30"/>
@@ -3086,20 +3149,20 @@
       <c r="C13" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D13" s="71" t="s">
+      <c r="D13" s="75" t="s">
         <v>65</v>
       </c>
-      <c r="E13" s="72"/>
-      <c r="F13" s="72"/>
-      <c r="G13" s="72"/>
-      <c r="H13" s="72"/>
-      <c r="I13" s="72"/>
-      <c r="J13" s="72"/>
-      <c r="K13" s="72"/>
-      <c r="L13" s="72"/>
-      <c r="M13" s="72"/>
-      <c r="N13" s="72"/>
-      <c r="O13" s="89"/>
+      <c r="E13" s="76"/>
+      <c r="F13" s="76"/>
+      <c r="G13" s="76"/>
+      <c r="H13" s="76"/>
+      <c r="I13" s="76"/>
+      <c r="J13" s="76"/>
+      <c r="K13" s="76"/>
+      <c r="L13" s="76"/>
+      <c r="M13" s="76"/>
+      <c r="N13" s="76"/>
+      <c r="O13" s="77"/>
       <c r="P13" s="7" t="s">
         <v>120</v>
       </c>
@@ -3154,7 +3217,7 @@
       <c r="AK13" s="24" t="s">
         <v>202</v>
       </c>
-      <c r="AL13" s="67" t="s">
+      <c r="AL13" s="66" t="s">
         <v>201</v>
       </c>
       <c r="AM13" s="8"/>
@@ -3178,15 +3241,15 @@
       <c r="AW13" s="6"/>
       <c r="AX13" s="6"/>
       <c r="AY13" s="9"/>
-      <c r="AZ13" s="7"/>
-      <c r="BA13" s="6"/>
-      <c r="BB13" s="13"/>
-      <c r="BC13" s="6"/>
+      <c r="AZ13" s="75"/>
+      <c r="BA13" s="76"/>
+      <c r="BB13" s="76"/>
+      <c r="BC13" s="76"/>
       <c r="BD13" s="6"/>
       <c r="BE13" s="8"/>
       <c r="BF13" s="31"/>
       <c r="BG13" s="29"/>
-      <c r="BH13" s="56"/>
+      <c r="BH13" s="55"/>
       <c r="BI13" s="29"/>
       <c r="BJ13" s="29"/>
       <c r="BK13" s="30"/>
@@ -3202,14 +3265,14 @@
       <c r="C14" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="D14" s="74" t="s">
+      <c r="D14" s="96" t="s">
         <v>108</v>
       </c>
-      <c r="E14" s="75"/>
-      <c r="F14" s="75"/>
-      <c r="G14" s="75"/>
-      <c r="H14" s="75"/>
-      <c r="I14" s="76"/>
+      <c r="E14" s="89"/>
+      <c r="F14" s="89"/>
+      <c r="G14" s="89"/>
+      <c r="H14" s="89"/>
+      <c r="I14" s="97"/>
       <c r="J14" s="10"/>
       <c r="K14" s="6"/>
       <c r="L14" s="8"/>
@@ -3288,11 +3351,11 @@
       <c r="AW14" s="6"/>
       <c r="AX14" s="6"/>
       <c r="AY14" s="9"/>
-      <c r="AZ14" s="28"/>
-      <c r="BA14" s="29"/>
-      <c r="BB14" s="56"/>
-      <c r="BC14" s="29"/>
-      <c r="BD14" s="29"/>
+      <c r="AZ14" s="75"/>
+      <c r="BA14" s="76"/>
+      <c r="BB14" s="76"/>
+      <c r="BC14" s="76"/>
+      <c r="BD14" s="6"/>
       <c r="BE14" s="30"/>
       <c r="BF14" s="10"/>
       <c r="BG14" s="6"/>
@@ -3312,14 +3375,14 @@
       <c r="C15" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="D15" s="74" t="s">
+      <c r="D15" s="96" t="s">
         <v>108</v>
       </c>
-      <c r="E15" s="75"/>
-      <c r="F15" s="75"/>
-      <c r="G15" s="75"/>
-      <c r="H15" s="75"/>
-      <c r="I15" s="76"/>
+      <c r="E15" s="89"/>
+      <c r="F15" s="89"/>
+      <c r="G15" s="89"/>
+      <c r="H15" s="89"/>
+      <c r="I15" s="97"/>
       <c r="J15" s="10"/>
       <c r="K15" s="6"/>
       <c r="L15" s="8"/>
@@ -3388,7 +3451,7 @@
       <c r="AY15" s="9"/>
       <c r="AZ15" s="28"/>
       <c r="BA15" s="29"/>
-      <c r="BB15" s="56"/>
+      <c r="BB15" s="55"/>
       <c r="BC15" s="29"/>
       <c r="BD15" s="29"/>
       <c r="BE15" s="30"/>
@@ -3483,14 +3546,14 @@
       <c r="C17" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="D17" s="71" t="s">
+      <c r="D17" s="75" t="s">
         <v>94</v>
       </c>
-      <c r="E17" s="72"/>
-      <c r="F17" s="72"/>
-      <c r="G17" s="72"/>
-      <c r="H17" s="72"/>
-      <c r="I17" s="73"/>
+      <c r="E17" s="76"/>
+      <c r="F17" s="76"/>
+      <c r="G17" s="76"/>
+      <c r="H17" s="76"/>
+      <c r="I17" s="95"/>
       <c r="J17" s="10"/>
       <c r="K17" s="6"/>
       <c r="L17" s="8"/>
@@ -3583,14 +3646,14 @@
       <c r="C18" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="D18" s="71" t="s">
+      <c r="D18" s="75" t="s">
         <v>95</v>
       </c>
-      <c r="E18" s="72"/>
-      <c r="F18" s="72"/>
-      <c r="G18" s="72"/>
-      <c r="H18" s="72"/>
-      <c r="I18" s="73"/>
+      <c r="E18" s="76"/>
+      <c r="F18" s="76"/>
+      <c r="G18" s="76"/>
+      <c r="H18" s="76"/>
+      <c r="I18" s="95"/>
       <c r="J18" s="10" t="s">
         <v>73</v>
       </c>
@@ -3607,17 +3670,17 @@
       <c r="O18" s="9" t="s">
         <v>59</v>
       </c>
-      <c r="P18" s="71" t="s">
+      <c r="P18" s="75" t="s">
         <v>72</v>
       </c>
-      <c r="Q18" s="72"/>
-      <c r="R18" s="72"/>
-      <c r="S18" s="72"/>
-      <c r="T18" s="72"/>
-      <c r="U18" s="72"/>
-      <c r="V18" s="72"/>
-      <c r="W18" s="72"/>
-      <c r="X18" s="89"/>
+      <c r="Q18" s="76"/>
+      <c r="R18" s="76"/>
+      <c r="S18" s="76"/>
+      <c r="T18" s="76"/>
+      <c r="U18" s="76"/>
+      <c r="V18" s="76"/>
+      <c r="W18" s="76"/>
+      <c r="X18" s="77"/>
       <c r="Y18" s="3" t="s">
         <v>151</v>
       </c>
@@ -3675,11 +3738,15 @@
         <v>140</v>
       </c>
       <c r="AY18" s="9"/>
-      <c r="AZ18" s="7"/>
-      <c r="BA18" s="6"/>
-      <c r="BB18" s="13"/>
-      <c r="BC18" s="6"/>
-      <c r="BD18" s="6"/>
+      <c r="AZ18" s="75" t="s">
+        <v>267</v>
+      </c>
+      <c r="BA18" s="76"/>
+      <c r="BB18" s="76"/>
+      <c r="BC18" s="76"/>
+      <c r="BD18" s="6" t="s">
+        <v>149</v>
+      </c>
       <c r="BE18" s="8"/>
       <c r="BF18" s="10"/>
       <c r="BG18" s="6"/>
@@ -3723,17 +3790,17 @@
         <v>104</v>
       </c>
       <c r="O19" s="9"/>
-      <c r="P19" s="71" t="s">
+      <c r="P19" s="75" t="s">
         <v>72</v>
       </c>
-      <c r="Q19" s="72"/>
-      <c r="R19" s="72"/>
-      <c r="S19" s="72"/>
-      <c r="T19" s="72"/>
-      <c r="U19" s="72"/>
-      <c r="V19" s="72"/>
-      <c r="W19" s="72"/>
-      <c r="X19" s="89"/>
+      <c r="Q19" s="76"/>
+      <c r="R19" s="76"/>
+      <c r="S19" s="76"/>
+      <c r="T19" s="76"/>
+      <c r="U19" s="76"/>
+      <c r="V19" s="76"/>
+      <c r="W19" s="76"/>
+      <c r="X19" s="77"/>
       <c r="Y19" s="3" t="s">
         <v>151</v>
       </c>
@@ -3963,20 +4030,20 @@
       <c r="C22" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="D22" s="71" t="s">
+      <c r="D22" s="75" t="s">
         <v>66</v>
       </c>
-      <c r="E22" s="72"/>
-      <c r="F22" s="72"/>
-      <c r="G22" s="72"/>
-      <c r="H22" s="72"/>
-      <c r="I22" s="72"/>
-      <c r="J22" s="72"/>
-      <c r="K22" s="72"/>
-      <c r="L22" s="72"/>
-      <c r="M22" s="72"/>
-      <c r="N22" s="72"/>
-      <c r="O22" s="89"/>
+      <c r="E22" s="76"/>
+      <c r="F22" s="76"/>
+      <c r="G22" s="76"/>
+      <c r="H22" s="76"/>
+      <c r="I22" s="76"/>
+      <c r="J22" s="76"/>
+      <c r="K22" s="76"/>
+      <c r="L22" s="76"/>
+      <c r="M22" s="76"/>
+      <c r="N22" s="76"/>
+      <c r="O22" s="77"/>
       <c r="P22" s="7" t="s">
         <v>126</v>
       </c>
@@ -4047,20 +4114,20 @@
       <c r="C23" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="D23" s="71" t="s">
+      <c r="D23" s="75" t="s">
         <v>70</v>
       </c>
-      <c r="E23" s="72"/>
-      <c r="F23" s="72"/>
-      <c r="G23" s="72"/>
-      <c r="H23" s="72"/>
-      <c r="I23" s="72"/>
-      <c r="J23" s="72"/>
-      <c r="K23" s="72"/>
-      <c r="L23" s="72"/>
-      <c r="M23" s="72"/>
-      <c r="N23" s="72"/>
-      <c r="O23" s="89"/>
+      <c r="E23" s="76"/>
+      <c r="F23" s="76"/>
+      <c r="G23" s="76"/>
+      <c r="H23" s="76"/>
+      <c r="I23" s="76"/>
+      <c r="J23" s="76"/>
+      <c r="K23" s="76"/>
+      <c r="L23" s="76"/>
+      <c r="M23" s="76"/>
+      <c r="N23" s="76"/>
+      <c r="O23" s="77"/>
       <c r="P23" s="7" t="s">
         <v>126</v>
       </c>
@@ -4134,11 +4201,15 @@
         <v>195</v>
       </c>
       <c r="AY23" s="9"/>
-      <c r="AZ23" s="7"/>
-      <c r="BA23" s="6"/>
-      <c r="BB23" s="13"/>
-      <c r="BC23" s="6"/>
-      <c r="BD23" s="6"/>
+      <c r="AZ23" s="101" t="s">
+        <v>269</v>
+      </c>
+      <c r="BA23" s="102"/>
+      <c r="BB23" s="102"/>
+      <c r="BC23" s="102"/>
+      <c r="BD23" s="103" t="s">
+        <v>78</v>
+      </c>
       <c r="BE23" s="8"/>
       <c r="BF23" s="10"/>
       <c r="BG23" s="6"/>
@@ -4158,14 +4229,14 @@
       <c r="C24" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="D24" s="77" t="s">
+      <c r="D24" s="87" t="s">
         <v>109</v>
       </c>
-      <c r="E24" s="77"/>
-      <c r="F24" s="77"/>
-      <c r="G24" s="77"/>
-      <c r="H24" s="77"/>
-      <c r="I24" s="78"/>
+      <c r="E24" s="87"/>
+      <c r="F24" s="87"/>
+      <c r="G24" s="87"/>
+      <c r="H24" s="87"/>
+      <c r="I24" s="98"/>
       <c r="J24" s="10" t="s">
         <v>73</v>
       </c>
@@ -4270,14 +4341,14 @@
       <c r="C25" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="D25" s="77" t="s">
+      <c r="D25" s="87" t="s">
         <v>109</v>
       </c>
-      <c r="E25" s="77"/>
-      <c r="F25" s="77"/>
-      <c r="G25" s="77"/>
-      <c r="H25" s="77"/>
-      <c r="I25" s="78"/>
+      <c r="E25" s="87"/>
+      <c r="F25" s="87"/>
+      <c r="G25" s="87"/>
+      <c r="H25" s="87"/>
+      <c r="I25" s="98"/>
       <c r="J25" s="10"/>
       <c r="K25" s="6"/>
       <c r="L25" s="8"/>
@@ -4620,11 +4691,15 @@
         <v>140</v>
       </c>
       <c r="AY28" s="9"/>
-      <c r="AZ28" s="7"/>
-      <c r="BA28" s="6"/>
-      <c r="BB28" s="13"/>
-      <c r="BC28" s="6"/>
-      <c r="BD28" s="6"/>
+      <c r="AZ28" s="99" t="s">
+        <v>272</v>
+      </c>
+      <c r="BA28" s="87"/>
+      <c r="BB28" s="87"/>
+      <c r="BC28" s="87"/>
+      <c r="BD28" s="71" t="s">
+        <v>211</v>
+      </c>
       <c r="BE28" s="8"/>
       <c r="BF28" s="10"/>
       <c r="BG28" s="6"/>
@@ -4712,10 +4787,10 @@
         <v>145</v>
       </c>
       <c r="AG29" s="9"/>
-      <c r="AH29" s="69" t="s">
+      <c r="AH29" s="68" t="s">
         <v>212</v>
       </c>
-      <c r="AI29" s="67" t="s">
+      <c r="AI29" s="66" t="s">
         <v>211</v>
       </c>
       <c r="AJ29" s="8"/>
@@ -4792,10 +4867,10 @@
       <c r="S30" s="10"/>
       <c r="T30" s="6"/>
       <c r="U30" s="6"/>
-      <c r="V30" s="70" t="s">
+      <c r="V30" s="69" t="s">
         <v>139</v>
       </c>
-      <c r="W30" s="70" t="s">
+      <c r="W30" s="69" t="s">
         <v>140</v>
       </c>
       <c r="X30" s="9"/>
@@ -4849,19 +4924,19 @@
       <c r="BN30" s="9"/>
     </row>
     <row r="31" spans="1:66" ht="27" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C31" s="58" t="s">
+      <c r="C31" s="57" t="s">
         <v>64</v>
       </c>
-      <c r="D31" s="59" t="s">
+      <c r="D31" s="58" t="s">
         <v>62</v>
       </c>
-      <c r="E31" s="60" t="s">
+      <c r="E31" s="59" t="s">
         <v>63</v>
       </c>
-      <c r="F31" s="61" t="s">
+      <c r="F31" s="60" t="s">
         <v>59</v>
       </c>
-      <c r="G31" s="49"/>
+      <c r="G31" s="48"/>
       <c r="H31" s="33"/>
       <c r="I31" s="34"/>
       <c r="J31" s="10"/>
@@ -4951,7 +5026,7 @@
       </c>
       <c r="L32" s="8"/>
       <c r="O32" s="9"/>
-      <c r="Q32" s="62"/>
+      <c r="Q32" s="61"/>
       <c r="Y32" s="7"/>
       <c r="Z32" s="6"/>
       <c r="AA32" s="8"/>
@@ -5024,17 +5099,17 @@
         <v>78</v>
       </c>
       <c r="O33" s="9"/>
-      <c r="P33" s="71" t="s">
+      <c r="P33" s="75" t="s">
         <v>71</v>
       </c>
-      <c r="Q33" s="72"/>
-      <c r="R33" s="72"/>
-      <c r="S33" s="72"/>
-      <c r="T33" s="72"/>
-      <c r="U33" s="72"/>
-      <c r="V33" s="72"/>
-      <c r="W33" s="72"/>
-      <c r="X33" s="89"/>
+      <c r="Q33" s="76"/>
+      <c r="R33" s="76"/>
+      <c r="S33" s="76"/>
+      <c r="T33" s="76"/>
+      <c r="U33" s="76"/>
+      <c r="V33" s="76"/>
+      <c r="W33" s="76"/>
+      <c r="X33" s="77"/>
       <c r="Y33" s="20" t="s">
         <v>81</v>
       </c>
@@ -5094,17 +5169,25 @@
         <v>145</v>
       </c>
       <c r="AY33" s="9"/>
-      <c r="AZ33" s="7"/>
-      <c r="BA33" s="6"/>
-      <c r="BB33" s="13"/>
-      <c r="BC33" s="6"/>
-      <c r="BD33" s="6"/>
+      <c r="AZ33" s="75" t="s">
+        <v>270</v>
+      </c>
+      <c r="BA33" s="76"/>
+      <c r="BB33" s="76"/>
+      <c r="BC33" s="76"/>
+      <c r="BD33" s="6" t="s">
+        <v>209</v>
+      </c>
       <c r="BE33" s="8"/>
-      <c r="BF33" s="10"/>
-      <c r="BG33" s="6"/>
-      <c r="BH33" s="13"/>
-      <c r="BI33" s="6"/>
-      <c r="BJ33" s="6"/>
+      <c r="BF33" s="100" t="s">
+        <v>276</v>
+      </c>
+      <c r="BG33" s="76"/>
+      <c r="BH33" s="76"/>
+      <c r="BI33" s="76"/>
+      <c r="BJ33" s="6" t="s">
+        <v>278</v>
+      </c>
       <c r="BK33" s="8"/>
       <c r="BL33" s="6"/>
       <c r="BM33" s="6"/>
@@ -5206,17 +5289,25 @@
         <v>145</v>
       </c>
       <c r="AY34" s="9"/>
-      <c r="AZ34" s="7"/>
-      <c r="BA34" s="6"/>
-      <c r="BB34" s="13"/>
-      <c r="BC34" s="6"/>
-      <c r="BD34" s="6"/>
+      <c r="AZ34" s="75" t="s">
+        <v>270</v>
+      </c>
+      <c r="BA34" s="76"/>
+      <c r="BB34" s="76"/>
+      <c r="BC34" s="76"/>
+      <c r="BD34" s="6" t="s">
+        <v>209</v>
+      </c>
       <c r="BE34" s="8"/>
-      <c r="BF34" s="10"/>
-      <c r="BG34" s="6"/>
-      <c r="BH34" s="13"/>
-      <c r="BI34" s="6"/>
-      <c r="BJ34" s="6"/>
+      <c r="BF34" s="100" t="s">
+        <v>277</v>
+      </c>
+      <c r="BG34" s="76"/>
+      <c r="BH34" s="76"/>
+      <c r="BI34" s="76"/>
+      <c r="BJ34" s="6" t="s">
+        <v>278</v>
+      </c>
       <c r="BK34" s="8"/>
       <c r="BL34" s="6"/>
       <c r="BM34" s="6"/>
@@ -5388,20 +5479,20 @@
       <c r="C37" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="D37" s="71" t="s">
+      <c r="D37" s="75" t="s">
         <v>69</v>
       </c>
-      <c r="E37" s="72"/>
-      <c r="F37" s="72"/>
-      <c r="G37" s="72"/>
-      <c r="H37" s="72"/>
-      <c r="I37" s="72"/>
-      <c r="J37" s="72"/>
-      <c r="K37" s="72"/>
-      <c r="L37" s="72"/>
-      <c r="M37" s="72"/>
-      <c r="N37" s="72"/>
-      <c r="O37" s="89"/>
+      <c r="E37" s="76"/>
+      <c r="F37" s="76"/>
+      <c r="G37" s="76"/>
+      <c r="H37" s="76"/>
+      <c r="I37" s="76"/>
+      <c r="J37" s="76"/>
+      <c r="K37" s="76"/>
+      <c r="L37" s="76"/>
+      <c r="M37" s="76"/>
+      <c r="N37" s="76"/>
+      <c r="O37" s="77"/>
       <c r="P37" s="7" t="s">
         <v>125</v>
       </c>
@@ -5474,14 +5565,14 @@
       <c r="C38" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="D38" s="77" t="s">
+      <c r="D38" s="87" t="s">
         <v>109</v>
       </c>
-      <c r="E38" s="77"/>
-      <c r="F38" s="77"/>
-      <c r="G38" s="77"/>
-      <c r="H38" s="77"/>
-      <c r="I38" s="78"/>
+      <c r="E38" s="87"/>
+      <c r="F38" s="87"/>
+      <c r="G38" s="87"/>
+      <c r="H38" s="87"/>
+      <c r="I38" s="98"/>
       <c r="J38" s="10" t="s">
         <v>111</v>
       </c>
@@ -5560,11 +5651,15 @@
         <v>257</v>
       </c>
       <c r="AY38" s="9"/>
-      <c r="AZ38" s="7"/>
-      <c r="BA38" s="6"/>
-      <c r="BB38" s="13"/>
-      <c r="BC38" s="6"/>
-      <c r="BD38" s="6"/>
+      <c r="AZ38" s="75" t="s">
+        <v>267</v>
+      </c>
+      <c r="BA38" s="76"/>
+      <c r="BB38" s="76"/>
+      <c r="BC38" s="76"/>
+      <c r="BD38" s="6" t="s">
+        <v>149</v>
+      </c>
       <c r="BE38" s="8"/>
       <c r="BF38" s="10"/>
       <c r="BG38" s="6"/>
@@ -5584,14 +5679,14 @@
       <c r="C39" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="D39" s="77" t="s">
+      <c r="D39" s="87" t="s">
         <v>110</v>
       </c>
-      <c r="E39" s="77"/>
-      <c r="F39" s="77"/>
-      <c r="G39" s="77"/>
-      <c r="H39" s="77"/>
-      <c r="I39" s="78"/>
+      <c r="E39" s="87"/>
+      <c r="F39" s="87"/>
+      <c r="G39" s="87"/>
+      <c r="H39" s="87"/>
+      <c r="I39" s="98"/>
       <c r="J39" s="10"/>
       <c r="K39" s="6"/>
       <c r="L39" s="8"/>
@@ -5660,11 +5755,15 @@
         <v>257</v>
       </c>
       <c r="AY39" s="9"/>
-      <c r="AZ39" s="7"/>
-      <c r="BA39" s="6"/>
-      <c r="BB39" s="13"/>
-      <c r="BC39" s="6"/>
-      <c r="BD39" s="6"/>
+      <c r="AZ39" s="75" t="s">
+        <v>267</v>
+      </c>
+      <c r="BA39" s="76"/>
+      <c r="BB39" s="76"/>
+      <c r="BC39" s="76"/>
+      <c r="BD39" s="6" t="s">
+        <v>149</v>
+      </c>
       <c r="BE39" s="8"/>
       <c r="BF39" s="10"/>
       <c r="BG39" s="6"/>
@@ -5849,17 +5948,17 @@
         <v>106</v>
       </c>
       <c r="O42" s="32"/>
-      <c r="P42" s="71" t="s">
+      <c r="P42" s="75" t="s">
         <v>91</v>
       </c>
-      <c r="Q42" s="72"/>
-      <c r="R42" s="72"/>
-      <c r="S42" s="72"/>
-      <c r="T42" s="72"/>
-      <c r="U42" s="72"/>
-      <c r="V42" s="72"/>
-      <c r="W42" s="72"/>
-      <c r="X42" s="89"/>
+      <c r="Q42" s="76"/>
+      <c r="R42" s="76"/>
+      <c r="S42" s="76"/>
+      <c r="T42" s="76"/>
+      <c r="U42" s="76"/>
+      <c r="V42" s="76"/>
+      <c r="W42" s="76"/>
+      <c r="X42" s="77"/>
       <c r="Y42" s="7" t="s">
         <v>162</v>
       </c>
@@ -5915,7 +6014,7 @@
       <c r="BE42" s="8"/>
       <c r="BF42" s="31"/>
       <c r="BG42" s="29"/>
-      <c r="BH42" s="56"/>
+      <c r="BH42" s="55"/>
       <c r="BI42" s="29"/>
       <c r="BJ42" s="29"/>
       <c r="BK42" s="30"/>
@@ -5951,10 +6050,10 @@
       </c>
       <c r="R43" s="8"/>
       <c r="U43" s="8"/>
-      <c r="V43" s="38" t="s">
+      <c r="V43" s="37" t="s">
         <v>139</v>
       </c>
-      <c r="W43" s="38" t="s">
+      <c r="W43" s="37" t="s">
         <v>140</v>
       </c>
       <c r="X43" s="9"/>
@@ -6007,7 +6106,7 @@
       <c r="AY43" s="9"/>
       <c r="AZ43" s="28"/>
       <c r="BA43" s="29"/>
-      <c r="BB43" s="56"/>
+      <c r="BB43" s="55"/>
       <c r="BC43" s="29"/>
       <c r="BD43" s="29"/>
       <c r="BE43" s="30"/>
@@ -6099,15 +6198,19 @@
       <c r="AW44" s="6"/>
       <c r="AX44" s="6"/>
       <c r="AY44" s="9"/>
-      <c r="AZ44" s="7"/>
-      <c r="BA44" s="6"/>
-      <c r="BB44" s="13"/>
-      <c r="BC44" s="6"/>
-      <c r="BD44" s="6"/>
+      <c r="AZ44" s="75" t="s">
+        <v>270</v>
+      </c>
+      <c r="BA44" s="76"/>
+      <c r="BB44" s="76"/>
+      <c r="BC44" s="76"/>
+      <c r="BD44" s="6" t="s">
+        <v>209</v>
+      </c>
       <c r="BE44" s="8"/>
       <c r="BF44" s="31"/>
       <c r="BG44" s="29"/>
-      <c r="BH44" s="56"/>
+      <c r="BH44" s="55"/>
       <c r="BI44" s="29"/>
       <c r="BJ44" s="29"/>
       <c r="BK44" s="30"/>
@@ -6183,15 +6286,19 @@
         <v>140</v>
       </c>
       <c r="AY45" s="9"/>
-      <c r="AZ45" s="7"/>
-      <c r="BA45" s="6"/>
-      <c r="BB45" s="13"/>
-      <c r="BC45" s="6"/>
-      <c r="BD45" s="6"/>
+      <c r="AZ45" s="75" t="s">
+        <v>271</v>
+      </c>
+      <c r="BA45" s="76"/>
+      <c r="BB45" s="76"/>
+      <c r="BC45" s="76"/>
+      <c r="BD45" s="6" t="s">
+        <v>209</v>
+      </c>
       <c r="BE45" s="8"/>
       <c r="BF45" s="31"/>
       <c r="BG45" s="29"/>
-      <c r="BH45" s="56"/>
+      <c r="BH45" s="55"/>
       <c r="BI45" s="29"/>
       <c r="BJ45" s="29"/>
       <c r="BK45" s="30"/>
@@ -6274,10 +6381,10 @@
       <c r="C47" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="D47" s="40"/>
+      <c r="D47" s="39"/>
       <c r="E47" s="33"/>
       <c r="F47" s="34"/>
-      <c r="G47" s="49"/>
+      <c r="G47" s="48"/>
       <c r="H47" s="33"/>
       <c r="I47" s="34"/>
       <c r="J47" s="10"/>
@@ -6350,11 +6457,19 @@
       <c r="AW47" s="6"/>
       <c r="AX47" s="6"/>
       <c r="AY47" s="9"/>
-      <c r="AZ47" s="7"/>
-      <c r="BA47" s="6"/>
+      <c r="AZ47" s="7" t="s">
+        <v>274</v>
+      </c>
+      <c r="BA47" s="71" t="s">
+        <v>211</v>
+      </c>
       <c r="BB47" s="13"/>
-      <c r="BC47" s="6"/>
-      <c r="BD47" s="6"/>
+      <c r="BC47" s="6" t="s">
+        <v>279</v>
+      </c>
+      <c r="BD47" s="6" t="s">
+        <v>149</v>
+      </c>
       <c r="BE47" s="8"/>
       <c r="BF47" s="10"/>
       <c r="BG47" s="6"/>
@@ -6374,10 +6489,10 @@
       <c r="C48" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D48" s="40"/>
+      <c r="D48" s="39"/>
       <c r="E48" s="33"/>
       <c r="F48" s="34"/>
-      <c r="G48" s="49"/>
+      <c r="G48" s="48"/>
       <c r="H48" s="33"/>
       <c r="I48" s="34"/>
       <c r="J48" s="10"/>
@@ -6450,11 +6565,19 @@
       <c r="AW48" s="6"/>
       <c r="AX48" s="6"/>
       <c r="AY48" s="9"/>
-      <c r="AZ48" s="28"/>
-      <c r="BA48" s="29"/>
-      <c r="BB48" s="56"/>
-      <c r="BC48" s="29"/>
-      <c r="BD48" s="29"/>
+      <c r="AZ48" s="28" t="s">
+        <v>274</v>
+      </c>
+      <c r="BA48" s="71" t="s">
+        <v>211</v>
+      </c>
+      <c r="BB48" s="55"/>
+      <c r="BC48" s="29" t="s">
+        <v>279</v>
+      </c>
+      <c r="BD48" s="6" t="s">
+        <v>149</v>
+      </c>
       <c r="BE48" s="30"/>
       <c r="BF48" s="10"/>
       <c r="BG48" s="6"/>
@@ -6474,10 +6597,10 @@
       <c r="C49" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="D49" s="40"/>
+      <c r="D49" s="39"/>
       <c r="E49" s="33"/>
       <c r="F49" s="34"/>
-      <c r="G49" s="49"/>
+      <c r="G49" s="48"/>
       <c r="H49" s="33"/>
       <c r="I49" s="34"/>
       <c r="J49" s="10"/>
@@ -6553,11 +6676,15 @@
       <c r="AW49" s="6"/>
       <c r="AX49" s="6"/>
       <c r="AY49" s="9"/>
-      <c r="AZ49" s="7"/>
-      <c r="BA49" s="6"/>
-      <c r="BB49" s="13"/>
-      <c r="BC49" s="6"/>
-      <c r="BD49" s="6"/>
+      <c r="AZ49" s="99" t="s">
+        <v>273</v>
+      </c>
+      <c r="BA49" s="87"/>
+      <c r="BB49" s="87"/>
+      <c r="BC49" s="87"/>
+      <c r="BD49" s="71" t="s">
+        <v>211</v>
+      </c>
       <c r="BE49" s="8"/>
       <c r="BF49" s="10"/>
       <c r="BG49" s="6"/>
@@ -6577,13 +6704,13 @@
       <c r="C50" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="D50" s="41"/>
-      <c r="E50" s="42"/>
-      <c r="F50" s="47"/>
-      <c r="G50" s="50"/>
-      <c r="H50" s="42"/>
-      <c r="I50" s="47"/>
-      <c r="J50" s="53"/>
+      <c r="D50" s="40"/>
+      <c r="E50" s="41"/>
+      <c r="F50" s="46"/>
+      <c r="G50" s="49"/>
+      <c r="H50" s="41"/>
+      <c r="I50" s="46"/>
+      <c r="J50" s="52"/>
       <c r="K50" s="16"/>
       <c r="L50" s="17"/>
       <c r="M50" s="16"/>
@@ -6592,7 +6719,7 @@
       <c r="P50" s="15"/>
       <c r="Q50" s="16"/>
       <c r="R50" s="17"/>
-      <c r="S50" s="53"/>
+      <c r="S50" s="52"/>
       <c r="T50" s="16"/>
       <c r="U50" s="17"/>
       <c r="V50" s="6" t="s">
@@ -6622,7 +6749,7 @@
         <v>147</v>
       </c>
       <c r="AJ50" s="17"/>
-      <c r="AK50" s="53"/>
+      <c r="AK50" s="52"/>
       <c r="AL50" s="16"/>
       <c r="AM50" s="17"/>
       <c r="AN50" s="6" t="s">
@@ -6634,7 +6761,7 @@
       <c r="AQ50" s="15"/>
       <c r="AR50" s="16"/>
       <c r="AS50" s="17"/>
-      <c r="AT50" s="53"/>
+      <c r="AT50" s="52"/>
       <c r="AU50" s="16"/>
       <c r="AV50" s="17"/>
       <c r="AW50" s="16"/>
@@ -6646,7 +6773,7 @@
       <c r="BC50" s="16"/>
       <c r="BD50" s="16"/>
       <c r="BE50" s="17"/>
-      <c r="BF50" s="53"/>
+      <c r="BF50" s="52"/>
       <c r="BG50" s="16"/>
       <c r="BH50" s="19"/>
       <c r="BI50" s="16"/>
@@ -6725,13 +6852,13 @@
       <c r="BN51" s="6"/>
     </row>
     <row r="52" spans="1:66" ht="39.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A52" s="68" t="s">
+      <c r="A52" s="67" t="s">
         <v>152</v>
       </c>
-      <c r="B52" s="68" t="s">
+      <c r="B52" s="67" t="s">
         <v>0</v>
       </c>
-      <c r="C52" s="68" t="s">
+      <c r="C52" s="67" t="s">
         <v>20</v>
       </c>
       <c r="D52" s="6"/>
@@ -6780,39 +6907,39 @@
         <v>257</v>
       </c>
       <c r="AY52" s="6"/>
-      <c r="AZ52" s="72"/>
-      <c r="BA52" s="72"/>
-      <c r="BB52" s="72"/>
-      <c r="BC52" s="72"/>
-      <c r="BD52" s="72"/>
-      <c r="BE52" s="72"/>
-      <c r="BF52" s="72"/>
-      <c r="BG52" s="72"/>
-      <c r="BH52" s="72"/>
-      <c r="BI52" s="72"/>
-      <c r="BJ52" s="72"/>
-      <c r="BK52" s="72"/>
+      <c r="AZ52" s="76"/>
+      <c r="BA52" s="76"/>
+      <c r="BB52" s="76"/>
+      <c r="BC52" s="76"/>
+      <c r="BD52" s="76"/>
+      <c r="BE52" s="76"/>
+      <c r="BF52" s="76"/>
+      <c r="BG52" s="76"/>
+      <c r="BH52" s="76"/>
+      <c r="BI52" s="76"/>
+      <c r="BJ52" s="76"/>
+      <c r="BK52" s="76"/>
       <c r="BL52" s="6"/>
       <c r="BM52" s="6"/>
       <c r="BN52" s="6"/>
     </row>
     <row r="53" spans="1:66" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A53" s="68"/>
-      <c r="B53" s="68" t="s">
+      <c r="A53" s="67"/>
+      <c r="B53" s="67" t="s">
         <v>1</v>
       </c>
-      <c r="C53" s="68" t="s">
+      <c r="C53" s="67" t="s">
         <v>21</v>
       </c>
       <c r="D53" s="6"/>
       <c r="E53" s="6"/>
       <c r="F53" s="6"/>
-      <c r="G53" s="72"/>
-      <c r="H53" s="72"/>
-      <c r="I53" s="72"/>
-      <c r="J53" s="72"/>
-      <c r="K53" s="72"/>
-      <c r="L53" s="72"/>
+      <c r="G53" s="76"/>
+      <c r="H53" s="76"/>
+      <c r="I53" s="76"/>
+      <c r="J53" s="76"/>
+      <c r="K53" s="76"/>
+      <c r="L53" s="76"/>
       <c r="M53" s="6"/>
       <c r="N53" s="6"/>
       <c r="O53" s="6"/>
@@ -6875,33 +7002,33 @@
       <c r="BC53" s="6"/>
       <c r="BD53" s="6"/>
       <c r="BE53" s="6"/>
-      <c r="BF53" s="72"/>
-      <c r="BG53" s="72"/>
-      <c r="BH53" s="72"/>
-      <c r="BI53" s="72"/>
-      <c r="BJ53" s="72"/>
-      <c r="BK53" s="72"/>
+      <c r="BF53" s="76"/>
+      <c r="BG53" s="76"/>
+      <c r="BH53" s="76"/>
+      <c r="BI53" s="76"/>
+      <c r="BJ53" s="76"/>
+      <c r="BK53" s="76"/>
       <c r="BL53" s="6"/>
       <c r="BM53" s="6"/>
       <c r="BN53" s="6"/>
     </row>
     <row r="54" spans="1:66" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A54" s="68"/>
-      <c r="B54" s="68" t="s">
+      <c r="A54" s="67"/>
+      <c r="B54" s="67" t="s">
         <v>2</v>
       </c>
-      <c r="C54" s="68" t="s">
+      <c r="C54" s="67" t="s">
         <v>22</v>
       </c>
       <c r="D54" s="6"/>
       <c r="E54" s="6"/>
       <c r="F54" s="6"/>
-      <c r="G54" s="72"/>
-      <c r="H54" s="72"/>
-      <c r="I54" s="72"/>
-      <c r="J54" s="72"/>
-      <c r="K54" s="72"/>
-      <c r="L54" s="72"/>
+      <c r="G54" s="76"/>
+      <c r="H54" s="76"/>
+      <c r="I54" s="76"/>
+      <c r="J54" s="76"/>
+      <c r="K54" s="76"/>
+      <c r="L54" s="76"/>
       <c r="M54" s="6"/>
       <c r="N54" s="6"/>
       <c r="O54" s="6"/>
@@ -6963,22 +7090,22 @@
       <c r="BC54" s="6"/>
       <c r="BD54" s="6"/>
       <c r="BE54" s="6"/>
-      <c r="BF54" s="72"/>
-      <c r="BG54" s="72"/>
-      <c r="BH54" s="72"/>
-      <c r="BI54" s="72"/>
-      <c r="BJ54" s="72"/>
-      <c r="BK54" s="72"/>
+      <c r="BF54" s="76"/>
+      <c r="BG54" s="76"/>
+      <c r="BH54" s="76"/>
+      <c r="BI54" s="76"/>
+      <c r="BJ54" s="76"/>
+      <c r="BK54" s="76"/>
       <c r="BL54" s="6"/>
       <c r="BM54" s="6"/>
       <c r="BN54" s="6"/>
     </row>
     <row r="55" spans="1:66" x14ac:dyDescent="0.25">
-      <c r="A55" s="68"/>
-      <c r="B55" s="68" t="s">
+      <c r="A55" s="67"/>
+      <c r="B55" s="67" t="s">
         <v>3</v>
       </c>
-      <c r="C55" s="68" t="s">
+      <c r="C55" s="67" t="s">
         <v>23</v>
       </c>
       <c r="D55" s="6"/>
@@ -7035,29 +7162,29 @@
       <c r="BC55" s="6"/>
       <c r="BD55" s="6"/>
       <c r="BE55" s="6"/>
-      <c r="BF55" s="72"/>
-      <c r="BG55" s="72"/>
-      <c r="BH55" s="72"/>
-      <c r="BI55" s="72"/>
-      <c r="BJ55" s="72"/>
-      <c r="BK55" s="72"/>
+      <c r="BF55" s="76"/>
+      <c r="BG55" s="76"/>
+      <c r="BH55" s="76"/>
+      <c r="BI55" s="76"/>
+      <c r="BJ55" s="76"/>
+      <c r="BK55" s="76"/>
       <c r="BL55" s="6"/>
       <c r="BM55" s="6"/>
       <c r="BN55" s="6"/>
     </row>
     <row r="56" spans="1:66" x14ac:dyDescent="0.25">
-      <c r="C56" s="68" t="s">
+      <c r="C56" s="67" t="s">
         <v>37</v>
       </c>
       <c r="D56" s="6"/>
       <c r="E56" s="6"/>
       <c r="F56" s="6"/>
-      <c r="G56" s="72"/>
-      <c r="H56" s="72"/>
-      <c r="I56" s="72"/>
-      <c r="J56" s="72"/>
-      <c r="K56" s="72"/>
-      <c r="L56" s="72"/>
+      <c r="G56" s="76"/>
+      <c r="H56" s="76"/>
+      <c r="I56" s="76"/>
+      <c r="J56" s="76"/>
+      <c r="K56" s="76"/>
+      <c r="L56" s="76"/>
       <c r="M56" s="6"/>
       <c r="N56" s="6"/>
       <c r="O56" s="6"/>
@@ -7114,24 +7241,24 @@
       <c r="BN56" s="6"/>
     </row>
     <row r="57" spans="1:66" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A57" s="68" t="s">
+      <c r="A57" s="67" t="s">
         <v>153</v>
       </c>
-      <c r="B57" s="68" t="s">
+      <c r="B57" s="67" t="s">
         <v>0</v>
       </c>
-      <c r="C57" s="68" t="s">
+      <c r="C57" s="67" t="s">
         <v>20</v>
       </c>
       <c r="D57" s="6"/>
       <c r="E57" s="6"/>
       <c r="F57" s="6"/>
-      <c r="G57" s="72"/>
-      <c r="H57" s="72"/>
-      <c r="I57" s="72"/>
-      <c r="J57" s="72"/>
-      <c r="K57" s="72"/>
-      <c r="L57" s="72"/>
+      <c r="G57" s="76"/>
+      <c r="H57" s="76"/>
+      <c r="I57" s="76"/>
+      <c r="J57" s="76"/>
+      <c r="K57" s="76"/>
+      <c r="L57" s="76"/>
       <c r="M57" s="6"/>
       <c r="N57" s="6"/>
       <c r="O57" s="6"/>
@@ -7188,19 +7315,19 @@
       <c r="BN57" s="6"/>
     </row>
     <row r="58" spans="1:66" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A58" s="68"/>
-      <c r="B58" s="68" t="s">
+      <c r="A58" s="67"/>
+      <c r="B58" s="67" t="s">
         <v>1</v>
       </c>
-      <c r="C58" s="68" t="s">
+      <c r="C58" s="67" t="s">
         <v>21</v>
       </c>
-      <c r="D58" s="79"/>
-      <c r="E58" s="79"/>
-      <c r="F58" s="79"/>
-      <c r="G58" s="79"/>
-      <c r="H58" s="79"/>
-      <c r="I58" s="79"/>
+      <c r="D58" s="94"/>
+      <c r="E58" s="94"/>
+      <c r="F58" s="94"/>
+      <c r="G58" s="94"/>
+      <c r="H58" s="94"/>
+      <c r="I58" s="94"/>
       <c r="J58" s="6"/>
       <c r="K58" s="6"/>
       <c r="L58" s="6"/>
@@ -7254,12 +7381,13 @@
         <v>80</v>
       </c>
       <c r="AY58" s="6"/>
-      <c r="AZ58" s="72"/>
-      <c r="BA58" s="72"/>
-      <c r="BB58" s="72"/>
-      <c r="BC58" s="72"/>
-      <c r="BD58" s="72"/>
-      <c r="BE58" s="72"/>
+      <c r="BC58" s="3" t="s">
+        <v>280</v>
+      </c>
+      <c r="BD58" s="6" t="s">
+        <v>149</v>
+      </c>
+      <c r="BE58" s="6"/>
       <c r="BF58" s="6"/>
       <c r="BG58" s="6"/>
       <c r="BH58" s="6"/>
@@ -7271,19 +7399,19 @@
       <c r="BN58" s="6"/>
     </row>
     <row r="59" spans="1:66" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A59" s="68"/>
-      <c r="B59" s="68" t="s">
+      <c r="A59" s="67"/>
+      <c r="B59" s="67" t="s">
         <v>2</v>
       </c>
-      <c r="C59" s="68" t="s">
+      <c r="C59" s="67" t="s">
         <v>22</v>
       </c>
-      <c r="D59" s="79"/>
-      <c r="E59" s="79"/>
-      <c r="F59" s="79"/>
-      <c r="G59" s="79"/>
-      <c r="H59" s="79"/>
-      <c r="I59" s="79"/>
+      <c r="D59" s="94"/>
+      <c r="E59" s="94"/>
+      <c r="F59" s="94"/>
+      <c r="G59" s="94"/>
+      <c r="H59" s="94"/>
+      <c r="I59" s="94"/>
       <c r="J59" s="6"/>
       <c r="K59" s="6"/>
       <c r="L59" s="6"/>
@@ -7338,28 +7466,32 @@
       <c r="AW59" s="6"/>
       <c r="AX59" s="6"/>
       <c r="AY59" s="6"/>
-      <c r="AZ59" s="72"/>
-      <c r="BA59" s="72"/>
-      <c r="BB59" s="72"/>
-      <c r="BC59" s="72"/>
-      <c r="BD59" s="72"/>
-      <c r="BE59" s="72"/>
-      <c r="BF59" s="72"/>
-      <c r="BG59" s="72"/>
-      <c r="BH59" s="72"/>
-      <c r="BI59" s="72"/>
-      <c r="BJ59" s="72"/>
-      <c r="BK59" s="72"/>
+      <c r="AZ59" s="76" t="s">
+        <v>268</v>
+      </c>
+      <c r="BA59" s="76"/>
+      <c r="BB59" s="76"/>
+      <c r="BC59" s="76"/>
+      <c r="BD59" s="6" t="s">
+        <v>149</v>
+      </c>
+      <c r="BE59" s="70"/>
+      <c r="BF59" s="76"/>
+      <c r="BG59" s="76"/>
+      <c r="BH59" s="76"/>
+      <c r="BI59" s="76"/>
+      <c r="BJ59" s="76"/>
+      <c r="BK59" s="76"/>
       <c r="BL59" s="6"/>
       <c r="BM59" s="6"/>
       <c r="BN59" s="6"/>
     </row>
     <row r="60" spans="1:66" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A60" s="68"/>
-      <c r="B60" s="68" t="s">
+      <c r="A60" s="67"/>
+      <c r="B60" s="67" t="s">
         <v>3</v>
       </c>
-      <c r="C60" s="68" t="s">
+      <c r="C60" s="67" t="s">
         <v>23</v>
       </c>
       <c r="D60" s="6"/>
@@ -7424,12 +7556,12 @@
       <c r="BC60" s="6"/>
       <c r="BD60" s="6"/>
       <c r="BE60" s="6"/>
-      <c r="BF60" s="72"/>
-      <c r="BG60" s="72"/>
-      <c r="BH60" s="72"/>
-      <c r="BI60" s="72"/>
-      <c r="BJ60" s="72"/>
-      <c r="BK60" s="72"/>
+      <c r="BF60" s="76"/>
+      <c r="BG60" s="76"/>
+      <c r="BH60" s="76"/>
+      <c r="BI60" s="76"/>
+      <c r="BJ60" s="76"/>
+      <c r="BK60" s="76"/>
       <c r="BL60" s="6"/>
       <c r="BM60" s="6"/>
       <c r="BN60" s="6"/>
@@ -7503,24 +7635,24 @@
       <c r="BN61" s="6"/>
     </row>
     <row r="62" spans="1:66" ht="75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A62" s="68" t="s">
+      <c r="A62" s="67" t="s">
         <v>154</v>
       </c>
-      <c r="B62" s="68" t="s">
+      <c r="B62" s="67" t="s">
         <v>0</v>
       </c>
-      <c r="C62" s="68" t="s">
+      <c r="C62" s="67" t="s">
         <v>20</v>
       </c>
       <c r="D62" s="6"/>
       <c r="E62" s="6"/>
       <c r="F62" s="6"/>
-      <c r="G62" s="72"/>
-      <c r="H62" s="72"/>
-      <c r="I62" s="72"/>
-      <c r="J62" s="72"/>
-      <c r="K62" s="72"/>
-      <c r="L62" s="72"/>
+      <c r="G62" s="76"/>
+      <c r="H62" s="76"/>
+      <c r="I62" s="76"/>
+      <c r="J62" s="76"/>
+      <c r="K62" s="76"/>
+      <c r="L62" s="76"/>
       <c r="M62" s="6"/>
       <c r="N62" s="6"/>
       <c r="O62" s="6"/>
@@ -7566,33 +7698,33 @@
       <c r="BC62" s="6"/>
       <c r="BD62" s="6"/>
       <c r="BE62" s="6"/>
-      <c r="BF62" s="72"/>
-      <c r="BG62" s="72"/>
-      <c r="BH62" s="72"/>
-      <c r="BI62" s="72"/>
-      <c r="BJ62" s="72"/>
-      <c r="BK62" s="72"/>
+      <c r="BF62" s="76"/>
+      <c r="BG62" s="76"/>
+      <c r="BH62" s="76"/>
+      <c r="BI62" s="76"/>
+      <c r="BJ62" s="76"/>
+      <c r="BK62" s="76"/>
       <c r="BL62" s="6"/>
       <c r="BM62" s="6"/>
       <c r="BN62" s="6"/>
     </row>
     <row r="63" spans="1:66" ht="36.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A63" s="68"/>
-      <c r="B63" s="68" t="s">
+      <c r="A63" s="67"/>
+      <c r="B63" s="67" t="s">
         <v>1</v>
       </c>
-      <c r="C63" s="68" t="s">
+      <c r="C63" s="67" t="s">
         <v>21</v>
       </c>
       <c r="D63" s="6"/>
       <c r="E63" s="6"/>
       <c r="F63" s="6"/>
-      <c r="G63" s="72"/>
-      <c r="H63" s="72"/>
-      <c r="I63" s="72"/>
-      <c r="J63" s="72"/>
-      <c r="K63" s="72"/>
-      <c r="L63" s="72"/>
+      <c r="G63" s="76"/>
+      <c r="H63" s="76"/>
+      <c r="I63" s="76"/>
+      <c r="J63" s="76"/>
+      <c r="K63" s="76"/>
+      <c r="L63" s="76"/>
       <c r="M63" s="6"/>
       <c r="N63" s="6"/>
       <c r="O63" s="6"/>
@@ -7650,30 +7782,30 @@
       <c r="BC63" s="6"/>
       <c r="BD63" s="6"/>
       <c r="BE63" s="6"/>
-      <c r="BF63" s="72"/>
-      <c r="BG63" s="72"/>
-      <c r="BH63" s="72"/>
-      <c r="BI63" s="72"/>
-      <c r="BJ63" s="72"/>
-      <c r="BK63" s="72"/>
+      <c r="BF63" s="76"/>
+      <c r="BG63" s="76"/>
+      <c r="BH63" s="76"/>
+      <c r="BI63" s="76"/>
+      <c r="BJ63" s="76"/>
+      <c r="BK63" s="76"/>
       <c r="BL63" s="6"/>
       <c r="BM63" s="6"/>
       <c r="BN63" s="6"/>
     </row>
     <row r="64" spans="1:66" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A64" s="68"/>
-      <c r="B64" s="68" t="s">
+      <c r="A64" s="67"/>
+      <c r="B64" s="67" t="s">
         <v>2</v>
       </c>
-      <c r="C64" s="68" t="s">
+      <c r="C64" s="67" t="s">
         <v>22</v>
       </c>
-      <c r="D64" s="72"/>
-      <c r="E64" s="72"/>
-      <c r="F64" s="72"/>
-      <c r="G64" s="72"/>
-      <c r="H64" s="72"/>
-      <c r="I64" s="72"/>
+      <c r="D64" s="76"/>
+      <c r="E64" s="76"/>
+      <c r="F64" s="76"/>
+      <c r="G64" s="76"/>
+      <c r="H64" s="76"/>
+      <c r="I64" s="76"/>
       <c r="J64" s="6"/>
       <c r="K64" s="6"/>
       <c r="L64" s="6"/>
@@ -7724,28 +7856,32 @@
       <c r="AW64" s="6"/>
       <c r="AX64" s="6"/>
       <c r="AY64" s="6"/>
-      <c r="AZ64" s="6"/>
-      <c r="BA64" s="6"/>
+      <c r="AZ64" s="29" t="s">
+        <v>275</v>
+      </c>
+      <c r="BA64" s="71" t="s">
+        <v>211</v>
+      </c>
       <c r="BB64" s="6"/>
       <c r="BC64" s="6"/>
       <c r="BD64" s="6"/>
       <c r="BE64" s="6"/>
-      <c r="BF64" s="72"/>
-      <c r="BG64" s="72"/>
-      <c r="BH64" s="72"/>
-      <c r="BI64" s="72"/>
-      <c r="BJ64" s="72"/>
-      <c r="BK64" s="72"/>
+      <c r="BF64" s="76"/>
+      <c r="BG64" s="76"/>
+      <c r="BH64" s="76"/>
+      <c r="BI64" s="76"/>
+      <c r="BJ64" s="76"/>
+      <c r="BK64" s="76"/>
       <c r="BL64" s="6"/>
       <c r="BM64" s="6"/>
       <c r="BN64" s="6"/>
     </row>
     <row r="65" spans="1:66" ht="40.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A65" s="68"/>
-      <c r="B65" s="68" t="s">
+      <c r="A65" s="67"/>
+      <c r="B65" s="67" t="s">
         <v>3</v>
       </c>
-      <c r="C65" s="68" t="s">
+      <c r="C65" s="67" t="s">
         <v>23</v>
       </c>
       <c r="D65" s="6"/>
@@ -7806,24 +7942,24 @@
       <c r="BC65" s="6"/>
       <c r="BD65" s="6"/>
       <c r="BE65" s="6"/>
-      <c r="BF65" s="72"/>
-      <c r="BG65" s="72"/>
-      <c r="BH65" s="72"/>
-      <c r="BI65" s="72"/>
-      <c r="BJ65" s="72"/>
-      <c r="BK65" s="72"/>
+      <c r="BF65" s="76"/>
+      <c r="BG65" s="76"/>
+      <c r="BH65" s="76"/>
+      <c r="BI65" s="76"/>
+      <c r="BJ65" s="76"/>
+      <c r="BK65" s="76"/>
       <c r="BL65" s="6"/>
       <c r="BM65" s="6"/>
       <c r="BN65" s="6"/>
     </row>
     <row r="66" spans="1:66" ht="30" x14ac:dyDescent="0.25">
-      <c r="A66" s="68" t="s">
+      <c r="A66" s="67" t="s">
         <v>155</v>
       </c>
-      <c r="B66" s="68" t="s">
+      <c r="B66" s="67" t="s">
         <v>0</v>
       </c>
-      <c r="C66" s="68" t="s">
+      <c r="C66" s="67" t="s">
         <v>20</v>
       </c>
       <c r="D66" s="6"/>
@@ -7891,19 +8027,19 @@
       <c r="BN66" s="6"/>
     </row>
     <row r="67" spans="1:66" ht="42.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A67" s="68"/>
-      <c r="B67" s="68" t="s">
+      <c r="A67" s="67"/>
+      <c r="B67" s="67" t="s">
         <v>1</v>
       </c>
-      <c r="C67" s="68" t="s">
+      <c r="C67" s="67" t="s">
         <v>21</v>
       </c>
-      <c r="D67" s="72"/>
-      <c r="E67" s="72"/>
-      <c r="F67" s="72"/>
-      <c r="G67" s="72"/>
-      <c r="H67" s="72"/>
-      <c r="I67" s="72"/>
+      <c r="D67" s="76"/>
+      <c r="E67" s="76"/>
+      <c r="F67" s="76"/>
+      <c r="G67" s="76"/>
+      <c r="H67" s="76"/>
+      <c r="I67" s="76"/>
       <c r="J67" s="6"/>
       <c r="K67" s="6"/>
       <c r="L67" s="6"/>
@@ -7950,12 +8086,12 @@
         <v>195</v>
       </c>
       <c r="AY67" s="6"/>
-      <c r="AZ67" s="72"/>
-      <c r="BA67" s="72"/>
-      <c r="BB67" s="72"/>
-      <c r="BC67" s="72"/>
-      <c r="BD67" s="72"/>
-      <c r="BE67" s="72"/>
+      <c r="AZ67" s="76"/>
+      <c r="BA67" s="76"/>
+      <c r="BB67" s="76"/>
+      <c r="BC67" s="76"/>
+      <c r="BD67" s="76"/>
+      <c r="BE67" s="76"/>
       <c r="BF67" s="6"/>
       <c r="BG67" s="6"/>
       <c r="BH67" s="6"/>
@@ -7967,22 +8103,22 @@
       <c r="BN67" s="6"/>
     </row>
     <row r="68" spans="1:66" ht="39.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A68" s="68"/>
-      <c r="B68" s="68" t="s">
+      <c r="A68" s="67"/>
+      <c r="B68" s="67" t="s">
         <v>2</v>
       </c>
-      <c r="C68" s="68" t="s">
+      <c r="C68" s="67" t="s">
         <v>22</v>
       </c>
       <c r="D68" s="6"/>
       <c r="E68" s="6"/>
       <c r="F68" s="6"/>
-      <c r="G68" s="72"/>
-      <c r="H68" s="72"/>
-      <c r="I68" s="72"/>
-      <c r="J68" s="72"/>
-      <c r="K68" s="72"/>
-      <c r="L68" s="72"/>
+      <c r="G68" s="76"/>
+      <c r="H68" s="76"/>
+      <c r="I68" s="76"/>
+      <c r="J68" s="76"/>
+      <c r="K68" s="76"/>
+      <c r="L68" s="76"/>
       <c r="M68" s="6"/>
       <c r="N68" s="6"/>
       <c r="O68" s="6"/>
@@ -8043,22 +8179,22 @@
       <c r="BN68" s="6"/>
     </row>
     <row r="69" spans="1:66" ht="42" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A69" s="68"/>
-      <c r="B69" s="68" t="s">
+      <c r="A69" s="67"/>
+      <c r="B69" s="67" t="s">
         <v>3</v>
       </c>
-      <c r="C69" s="68" t="s">
+      <c r="C69" s="67" t="s">
         <v>23</v>
       </c>
       <c r="D69" s="6"/>
       <c r="E69" s="6"/>
       <c r="F69" s="6"/>
-      <c r="G69" s="72"/>
-      <c r="H69" s="72"/>
-      <c r="I69" s="72"/>
-      <c r="J69" s="72"/>
-      <c r="K69" s="72"/>
-      <c r="L69" s="72"/>
+      <c r="G69" s="76"/>
+      <c r="H69" s="76"/>
+      <c r="I69" s="76"/>
+      <c r="J69" s="76"/>
+      <c r="K69" s="76"/>
+      <c r="L69" s="76"/>
       <c r="M69" s="6"/>
       <c r="N69" s="6"/>
       <c r="O69" s="6"/>
@@ -8104,18 +8240,18 @@
       <c r="BC69" s="6"/>
       <c r="BD69" s="6"/>
       <c r="BE69" s="6"/>
-      <c r="BF69" s="75"/>
-      <c r="BG69" s="75"/>
-      <c r="BH69" s="75"/>
-      <c r="BI69" s="75"/>
-      <c r="BJ69" s="75"/>
-      <c r="BK69" s="75"/>
+      <c r="BF69" s="89"/>
+      <c r="BG69" s="89"/>
+      <c r="BH69" s="89"/>
+      <c r="BI69" s="89"/>
+      <c r="BJ69" s="89"/>
+      <c r="BK69" s="89"/>
       <c r="BL69" s="6"/>
       <c r="BM69" s="6"/>
       <c r="BN69" s="6"/>
     </row>
     <row r="70" spans="1:66" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C70" s="66" t="s">
+      <c r="C70" s="65" t="s">
         <v>36</v>
       </c>
       <c r="D70" s="6"/>
@@ -8183,13 +8319,13 @@
       <c r="BN70" s="6"/>
     </row>
     <row r="71" spans="1:66" ht="30" x14ac:dyDescent="0.25">
-      <c r="A71" s="68" t="s">
+      <c r="A71" s="67" t="s">
         <v>156</v>
       </c>
-      <c r="B71" s="68" t="s">
+      <c r="B71" s="67" t="s">
         <v>0</v>
       </c>
-      <c r="C71" s="68" t="s">
+      <c r="C71" s="67" t="s">
         <v>20</v>
       </c>
       <c r="D71" s="6"/>
@@ -8240,12 +8376,12 @@
       <c r="AW71" s="6"/>
       <c r="AX71" s="6"/>
       <c r="AY71" s="6"/>
-      <c r="AZ71" s="75"/>
-      <c r="BA71" s="75"/>
-      <c r="BB71" s="75"/>
-      <c r="BC71" s="75"/>
-      <c r="BD71" s="75"/>
-      <c r="BE71" s="75"/>
+      <c r="AZ71" s="89"/>
+      <c r="BA71" s="89"/>
+      <c r="BB71" s="89"/>
+      <c r="BC71" s="89"/>
+      <c r="BD71" s="89"/>
+      <c r="BE71" s="89"/>
       <c r="BF71" s="6"/>
       <c r="BG71" s="6"/>
       <c r="BH71" s="6"/>
@@ -8257,19 +8393,19 @@
       <c r="BN71" s="6"/>
     </row>
     <row r="72" spans="1:66" ht="48" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A72" s="68"/>
-      <c r="B72" s="68" t="s">
+      <c r="A72" s="67"/>
+      <c r="B72" s="67" t="s">
         <v>1</v>
       </c>
-      <c r="C72" s="68" t="s">
+      <c r="C72" s="67" t="s">
         <v>21</v>
       </c>
-      <c r="D72" s="72"/>
-      <c r="E72" s="72"/>
-      <c r="F72" s="72"/>
-      <c r="G72" s="72"/>
-      <c r="H72" s="72"/>
-      <c r="I72" s="72"/>
+      <c r="D72" s="76"/>
+      <c r="E72" s="76"/>
+      <c r="F72" s="76"/>
+      <c r="G72" s="76"/>
+      <c r="H72" s="76"/>
+      <c r="I72" s="76"/>
       <c r="J72" s="6"/>
       <c r="K72" s="6"/>
       <c r="L72" s="6"/>
@@ -8329,19 +8465,19 @@
       <c r="BN72" s="6"/>
     </row>
     <row r="73" spans="1:66" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A73" s="68"/>
-      <c r="B73" s="68" t="s">
+      <c r="A73" s="67"/>
+      <c r="B73" s="67" t="s">
         <v>2</v>
       </c>
-      <c r="C73" s="68" t="s">
+      <c r="C73" s="67" t="s">
         <v>22</v>
       </c>
-      <c r="D73" s="72"/>
-      <c r="E73" s="72"/>
-      <c r="F73" s="72"/>
-      <c r="G73" s="72"/>
-      <c r="H73" s="72"/>
-      <c r="I73" s="72"/>
+      <c r="D73" s="76"/>
+      <c r="E73" s="76"/>
+      <c r="F73" s="76"/>
+      <c r="G73" s="76"/>
+      <c r="H73" s="76"/>
+      <c r="I73" s="76"/>
       <c r="J73" s="6"/>
       <c r="K73" s="6"/>
       <c r="L73" s="6"/>
@@ -8390,30 +8526,30 @@
       <c r="BC73" s="6"/>
       <c r="BD73" s="6"/>
       <c r="BE73" s="6"/>
-      <c r="BF73" s="72"/>
-      <c r="BG73" s="72"/>
-      <c r="BH73" s="72"/>
-      <c r="BI73" s="72"/>
-      <c r="BJ73" s="72"/>
-      <c r="BK73" s="72"/>
+      <c r="BF73" s="76"/>
+      <c r="BG73" s="76"/>
+      <c r="BH73" s="76"/>
+      <c r="BI73" s="76"/>
+      <c r="BJ73" s="76"/>
+      <c r="BK73" s="76"/>
       <c r="BL73" s="6"/>
       <c r="BM73" s="6"/>
       <c r="BN73" s="6"/>
     </row>
     <row r="74" spans="1:66" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A74" s="68"/>
-      <c r="B74" s="68" t="s">
+      <c r="A74" s="67"/>
+      <c r="B74" s="67" t="s">
         <v>3</v>
       </c>
-      <c r="C74" s="68" t="s">
+      <c r="C74" s="67" t="s">
         <v>23</v>
       </c>
-      <c r="D74" s="79"/>
-      <c r="E74" s="79"/>
-      <c r="F74" s="79"/>
-      <c r="G74" s="79"/>
-      <c r="H74" s="79"/>
-      <c r="I74" s="79"/>
+      <c r="D74" s="94"/>
+      <c r="E74" s="94"/>
+      <c r="F74" s="94"/>
+      <c r="G74" s="94"/>
+      <c r="H74" s="94"/>
+      <c r="I74" s="94"/>
       <c r="J74" s="6"/>
       <c r="K74" s="6"/>
       <c r="L74" s="6"/>
@@ -8462,23 +8598,23 @@
       <c r="BC74" s="6"/>
       <c r="BD74" s="6"/>
       <c r="BE74" s="6"/>
-      <c r="BF74" s="72"/>
-      <c r="BG74" s="72"/>
-      <c r="BH74" s="72"/>
-      <c r="BI74" s="72"/>
-      <c r="BJ74" s="72"/>
-      <c r="BK74" s="72"/>
+      <c r="BF74" s="76"/>
+      <c r="BG74" s="76"/>
+      <c r="BH74" s="76"/>
+      <c r="BI74" s="76"/>
+      <c r="BJ74" s="76"/>
+      <c r="BK74" s="76"/>
       <c r="BL74" s="6"/>
       <c r="BM74" s="6"/>
       <c r="BN74" s="6"/>
     </row>
     <row r="75" spans="1:66" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D75" s="79"/>
-      <c r="E75" s="79"/>
-      <c r="F75" s="79"/>
-      <c r="G75" s="79"/>
-      <c r="H75" s="79"/>
-      <c r="I75" s="79"/>
+      <c r="D75" s="94"/>
+      <c r="E75" s="94"/>
+      <c r="F75" s="94"/>
+      <c r="G75" s="94"/>
+      <c r="H75" s="94"/>
+      <c r="I75" s="94"/>
       <c r="J75" s="6"/>
       <c r="K75" s="6"/>
       <c r="L75" s="6"/>
@@ -8527,20 +8663,20 @@
       <c r="BC75" s="6"/>
       <c r="BD75" s="6"/>
       <c r="BE75" s="6"/>
-      <c r="BF75" s="72"/>
-      <c r="BG75" s="72"/>
-      <c r="BH75" s="72"/>
-      <c r="BI75" s="72"/>
-      <c r="BJ75" s="72"/>
-      <c r="BK75" s="72"/>
+      <c r="BF75" s="76"/>
+      <c r="BG75" s="76"/>
+      <c r="BH75" s="76"/>
+      <c r="BI75" s="76"/>
+      <c r="BJ75" s="76"/>
+      <c r="BK75" s="76"/>
       <c r="BL75" s="6"/>
       <c r="BM75" s="6"/>
       <c r="BN75" s="6"/>
     </row>
     <row r="76" spans="1:66" x14ac:dyDescent="0.25">
-      <c r="A76" s="68"/>
-      <c r="B76" s="68"/>
-      <c r="C76" s="68"/>
+      <c r="A76" s="67"/>
+      <c r="B76" s="67"/>
+      <c r="C76" s="67"/>
       <c r="D76" s="6"/>
       <c r="E76" s="6"/>
       <c r="F76" s="6"/>
@@ -8606,15 +8742,15 @@
       <c r="BN76" s="6"/>
     </row>
     <row r="77" spans="1:66" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A77" s="68"/>
-      <c r="B77" s="68"/>
-      <c r="C77" s="68"/>
-      <c r="D77" s="79"/>
-      <c r="E77" s="79"/>
-      <c r="F77" s="79"/>
-      <c r="G77" s="79"/>
-      <c r="H77" s="79"/>
-      <c r="I77" s="79"/>
+      <c r="A77" s="67"/>
+      <c r="B77" s="67"/>
+      <c r="C77" s="67"/>
+      <c r="D77" s="94"/>
+      <c r="E77" s="94"/>
+      <c r="F77" s="94"/>
+      <c r="G77" s="94"/>
+      <c r="H77" s="94"/>
+      <c r="I77" s="94"/>
       <c r="J77" s="6"/>
       <c r="K77" s="6"/>
       <c r="L77" s="6"/>
@@ -8663,26 +8799,26 @@
       <c r="BC77" s="6"/>
       <c r="BD77" s="6"/>
       <c r="BE77" s="6"/>
-      <c r="BF77" s="72"/>
-      <c r="BG77" s="72"/>
-      <c r="BH77" s="72"/>
-      <c r="BI77" s="72"/>
-      <c r="BJ77" s="72"/>
-      <c r="BK77" s="72"/>
+      <c r="BF77" s="76"/>
+      <c r="BG77" s="76"/>
+      <c r="BH77" s="76"/>
+      <c r="BI77" s="76"/>
+      <c r="BJ77" s="76"/>
+      <c r="BK77" s="76"/>
       <c r="BL77" s="6"/>
       <c r="BM77" s="6"/>
       <c r="BN77" s="6"/>
     </row>
     <row r="78" spans="1:66" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A78" s="68"/>
-      <c r="B78" s="68"/>
-      <c r="C78" s="68"/>
-      <c r="D78" s="79"/>
-      <c r="E78" s="79"/>
-      <c r="F78" s="79"/>
-      <c r="G78" s="79"/>
-      <c r="H78" s="79"/>
-      <c r="I78" s="79"/>
+      <c r="A78" s="67"/>
+      <c r="B78" s="67"/>
+      <c r="C78" s="67"/>
+      <c r="D78" s="94"/>
+      <c r="E78" s="94"/>
+      <c r="F78" s="94"/>
+      <c r="G78" s="94"/>
+      <c r="H78" s="94"/>
+      <c r="I78" s="94"/>
       <c r="J78" s="6"/>
       <c r="K78" s="6"/>
       <c r="L78" s="6"/>
@@ -8731,26 +8867,26 @@
       <c r="BC78" s="6"/>
       <c r="BD78" s="6"/>
       <c r="BE78" s="6"/>
-      <c r="BF78" s="72"/>
-      <c r="BG78" s="72"/>
-      <c r="BH78" s="72"/>
-      <c r="BI78" s="72"/>
-      <c r="BJ78" s="72"/>
-      <c r="BK78" s="72"/>
+      <c r="BF78" s="76"/>
+      <c r="BG78" s="76"/>
+      <c r="BH78" s="76"/>
+      <c r="BI78" s="76"/>
+      <c r="BJ78" s="76"/>
+      <c r="BK78" s="76"/>
       <c r="BL78" s="6"/>
       <c r="BM78" s="6"/>
       <c r="BN78" s="6"/>
     </row>
     <row r="79" spans="1:66" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A79" s="68"/>
-      <c r="B79" s="68"/>
-      <c r="C79" s="68"/>
-      <c r="D79" s="79"/>
-      <c r="E79" s="79"/>
-      <c r="F79" s="79"/>
-      <c r="G79" s="79"/>
-      <c r="H79" s="79"/>
-      <c r="I79" s="79"/>
+      <c r="A79" s="67"/>
+      <c r="B79" s="67"/>
+      <c r="C79" s="67"/>
+      <c r="D79" s="94"/>
+      <c r="E79" s="94"/>
+      <c r="F79" s="94"/>
+      <c r="G79" s="94"/>
+      <c r="H79" s="94"/>
+      <c r="I79" s="94"/>
       <c r="J79" s="6"/>
       <c r="K79" s="6"/>
       <c r="L79" s="6"/>
@@ -8799,23 +8935,23 @@
       <c r="BC79" s="6"/>
       <c r="BD79" s="6"/>
       <c r="BE79" s="6"/>
-      <c r="BF79" s="72"/>
-      <c r="BG79" s="72"/>
-      <c r="BH79" s="72"/>
-      <c r="BI79" s="72"/>
-      <c r="BJ79" s="72"/>
-      <c r="BK79" s="72"/>
+      <c r="BF79" s="76"/>
+      <c r="BG79" s="76"/>
+      <c r="BH79" s="76"/>
+      <c r="BI79" s="76"/>
+      <c r="BJ79" s="76"/>
+      <c r="BK79" s="76"/>
       <c r="BL79" s="6"/>
       <c r="BM79" s="6"/>
       <c r="BN79" s="6"/>
     </row>
     <row r="80" spans="1:66" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D80" s="72"/>
-      <c r="E80" s="72"/>
-      <c r="F80" s="72"/>
-      <c r="G80" s="72"/>
-      <c r="H80" s="72"/>
-      <c r="I80" s="72"/>
+      <c r="D80" s="76"/>
+      <c r="E80" s="76"/>
+      <c r="F80" s="76"/>
+      <c r="G80" s="76"/>
+      <c r="H80" s="76"/>
+      <c r="I80" s="76"/>
       <c r="J80" s="6"/>
       <c r="K80" s="6"/>
       <c r="L80" s="6"/>
@@ -8875,9 +9011,9 @@
       <c r="BN80" s="6"/>
     </row>
     <row r="81" spans="1:66" x14ac:dyDescent="0.25">
-      <c r="A81" s="68"/>
-      <c r="B81" s="68"/>
-      <c r="C81" s="68"/>
+      <c r="A81" s="67"/>
+      <c r="B81" s="67"/>
+      <c r="C81" s="67"/>
       <c r="D81" s="6"/>
       <c r="E81" s="6"/>
       <c r="F81" s="6"/>
@@ -8943,15 +9079,15 @@
       <c r="BN81" s="6"/>
     </row>
     <row r="82" spans="1:66" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A82" s="68"/>
-      <c r="B82" s="68"/>
-      <c r="C82" s="68"/>
-      <c r="D82" s="79"/>
-      <c r="E82" s="79"/>
-      <c r="F82" s="79"/>
-      <c r="G82" s="79"/>
-      <c r="H82" s="79"/>
-      <c r="I82" s="79"/>
+      <c r="A82" s="67"/>
+      <c r="B82" s="67"/>
+      <c r="C82" s="67"/>
+      <c r="D82" s="94"/>
+      <c r="E82" s="94"/>
+      <c r="F82" s="94"/>
+      <c r="G82" s="94"/>
+      <c r="H82" s="94"/>
+      <c r="I82" s="94"/>
       <c r="J82" s="6"/>
       <c r="K82" s="6"/>
       <c r="L82" s="6"/>
@@ -9000,26 +9136,26 @@
       <c r="BC82" s="6"/>
       <c r="BD82" s="6"/>
       <c r="BE82" s="6"/>
-      <c r="BF82" s="72"/>
-      <c r="BG82" s="72"/>
-      <c r="BH82" s="72"/>
-      <c r="BI82" s="72"/>
-      <c r="BJ82" s="72"/>
-      <c r="BK82" s="72"/>
+      <c r="BF82" s="76"/>
+      <c r="BG82" s="76"/>
+      <c r="BH82" s="76"/>
+      <c r="BI82" s="76"/>
+      <c r="BJ82" s="76"/>
+      <c r="BK82" s="76"/>
       <c r="BL82" s="6"/>
       <c r="BM82" s="6"/>
       <c r="BN82" s="6"/>
     </row>
     <row r="83" spans="1:66" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A83" s="68"/>
-      <c r="B83" s="68"/>
-      <c r="C83" s="68"/>
-      <c r="D83" s="72"/>
-      <c r="E83" s="72"/>
-      <c r="F83" s="72"/>
-      <c r="G83" s="72"/>
-      <c r="H83" s="72"/>
-      <c r="I83" s="72"/>
+      <c r="A83" s="67"/>
+      <c r="B83" s="67"/>
+      <c r="C83" s="67"/>
+      <c r="D83" s="76"/>
+      <c r="E83" s="76"/>
+      <c r="F83" s="76"/>
+      <c r="G83" s="76"/>
+      <c r="H83" s="76"/>
+      <c r="I83" s="76"/>
       <c r="J83" s="6"/>
       <c r="K83" s="6"/>
       <c r="L83" s="6"/>
@@ -9079,15 +9215,15 @@
       <c r="BN83" s="6"/>
     </row>
     <row r="84" spans="1:66" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A84" s="68"/>
-      <c r="B84" s="68"/>
-      <c r="C84" s="68"/>
-      <c r="D84" s="72"/>
-      <c r="E84" s="72"/>
-      <c r="F84" s="72"/>
-      <c r="G84" s="72"/>
-      <c r="H84" s="72"/>
-      <c r="I84" s="72"/>
+      <c r="A84" s="67"/>
+      <c r="B84" s="67"/>
+      <c r="C84" s="67"/>
+      <c r="D84" s="76"/>
+      <c r="E84" s="76"/>
+      <c r="F84" s="76"/>
+      <c r="G84" s="76"/>
+      <c r="H84" s="76"/>
+      <c r="I84" s="76"/>
       <c r="J84" s="6"/>
       <c r="K84" s="6"/>
       <c r="L84" s="6"/>
@@ -9150,12 +9286,12 @@
       <c r="A85" s="21"/>
       <c r="B85" s="21"/>
       <c r="C85" s="21"/>
-      <c r="D85" s="79"/>
-      <c r="E85" s="79"/>
-      <c r="F85" s="79"/>
-      <c r="G85" s="79"/>
-      <c r="H85" s="79"/>
-      <c r="I85" s="79"/>
+      <c r="D85" s="94"/>
+      <c r="E85" s="94"/>
+      <c r="F85" s="94"/>
+      <c r="G85" s="94"/>
+      <c r="H85" s="94"/>
+      <c r="I85" s="94"/>
       <c r="J85" s="6"/>
       <c r="K85" s="6"/>
       <c r="L85" s="6"/>
@@ -9204,12 +9340,12 @@
       <c r="BC85" s="6"/>
       <c r="BD85" s="6"/>
       <c r="BE85" s="6"/>
-      <c r="BF85" s="72"/>
-      <c r="BG85" s="72"/>
-      <c r="BH85" s="72"/>
-      <c r="BI85" s="72"/>
-      <c r="BJ85" s="72"/>
-      <c r="BK85" s="72"/>
+      <c r="BF85" s="76"/>
+      <c r="BG85" s="76"/>
+      <c r="BH85" s="76"/>
+      <c r="BI85" s="76"/>
+      <c r="BJ85" s="76"/>
+      <c r="BK85" s="76"/>
       <c r="BL85" s="6"/>
       <c r="BM85" s="6"/>
       <c r="BN85" s="6"/>
@@ -9626,7 +9762,143 @@
       <c r="AB92" s="4"/>
     </row>
   </sheetData>
-  <mergeCells count="144">
+  <mergeCells count="160">
+    <mergeCell ref="AZ45:BC45"/>
+    <mergeCell ref="AZ44:BC44"/>
+    <mergeCell ref="AZ33:BC33"/>
+    <mergeCell ref="AZ34:BC34"/>
+    <mergeCell ref="AZ8:BC8"/>
+    <mergeCell ref="AZ9:BC9"/>
+    <mergeCell ref="AZ28:BC28"/>
+    <mergeCell ref="AZ49:BC49"/>
+    <mergeCell ref="BF33:BI33"/>
+    <mergeCell ref="BF34:BI34"/>
+    <mergeCell ref="D18:I18"/>
+    <mergeCell ref="D9:I9"/>
+    <mergeCell ref="D10:I10"/>
+    <mergeCell ref="D14:I14"/>
+    <mergeCell ref="D15:I15"/>
+    <mergeCell ref="D38:I38"/>
+    <mergeCell ref="D39:I39"/>
+    <mergeCell ref="D24:I24"/>
+    <mergeCell ref="D25:I25"/>
+    <mergeCell ref="D67:I67"/>
+    <mergeCell ref="D72:I72"/>
+    <mergeCell ref="D64:I64"/>
+    <mergeCell ref="G63:L63"/>
+    <mergeCell ref="G56:L56"/>
+    <mergeCell ref="G57:L57"/>
+    <mergeCell ref="D85:I85"/>
+    <mergeCell ref="D58:I58"/>
+    <mergeCell ref="D59:I59"/>
+    <mergeCell ref="D79:I79"/>
+    <mergeCell ref="D73:I73"/>
+    <mergeCell ref="D80:I80"/>
+    <mergeCell ref="D82:I82"/>
+    <mergeCell ref="D83:I83"/>
+    <mergeCell ref="D84:I84"/>
+    <mergeCell ref="D77:I77"/>
+    <mergeCell ref="D78:I78"/>
+    <mergeCell ref="D74:I74"/>
+    <mergeCell ref="D75:I75"/>
+    <mergeCell ref="G68:L68"/>
+    <mergeCell ref="G69:L69"/>
+    <mergeCell ref="G62:L62"/>
+    <mergeCell ref="G53:L53"/>
+    <mergeCell ref="G54:L54"/>
+    <mergeCell ref="AQ1:AY1"/>
+    <mergeCell ref="AZ1:BN1"/>
+    <mergeCell ref="AZ3:BB3"/>
+    <mergeCell ref="P1:X1"/>
+    <mergeCell ref="AQ2:AS3"/>
+    <mergeCell ref="AT2:AV3"/>
+    <mergeCell ref="AE2:AG3"/>
+    <mergeCell ref="AH2:AJ3"/>
+    <mergeCell ref="D1:O1"/>
+    <mergeCell ref="AZ2:BE2"/>
+    <mergeCell ref="BF2:BK2"/>
+    <mergeCell ref="BL2:BN2"/>
+    <mergeCell ref="BL3:BN3"/>
+    <mergeCell ref="D12:O12"/>
+    <mergeCell ref="D13:O13"/>
+    <mergeCell ref="D23:O23"/>
+    <mergeCell ref="D22:O22"/>
+    <mergeCell ref="D37:O37"/>
+    <mergeCell ref="P18:X18"/>
+    <mergeCell ref="P19:X19"/>
+    <mergeCell ref="P33:X33"/>
+    <mergeCell ref="D17:I17"/>
+    <mergeCell ref="BR3:BT3"/>
+    <mergeCell ref="D2:F3"/>
+    <mergeCell ref="G2:I3"/>
+    <mergeCell ref="J2:L3"/>
+    <mergeCell ref="M2:O3"/>
+    <mergeCell ref="P2:R3"/>
+    <mergeCell ref="S2:U3"/>
+    <mergeCell ref="V2:X3"/>
+    <mergeCell ref="Y2:AA3"/>
+    <mergeCell ref="AB2:AD3"/>
+    <mergeCell ref="BC3:BE3"/>
+    <mergeCell ref="BF3:BH3"/>
+    <mergeCell ref="BI3:BK3"/>
+    <mergeCell ref="BO3:BQ3"/>
+    <mergeCell ref="AK2:AM3"/>
+    <mergeCell ref="AN2:AP3"/>
+    <mergeCell ref="BF85:BK85"/>
+    <mergeCell ref="BF75:BK75"/>
+    <mergeCell ref="BF74:BK74"/>
+    <mergeCell ref="BF59:BK59"/>
+    <mergeCell ref="BF60:BK60"/>
+    <mergeCell ref="BF65:BK65"/>
+    <mergeCell ref="BF55:BK55"/>
+    <mergeCell ref="AW2:AY3"/>
+    <mergeCell ref="Y1:AG1"/>
+    <mergeCell ref="AH1:AP1"/>
+    <mergeCell ref="AZ71:BE71"/>
+    <mergeCell ref="AZ67:BE67"/>
+    <mergeCell ref="AZ52:BE52"/>
+    <mergeCell ref="AK5:AM5"/>
+    <mergeCell ref="AN5:AP5"/>
+    <mergeCell ref="AQ5:AS5"/>
+    <mergeCell ref="AT5:AV5"/>
+    <mergeCell ref="AW5:AY5"/>
+    <mergeCell ref="AZ5:BB5"/>
+    <mergeCell ref="BC5:BE5"/>
+    <mergeCell ref="BF52:BK52"/>
+    <mergeCell ref="BF82:BK82"/>
+    <mergeCell ref="BL4:BN4"/>
+    <mergeCell ref="AW4:AY4"/>
+    <mergeCell ref="AZ4:BB4"/>
+    <mergeCell ref="BF79:BK79"/>
+    <mergeCell ref="BF77:BK77"/>
+    <mergeCell ref="BF78:BK78"/>
+    <mergeCell ref="BF69:BK69"/>
+    <mergeCell ref="BF53:BK53"/>
+    <mergeCell ref="BF64:BK64"/>
+    <mergeCell ref="BF73:BK73"/>
+    <mergeCell ref="BF63:BK63"/>
+    <mergeCell ref="BF62:BK62"/>
+    <mergeCell ref="BF54:BK54"/>
+    <mergeCell ref="BL5:BN5"/>
+    <mergeCell ref="AZ23:BC23"/>
+    <mergeCell ref="AZ18:BC18"/>
+    <mergeCell ref="AZ38:BC38"/>
+    <mergeCell ref="AZ39:BC39"/>
+    <mergeCell ref="AZ59:BC59"/>
+    <mergeCell ref="AZ12:BC12"/>
+    <mergeCell ref="AZ13:BC13"/>
+    <mergeCell ref="AZ14:BC14"/>
+    <mergeCell ref="D5:F5"/>
+    <mergeCell ref="G5:I5"/>
+    <mergeCell ref="Y5:AA5"/>
+    <mergeCell ref="S5:U5"/>
+    <mergeCell ref="V5:X5"/>
+    <mergeCell ref="AH5:AJ5"/>
+    <mergeCell ref="AB5:AD5"/>
+    <mergeCell ref="AE5:AG5"/>
+    <mergeCell ref="J5:L5"/>
+    <mergeCell ref="M5:O5"/>
+    <mergeCell ref="P5:R5"/>
     <mergeCell ref="D7:O7"/>
     <mergeCell ref="D8:O8"/>
     <mergeCell ref="P9:X9"/>
@@ -9651,126 +9923,6 @@
     <mergeCell ref="G4:I4"/>
     <mergeCell ref="J4:L4"/>
     <mergeCell ref="M4:O4"/>
-    <mergeCell ref="D5:F5"/>
-    <mergeCell ref="G5:I5"/>
-    <mergeCell ref="Y5:AA5"/>
-    <mergeCell ref="S5:U5"/>
-    <mergeCell ref="V5:X5"/>
-    <mergeCell ref="AH5:AJ5"/>
-    <mergeCell ref="AB5:AD5"/>
-    <mergeCell ref="AE5:AG5"/>
-    <mergeCell ref="J5:L5"/>
-    <mergeCell ref="M5:O5"/>
-    <mergeCell ref="P5:R5"/>
-    <mergeCell ref="BL4:BN4"/>
-    <mergeCell ref="AW4:AY4"/>
-    <mergeCell ref="AZ4:BB4"/>
-    <mergeCell ref="BF79:BK79"/>
-    <mergeCell ref="BF77:BK77"/>
-    <mergeCell ref="BF78:BK78"/>
-    <mergeCell ref="BF69:BK69"/>
-    <mergeCell ref="BF53:BK53"/>
-    <mergeCell ref="BF64:BK64"/>
-    <mergeCell ref="BF73:BK73"/>
-    <mergeCell ref="BF63:BK63"/>
-    <mergeCell ref="BF62:BK62"/>
-    <mergeCell ref="BF54:BK54"/>
-    <mergeCell ref="BL5:BN5"/>
-    <mergeCell ref="BF85:BK85"/>
-    <mergeCell ref="BF75:BK75"/>
-    <mergeCell ref="BF74:BK74"/>
-    <mergeCell ref="BF59:BK59"/>
-    <mergeCell ref="BF60:BK60"/>
-    <mergeCell ref="BF65:BK65"/>
-    <mergeCell ref="BF55:BK55"/>
-    <mergeCell ref="AW2:AY3"/>
-    <mergeCell ref="Y1:AG1"/>
-    <mergeCell ref="AH1:AP1"/>
-    <mergeCell ref="AZ71:BE71"/>
-    <mergeCell ref="AZ67:BE67"/>
-    <mergeCell ref="AZ58:BE58"/>
-    <mergeCell ref="AZ59:BE59"/>
-    <mergeCell ref="AZ52:BE52"/>
-    <mergeCell ref="AK5:AM5"/>
-    <mergeCell ref="AN5:AP5"/>
-    <mergeCell ref="AQ5:AS5"/>
-    <mergeCell ref="AT5:AV5"/>
-    <mergeCell ref="AW5:AY5"/>
-    <mergeCell ref="AZ5:BB5"/>
-    <mergeCell ref="BC5:BE5"/>
-    <mergeCell ref="BF52:BK52"/>
-    <mergeCell ref="BF82:BK82"/>
-    <mergeCell ref="BR3:BT3"/>
-    <mergeCell ref="D2:F3"/>
-    <mergeCell ref="G2:I3"/>
-    <mergeCell ref="J2:L3"/>
-    <mergeCell ref="M2:O3"/>
-    <mergeCell ref="P2:R3"/>
-    <mergeCell ref="S2:U3"/>
-    <mergeCell ref="V2:X3"/>
-    <mergeCell ref="Y2:AA3"/>
-    <mergeCell ref="AB2:AD3"/>
-    <mergeCell ref="BC3:BE3"/>
-    <mergeCell ref="BF3:BH3"/>
-    <mergeCell ref="BI3:BK3"/>
-    <mergeCell ref="BO3:BQ3"/>
-    <mergeCell ref="AK2:AM3"/>
-    <mergeCell ref="AN2:AP3"/>
-    <mergeCell ref="G53:L53"/>
-    <mergeCell ref="G54:L54"/>
-    <mergeCell ref="AQ1:AY1"/>
-    <mergeCell ref="AZ1:BN1"/>
-    <mergeCell ref="AZ3:BB3"/>
-    <mergeCell ref="P1:X1"/>
-    <mergeCell ref="AQ2:AS3"/>
-    <mergeCell ref="AT2:AV3"/>
-    <mergeCell ref="AE2:AG3"/>
-    <mergeCell ref="AH2:AJ3"/>
-    <mergeCell ref="D1:O1"/>
-    <mergeCell ref="AZ2:BE2"/>
-    <mergeCell ref="BF2:BK2"/>
-    <mergeCell ref="BL2:BN2"/>
-    <mergeCell ref="BL3:BN3"/>
-    <mergeCell ref="D12:O12"/>
-    <mergeCell ref="D13:O13"/>
-    <mergeCell ref="D23:O23"/>
-    <mergeCell ref="D22:O22"/>
-    <mergeCell ref="D37:O37"/>
-    <mergeCell ref="P18:X18"/>
-    <mergeCell ref="P19:X19"/>
-    <mergeCell ref="P33:X33"/>
-    <mergeCell ref="D67:I67"/>
-    <mergeCell ref="D72:I72"/>
-    <mergeCell ref="D64:I64"/>
-    <mergeCell ref="G63:L63"/>
-    <mergeCell ref="G56:L56"/>
-    <mergeCell ref="G57:L57"/>
-    <mergeCell ref="D85:I85"/>
-    <mergeCell ref="D58:I58"/>
-    <mergeCell ref="D59:I59"/>
-    <mergeCell ref="D79:I79"/>
-    <mergeCell ref="D73:I73"/>
-    <mergeCell ref="D80:I80"/>
-    <mergeCell ref="D82:I82"/>
-    <mergeCell ref="D83:I83"/>
-    <mergeCell ref="D84:I84"/>
-    <mergeCell ref="D77:I77"/>
-    <mergeCell ref="D78:I78"/>
-    <mergeCell ref="D74:I74"/>
-    <mergeCell ref="D75:I75"/>
-    <mergeCell ref="G68:L68"/>
-    <mergeCell ref="G69:L69"/>
-    <mergeCell ref="G62:L62"/>
-    <mergeCell ref="D17:I17"/>
-    <mergeCell ref="D18:I18"/>
-    <mergeCell ref="D9:I9"/>
-    <mergeCell ref="D10:I10"/>
-    <mergeCell ref="D14:I14"/>
-    <mergeCell ref="D15:I15"/>
-    <mergeCell ref="D38:I38"/>
-    <mergeCell ref="D39:I39"/>
-    <mergeCell ref="D24:I24"/>
-    <mergeCell ref="D25:I25"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>